<commit_message>
moved UART Debug functionality to separate screen
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113581" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124793" uniqueCount="489">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1432,6 +1432,102 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle Parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART Debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART RX Debug</t>
   </si>
 </sst>
 </file>
@@ -2896,10 +2992,10 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>71</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -2908,29 +3004,29 @@
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
         <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>81</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -2942,29 +3038,29 @@
         <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>89</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>138</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
         <v>39</v>
@@ -2976,12 +3072,12 @@
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -2993,49 +3089,49 @@
         <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>181</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>180</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>144</v>
+        <v>293</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
         <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>146</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>147</v>
+        <v>294</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>42</v>
@@ -3044,12 +3140,12 @@
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>148</v>
+        <v>297</v>
       </c>
       <c r="C14" t="s">
         <v>39</v>
@@ -3061,15 +3157,15 @@
         <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>141</v>
+        <v>396</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>149</v>
+        <v>298</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
         <v>42</v>
@@ -3078,15 +3174,15 @@
         <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>155</v>
+        <v>299</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
         <v>42</v>
@@ -3095,46 +3191,46 @@
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>109</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>157</v>
+        <v>300</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
         <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>224</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>159</v>
+        <v>301</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>161</v>
+        <v>302</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -3146,12 +3242,12 @@
         <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>276</v>
+        <v>303</v>
       </c>
       <c r="C20" t="s">
         <v>39</v>
@@ -3163,66 +3259,66 @@
         <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>224</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>293</v>
+        <v>357</v>
       </c>
       <c r="C22" t="s">
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
         <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>223</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>294</v>
+        <v>360</v>
       </c>
       <c r="C23" t="s">
         <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>297</v>
+        <v>361</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
@@ -3231,15 +3327,15 @@
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>396</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>298</v>
+        <v>362</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
         <v>42</v>
@@ -3253,7 +3349,7 @@
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>299</v>
+        <v>365</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
@@ -3265,12 +3361,12 @@
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>398</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>300</v>
+        <v>369</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
@@ -3282,29 +3378,29 @@
         <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>109</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>301</v>
+        <v>376</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
         <v>43</v>
       </c>
       <c r="F28" t="s">
-        <v>263</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>302</v>
+        <v>377</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
@@ -3316,12 +3412,12 @@
         <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>338</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>303</v>
+        <v>378</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
@@ -3333,12 +3429,12 @@
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>262</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>304</v>
+        <v>379</v>
       </c>
       <c r="C31" t="s">
         <v>39</v>
@@ -3350,49 +3446,49 @@
         <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>109</v>
+        <v>347</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>357</v>
+        <v>380</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E32" t="s">
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>375</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E33" t="s">
         <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>75</v>
+        <v>385</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>361</v>
+        <v>382</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
@@ -3401,15 +3497,15 @@
         <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>223</v>
+        <v>383</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>362</v>
+        <v>386</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>
@@ -3418,15 +3514,15 @@
         <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>109</v>
+        <v>389</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
         <v>42</v>
@@ -3435,49 +3531,49 @@
         <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>223</v>
+        <v>390</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>364</v>
+        <v>388</v>
       </c>
       <c r="C37" t="s">
         <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s">
         <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>109</v>
+        <v>392</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>365</v>
+        <v>399</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E38" t="s">
         <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>371</v>
+        <v>400</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>369</v>
+        <v>401</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
         <v>42</v>
@@ -3486,32 +3582,32 @@
         <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>370</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>376</v>
+        <v>402</v>
       </c>
       <c r="C40" t="s">
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E40" t="s">
         <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>340</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>377</v>
+        <v>403</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
         <v>42</v>
@@ -3520,15 +3616,15 @@
         <v>43</v>
       </c>
       <c r="F41" t="s">
-        <v>338</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>378</v>
+        <v>404</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D42" t="s">
         <v>42</v>
@@ -3537,15 +3633,15 @@
         <v>43</v>
       </c>
       <c r="F42" t="s">
-        <v>336</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>379</v>
+        <v>407</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D43" t="s">
         <v>42</v>
@@ -3554,15 +3650,15 @@
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>347</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>380</v>
+        <v>408</v>
       </c>
       <c r="C44" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D44" t="s">
         <v>42</v>
@@ -3576,27 +3672,27 @@
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>381</v>
+        <v>409</v>
       </c>
       <c r="C45" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D45" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E45" t="s">
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>385</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>382</v>
+        <v>410</v>
       </c>
       <c r="C46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D46" t="s">
         <v>42</v>
@@ -3605,15 +3701,15 @@
         <v>43</v>
       </c>
       <c r="F46" t="s">
-        <v>383</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>386</v>
+        <v>411</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
         <v>42</v>
@@ -3622,12 +3718,12 @@
         <v>43</v>
       </c>
       <c r="F47" t="s">
-        <v>389</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>387</v>
+        <v>414</v>
       </c>
       <c r="C48" t="s">
         <v>39</v>
@@ -3639,49 +3735,49 @@
         <v>43</v>
       </c>
       <c r="F48" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>388</v>
+        <v>415</v>
       </c>
       <c r="C49" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D49" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E49" t="s">
         <v>43</v>
       </c>
       <c r="F49" t="s">
-        <v>392</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>399</v>
+        <v>416</v>
       </c>
       <c r="C50" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E50" t="s">
         <v>43</v>
       </c>
       <c r="F50" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>401</v>
+        <v>417</v>
       </c>
       <c r="C51" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D51" t="s">
         <v>42</v>
@@ -3690,15 +3786,15 @@
         <v>43</v>
       </c>
       <c r="F51" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>402</v>
+        <v>418</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D52" t="s">
         <v>42</v>
@@ -3707,15 +3803,15 @@
         <v>43</v>
       </c>
       <c r="F52" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>403</v>
+        <v>419</v>
       </c>
       <c r="C53" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D53" t="s">
         <v>42</v>
@@ -3724,15 +3820,15 @@
         <v>43</v>
       </c>
       <c r="F53" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>404</v>
+        <v>420</v>
       </c>
       <c r="C54" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D54" t="s">
         <v>42</v>
@@ -3741,15 +3837,15 @@
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>109</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>407</v>
+        <v>421</v>
       </c>
       <c r="C55" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
         <v>42</v>
@@ -3758,15 +3854,15 @@
         <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D56" t="s">
         <v>42</v>
@@ -3775,12 +3871,12 @@
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>109</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="C57" t="s">
         <v>37</v>
@@ -3792,63 +3888,63 @@
         <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>75</v>
+        <v>400</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="C58" t="s">
         <v>37</v>
       </c>
       <c r="D58" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E58" t="s">
         <v>43</v>
       </c>
       <c r="F58" t="s">
-        <v>223</v>
+        <v>359</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
       <c r="C59" t="s">
         <v>37</v>
       </c>
       <c r="D59" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E59" t="s">
         <v>43</v>
       </c>
       <c r="F59" t="s">
-        <v>109</v>
+        <v>359</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
       <c r="C60" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D60" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E60" t="s">
         <v>43</v>
       </c>
       <c r="F60" t="s">
-        <v>396</v>
+        <v>340</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>415</v>
+        <v>427</v>
       </c>
       <c r="C61" t="s">
         <v>39</v>
@@ -3860,12 +3956,12 @@
         <v>43</v>
       </c>
       <c r="F61" t="s">
-        <v>109</v>
+        <v>338</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
       <c r="C62" t="s">
         <v>39</v>
@@ -3877,12 +3973,12 @@
         <v>43</v>
       </c>
       <c r="F62" t="s">
-        <v>398</v>
+        <v>336</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="C63" t="s">
         <v>39</v>
@@ -3894,12 +3990,12 @@
         <v>43</v>
       </c>
       <c r="F63" t="s">
-        <v>109</v>
+        <v>347</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>418</v>
+        <v>430</v>
       </c>
       <c r="C64" t="s">
         <v>39</v>
@@ -3911,12 +4007,12 @@
         <v>43</v>
       </c>
       <c r="F64" t="s">
-        <v>263</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>419</v>
+        <v>431</v>
       </c>
       <c r="C65" t="s">
         <v>39</v>
@@ -3928,12 +4024,12 @@
         <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>109</v>
+        <v>385</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>420</v>
+        <v>432</v>
       </c>
       <c r="C66" t="s">
         <v>39</v>
@@ -3945,12 +4041,12 @@
         <v>43</v>
       </c>
       <c r="F66" t="s">
-        <v>262</v>
+        <v>442</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="C67" t="s">
         <v>39</v>
@@ -3962,12 +4058,12 @@
         <v>43</v>
       </c>
       <c r="F67" t="s">
-        <v>109</v>
+        <v>389</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>422</v>
+        <v>434</v>
       </c>
       <c r="C68" t="s">
         <v>39</v>
@@ -3979,12 +4075,12 @@
         <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>225</v>
+        <v>390</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="C69" t="s">
         <v>37</v>
@@ -3996,46 +4092,46 @@
         <v>43</v>
       </c>
       <c r="F69" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="C70" t="s">
         <v>37</v>
       </c>
       <c r="D70" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E70" t="s">
         <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>359</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="C71" t="s">
         <v>37</v>
       </c>
       <c r="D71" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E71" t="s">
         <v>43</v>
       </c>
       <c r="F71" t="s">
-        <v>359</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="C72" t="s">
         <v>37</v>
@@ -4047,29 +4143,29 @@
         <v>43</v>
       </c>
       <c r="F72" t="s">
-        <v>340</v>
+        <v>392</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D73" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E73" t="s">
         <v>43</v>
       </c>
       <c r="F73" t="s">
-        <v>338</v>
+        <v>392</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>428</v>
+        <v>443</v>
       </c>
       <c r="C74" t="s">
         <v>39</v>
@@ -4081,12 +4177,12 @@
         <v>43</v>
       </c>
       <c r="F74" t="s">
-        <v>336</v>
+        <v>450</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>429</v>
+        <v>444</v>
       </c>
       <c r="C75" t="s">
         <v>39</v>
@@ -4098,12 +4194,12 @@
         <v>43</v>
       </c>
       <c r="F75" t="s">
-        <v>347</v>
+        <v>109</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>430</v>
+        <v>446</v>
       </c>
       <c r="C76" t="s">
         <v>39</v>
@@ -4115,12 +4211,12 @@
         <v>43</v>
       </c>
       <c r="F76" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>431</v>
+        <v>447</v>
       </c>
       <c r="C77" t="s">
         <v>39</v>
@@ -4132,12 +4228,12 @@
         <v>43</v>
       </c>
       <c r="F77" t="s">
-        <v>385</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>432</v>
+        <v>453</v>
       </c>
       <c r="C78" t="s">
         <v>39</v>
@@ -4149,12 +4245,12 @@
         <v>43</v>
       </c>
       <c r="F78" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>433</v>
+        <v>454</v>
       </c>
       <c r="C79" t="s">
         <v>39</v>
@@ -4166,12 +4262,12 @@
         <v>43</v>
       </c>
       <c r="F79" t="s">
-        <v>389</v>
+        <v>109</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>434</v>
+        <v>455</v>
       </c>
       <c r="C80" t="s">
         <v>39</v>
@@ -4183,32 +4279,32 @@
         <v>43</v>
       </c>
       <c r="F80" t="s">
-        <v>390</v>
+        <v>452</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>435</v>
+        <v>456</v>
       </c>
       <c r="C81" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D81" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E81" t="s">
         <v>43</v>
       </c>
       <c r="F81" t="s">
-        <v>392</v>
+        <v>109</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>436</v>
+        <v>457</v>
       </c>
       <c r="C82" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D82" t="s">
         <v>42</v>
@@ -4217,15 +4313,15 @@
         <v>43</v>
       </c>
       <c r="F82" t="s">
-        <v>223</v>
+        <v>391</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>437</v>
+        <v>458</v>
       </c>
       <c r="C83" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D83" t="s">
         <v>42</v>
@@ -4234,49 +4330,49 @@
         <v>43</v>
       </c>
       <c r="F83" t="s">
-        <v>109</v>
+        <v>460</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>438</v>
+        <v>459</v>
       </c>
       <c r="C84" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D84" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E84" t="s">
         <v>43</v>
       </c>
       <c r="F84" t="s">
-        <v>392</v>
+        <v>461</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>439</v>
+        <v>462</v>
       </c>
       <c r="C85" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D85" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E85" t="s">
         <v>43</v>
       </c>
       <c r="F85" t="s">
-        <v>392</v>
+        <v>463</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>443</v>
+        <v>464</v>
       </c>
       <c r="C86" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D86" t="s">
         <v>42</v>
@@ -4285,49 +4381,49 @@
         <v>43</v>
       </c>
       <c r="F86" t="s">
-        <v>450</v>
+        <v>465</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>444</v>
+        <v>467</v>
       </c>
       <c r="C87" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D87" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E87" t="s">
         <v>43</v>
       </c>
       <c r="F87" t="s">
-        <v>109</v>
+        <v>468</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>446</v>
+        <v>469</v>
       </c>
       <c r="C88" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D88" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E88" t="s">
         <v>43</v>
       </c>
       <c r="F88" t="s">
-        <v>452</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>447</v>
+        <v>470</v>
       </c>
       <c r="C89" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D89" t="s">
         <v>42</v>
@@ -4336,15 +4432,15 @@
         <v>43</v>
       </c>
       <c r="F89" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>453</v>
+        <v>471</v>
       </c>
       <c r="C90" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D90" t="s">
         <v>42</v>
@@ -4353,12 +4449,12 @@
         <v>43</v>
       </c>
       <c r="F90" t="s">
-        <v>450</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>454</v>
+        <v>472</v>
       </c>
       <c r="C91" t="s">
         <v>39</v>
@@ -4370,12 +4466,12 @@
         <v>43</v>
       </c>
       <c r="F91" t="s">
-        <v>109</v>
+        <v>396</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>455</v>
+        <v>473</v>
       </c>
       <c r="C92" t="s">
         <v>39</v>
@@ -4387,12 +4483,12 @@
         <v>43</v>
       </c>
       <c r="F92" t="s">
-        <v>452</v>
+        <v>109</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>456</v>
+        <v>474</v>
       </c>
       <c r="C93" t="s">
         <v>39</v>
@@ -4404,13 +4500,181 @@
         <v>43</v>
       </c>
       <c r="F93" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="s">
+        <v>475</v>
+      </c>
+      <c r="C94" t="s">
+        <v>39</v>
+      </c>
+      <c r="D94" t="s">
+        <v>42</v>
+      </c>
+      <c r="E94" t="s">
+        <v>43</v>
+      </c>
+      <c r="F94" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
+    <row r="95">
+      <c r="B95" t="s">
+        <v>476</v>
+      </c>
+      <c r="C95" t="s">
+        <v>39</v>
+      </c>
+      <c r="D95" t="s">
+        <v>42</v>
+      </c>
+      <c r="E95" t="s">
+        <v>43</v>
+      </c>
+      <c r="F95" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="s">
+        <v>477</v>
+      </c>
+      <c r="C96" t="s">
+        <v>39</v>
+      </c>
+      <c r="D96" t="s">
+        <v>42</v>
+      </c>
+      <c r="E96" t="s">
+        <v>43</v>
+      </c>
+      <c r="F96" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="s">
+        <v>478</v>
+      </c>
+      <c r="C97" t="s">
+        <v>39</v>
+      </c>
+      <c r="D97" t="s">
+        <v>42</v>
+      </c>
+      <c r="E97" t="s">
+        <v>43</v>
+      </c>
+      <c r="F97" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="s">
+        <v>479</v>
+      </c>
+      <c r="C98" t="s">
+        <v>39</v>
+      </c>
+      <c r="D98" t="s">
+        <v>42</v>
+      </c>
+      <c r="E98" t="s">
+        <v>43</v>
+      </c>
+      <c r="F98" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="s">
+        <v>480</v>
+      </c>
+      <c r="C99" t="s">
+        <v>39</v>
+      </c>
+      <c r="D99" t="s">
+        <v>42</v>
+      </c>
+      <c r="E99" t="s">
+        <v>43</v>
+      </c>
+      <c r="F99" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="s">
+        <v>484</v>
+      </c>
+      <c r="C100" t="s">
+        <v>39</v>
+      </c>
+      <c r="D100" t="s">
+        <v>42</v>
+      </c>
+      <c r="E100" t="s">
+        <v>43</v>
+      </c>
+      <c r="F100" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="s">
+        <v>485</v>
+      </c>
+      <c r="C101" t="s">
+        <v>39</v>
+      </c>
+      <c r="D101" t="s">
+        <v>42</v>
+      </c>
+      <c r="E101" t="s">
+        <v>43</v>
+      </c>
+      <c r="F101" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="s">
+        <v>486</v>
+      </c>
+      <c r="C102" t="s">
+        <v>39</v>
+      </c>
+      <c r="D102" t="s">
+        <v>42</v>
+      </c>
+      <c r="E102" t="s">
+        <v>43</v>
+      </c>
+      <c r="F102" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="s">
+        <v>487</v>
+      </c>
+      <c r="C103" t="s">
+        <v>39</v>
+      </c>
+      <c r="D103" t="s">
+        <v>42</v>
+      </c>
+      <c r="E103" t="s">
+        <v>43</v>
+      </c>
+      <c r="F103" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="104"/>
+    <row r="105"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
major GUI modification, added #ifdefs to enable touchgfx simulator again
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124793" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147317" uniqueCount="556">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1528,6 +1528,207 @@
   </si>
   <si>
     <t xml:space="preserve">UART RX Debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID:      &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current      &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage:      &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency:          &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P  &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power:            &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current           &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency:      &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage:          &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Param1:           &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Param2:          &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Param1:          &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage         &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power             &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage           &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency       &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Param2           &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Param1           &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable Parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage            &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage           &lt;value&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power             &lt;value&gt;W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current           &lt;value&gt;A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency       &lt;value&gt;Hz</t>
   </si>
 </sst>
 </file>
@@ -3157,7 +3358,7 @@
         <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>396</v>
+        <v>506</v>
       </c>
     </row>
     <row r="15">
@@ -3191,7 +3392,7 @@
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>398</v>
+        <v>553</v>
       </c>
     </row>
     <row r="17">
@@ -3225,7 +3426,7 @@
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>263</v>
+        <v>554</v>
       </c>
     </row>
     <row r="19">
@@ -3259,7 +3460,7 @@
         <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>262</v>
+        <v>552</v>
       </c>
     </row>
     <row r="21">
@@ -4245,7 +4446,7 @@
         <v>43</v>
       </c>
       <c r="F78" t="s">
-        <v>450</v>
+        <v>555</v>
       </c>
     </row>
     <row r="79">
@@ -4279,7 +4480,7 @@
         <v>43</v>
       </c>
       <c r="F80" t="s">
-        <v>452</v>
+        <v>507</v>
       </c>
     </row>
     <row r="81">
@@ -4369,24 +4570,24 @@
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="C86" t="s">
         <v>37</v>
       </c>
       <c r="D86" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E86" t="s">
         <v>43</v>
       </c>
       <c r="F86" t="s">
-        <v>465</v>
+        <v>548</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C87" t="s">
         <v>37</v>
@@ -4398,29 +4599,29 @@
         <v>43</v>
       </c>
       <c r="F87" t="s">
-        <v>468</v>
+        <v>75</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C88" t="s">
         <v>37</v>
       </c>
       <c r="D88" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E88" t="s">
         <v>43</v>
       </c>
       <c r="F88" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C89" t="s">
         <v>37</v>
@@ -4432,15 +4633,15 @@
         <v>43</v>
       </c>
       <c r="F89" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C90" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D90" t="s">
         <v>42</v>
@@ -4449,12 +4650,12 @@
         <v>43</v>
       </c>
       <c r="F90" t="s">
-        <v>109</v>
+        <v>396</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C91" t="s">
         <v>39</v>
@@ -4466,12 +4667,12 @@
         <v>43</v>
       </c>
       <c r="F91" t="s">
-        <v>396</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C92" t="s">
         <v>39</v>
@@ -4483,12 +4684,12 @@
         <v>43</v>
       </c>
       <c r="F92" t="s">
-        <v>109</v>
+        <v>398</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C93" t="s">
         <v>39</v>
@@ -4500,12 +4701,12 @@
         <v>43</v>
       </c>
       <c r="F93" t="s">
-        <v>398</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C94" t="s">
         <v>39</v>
@@ -4517,12 +4718,12 @@
         <v>43</v>
       </c>
       <c r="F94" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C95" t="s">
         <v>39</v>
@@ -4534,12 +4735,12 @@
         <v>43</v>
       </c>
       <c r="F95" t="s">
-        <v>263</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C96" t="s">
         <v>39</v>
@@ -4551,12 +4752,12 @@
         <v>43</v>
       </c>
       <c r="F96" t="s">
-        <v>109</v>
+        <v>262</v>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C97" t="s">
         <v>39</v>
@@ -4568,12 +4769,12 @@
         <v>43</v>
       </c>
       <c r="F97" t="s">
-        <v>262</v>
+        <v>109</v>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C98" t="s">
         <v>39</v>
@@ -4585,12 +4786,12 @@
         <v>43</v>
       </c>
       <c r="F98" t="s">
-        <v>109</v>
+        <v>488</v>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="C99" t="s">
         <v>39</v>
@@ -4602,12 +4803,12 @@
         <v>43</v>
       </c>
       <c r="F99" t="s">
-        <v>488</v>
+        <v>450</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C100" t="s">
         <v>39</v>
@@ -4619,12 +4820,12 @@
         <v>43</v>
       </c>
       <c r="F100" t="s">
-        <v>450</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C101" t="s">
         <v>39</v>
@@ -4636,12 +4837,12 @@
         <v>43</v>
       </c>
       <c r="F101" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C102" t="s">
         <v>39</v>
@@ -4653,12 +4854,12 @@
         <v>43</v>
       </c>
       <c r="F102" t="s">
-        <v>452</v>
+        <v>109</v>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="s">
-        <v>487</v>
+        <v>508</v>
       </c>
       <c r="C103" t="s">
         <v>39</v>
@@ -4670,11 +4871,622 @@
         <v>43</v>
       </c>
       <c r="F103" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="s">
+        <v>509</v>
+      </c>
+      <c r="C104" t="s">
+        <v>39</v>
+      </c>
+      <c r="D104" t="s">
+        <v>42</v>
+      </c>
+      <c r="E104" t="s">
+        <v>43</v>
+      </c>
+      <c r="F104" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="104"/>
-    <row r="105"/>
+    <row r="105">
+      <c r="B105" t="s">
+        <v>510</v>
+      </c>
+      <c r="C105" t="s">
+        <v>39</v>
+      </c>
+      <c r="D105" t="s">
+        <v>42</v>
+      </c>
+      <c r="E105" t="s">
+        <v>43</v>
+      </c>
+      <c r="F105" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" t="s">
+        <v>511</v>
+      </c>
+      <c r="C106" t="s">
+        <v>39</v>
+      </c>
+      <c r="D106" t="s">
+        <v>42</v>
+      </c>
+      <c r="E106" t="s">
+        <v>43</v>
+      </c>
+      <c r="F106" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" t="s">
+        <v>512</v>
+      </c>
+      <c r="C107" t="s">
+        <v>39</v>
+      </c>
+      <c r="D107" t="s">
+        <v>42</v>
+      </c>
+      <c r="E107" t="s">
+        <v>43</v>
+      </c>
+      <c r="F107" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" t="s">
+        <v>513</v>
+      </c>
+      <c r="C108" t="s">
+        <v>39</v>
+      </c>
+      <c r="D108" t="s">
+        <v>42</v>
+      </c>
+      <c r="E108" t="s">
+        <v>43</v>
+      </c>
+      <c r="F108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" t="s">
+        <v>514</v>
+      </c>
+      <c r="C109" t="s">
+        <v>39</v>
+      </c>
+      <c r="D109" t="s">
+        <v>42</v>
+      </c>
+      <c r="E109" t="s">
+        <v>43</v>
+      </c>
+      <c r="F109" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" t="s">
+        <v>515</v>
+      </c>
+      <c r="C110" t="s">
+        <v>39</v>
+      </c>
+      <c r="D110" t="s">
+        <v>42</v>
+      </c>
+      <c r="E110" t="s">
+        <v>43</v>
+      </c>
+      <c r="F110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" t="s">
+        <v>516</v>
+      </c>
+      <c r="C111" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" t="s">
+        <v>42</v>
+      </c>
+      <c r="E111" t="s">
+        <v>43</v>
+      </c>
+      <c r="F111" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="B112" t="s">
+        <v>517</v>
+      </c>
+      <c r="C112" t="s">
+        <v>39</v>
+      </c>
+      <c r="D112" t="s">
+        <v>42</v>
+      </c>
+      <c r="E112" t="s">
+        <v>43</v>
+      </c>
+      <c r="F112" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113" t="s">
+        <v>518</v>
+      </c>
+      <c r="C113" t="s">
+        <v>39</v>
+      </c>
+      <c r="D113" t="s">
+        <v>42</v>
+      </c>
+      <c r="E113" t="s">
+        <v>43</v>
+      </c>
+      <c r="F113" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" t="s">
+        <v>519</v>
+      </c>
+      <c r="C114" t="s">
+        <v>39</v>
+      </c>
+      <c r="D114" t="s">
+        <v>42</v>
+      </c>
+      <c r="E114" t="s">
+        <v>43</v>
+      </c>
+      <c r="F114" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="B115" t="s">
+        <v>520</v>
+      </c>
+      <c r="C115" t="s">
+        <v>39</v>
+      </c>
+      <c r="D115" t="s">
+        <v>42</v>
+      </c>
+      <c r="E115" t="s">
+        <v>43</v>
+      </c>
+      <c r="F115" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="B116" t="s">
+        <v>521</v>
+      </c>
+      <c r="C116" t="s">
+        <v>39</v>
+      </c>
+      <c r="D116" t="s">
+        <v>42</v>
+      </c>
+      <c r="E116" t="s">
+        <v>43</v>
+      </c>
+      <c r="F116" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117" t="s">
+        <v>522</v>
+      </c>
+      <c r="C117" t="s">
+        <v>39</v>
+      </c>
+      <c r="D117" t="s">
+        <v>42</v>
+      </c>
+      <c r="E117" t="s">
+        <v>43</v>
+      </c>
+      <c r="F117" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="B118" t="s">
+        <v>523</v>
+      </c>
+      <c r="C118" t="s">
+        <v>39</v>
+      </c>
+      <c r="D118" t="s">
+        <v>42</v>
+      </c>
+      <c r="E118" t="s">
+        <v>43</v>
+      </c>
+      <c r="F118" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119" t="s">
+        <v>524</v>
+      </c>
+      <c r="C119" t="s">
+        <v>39</v>
+      </c>
+      <c r="D119" t="s">
+        <v>42</v>
+      </c>
+      <c r="E119" t="s">
+        <v>43</v>
+      </c>
+      <c r="F119" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" t="s">
+        <v>525</v>
+      </c>
+      <c r="C120" t="s">
+        <v>39</v>
+      </c>
+      <c r="D120" t="s">
+        <v>42</v>
+      </c>
+      <c r="E120" t="s">
+        <v>43</v>
+      </c>
+      <c r="F120" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="B121" t="s">
+        <v>526</v>
+      </c>
+      <c r="C121" t="s">
+        <v>39</v>
+      </c>
+      <c r="D121" t="s">
+        <v>42</v>
+      </c>
+      <c r="E121" t="s">
+        <v>43</v>
+      </c>
+      <c r="F121" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122" t="s">
+        <v>527</v>
+      </c>
+      <c r="C122" t="s">
+        <v>39</v>
+      </c>
+      <c r="D122" t="s">
+        <v>42</v>
+      </c>
+      <c r="E122" t="s">
+        <v>43</v>
+      </c>
+      <c r="F122" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123" t="s">
+        <v>528</v>
+      </c>
+      <c r="C123" t="s">
+        <v>39</v>
+      </c>
+      <c r="D123" t="s">
+        <v>42</v>
+      </c>
+      <c r="E123" t="s">
+        <v>43</v>
+      </c>
+      <c r="F123" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="B124" t="s">
+        <v>529</v>
+      </c>
+      <c r="C124" t="s">
+        <v>39</v>
+      </c>
+      <c r="D124" t="s">
+        <v>42</v>
+      </c>
+      <c r="E124" t="s">
+        <v>43</v>
+      </c>
+      <c r="F124" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125" t="s">
+        <v>530</v>
+      </c>
+      <c r="C125" t="s">
+        <v>39</v>
+      </c>
+      <c r="D125" t="s">
+        <v>42</v>
+      </c>
+      <c r="E125" t="s">
+        <v>43</v>
+      </c>
+      <c r="F125" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126" t="s">
+        <v>531</v>
+      </c>
+      <c r="C126" t="s">
+        <v>39</v>
+      </c>
+      <c r="D126" t="s">
+        <v>42</v>
+      </c>
+      <c r="E126" t="s">
+        <v>43</v>
+      </c>
+      <c r="F126" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" t="s">
+        <v>532</v>
+      </c>
+      <c r="C127" t="s">
+        <v>39</v>
+      </c>
+      <c r="D127" t="s">
+        <v>42</v>
+      </c>
+      <c r="E127" t="s">
+        <v>43</v>
+      </c>
+      <c r="F127" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128" t="s">
+        <v>533</v>
+      </c>
+      <c r="C128" t="s">
+        <v>39</v>
+      </c>
+      <c r="D128" t="s">
+        <v>42</v>
+      </c>
+      <c r="E128" t="s">
+        <v>43</v>
+      </c>
+      <c r="F128" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" t="s">
+        <v>534</v>
+      </c>
+      <c r="C129" t="s">
+        <v>39</v>
+      </c>
+      <c r="D129" t="s">
+        <v>42</v>
+      </c>
+      <c r="E129" t="s">
+        <v>43</v>
+      </c>
+      <c r="F129" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" t="s">
+        <v>535</v>
+      </c>
+      <c r="C130" t="s">
+        <v>39</v>
+      </c>
+      <c r="D130" t="s">
+        <v>42</v>
+      </c>
+      <c r="E130" t="s">
+        <v>43</v>
+      </c>
+      <c r="F130" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" t="s">
+        <v>536</v>
+      </c>
+      <c r="C131" t="s">
+        <v>39</v>
+      </c>
+      <c r="D131" t="s">
+        <v>42</v>
+      </c>
+      <c r="E131" t="s">
+        <v>43</v>
+      </c>
+      <c r="F131" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" t="s">
+        <v>537</v>
+      </c>
+      <c r="C132" t="s">
+        <v>39</v>
+      </c>
+      <c r="D132" t="s">
+        <v>42</v>
+      </c>
+      <c r="E132" t="s">
+        <v>43</v>
+      </c>
+      <c r="F132" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" t="s">
+        <v>538</v>
+      </c>
+      <c r="C133" t="s">
+        <v>39</v>
+      </c>
+      <c r="D133" t="s">
+        <v>42</v>
+      </c>
+      <c r="E133" t="s">
+        <v>43</v>
+      </c>
+      <c r="F133" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" t="s">
+        <v>539</v>
+      </c>
+      <c r="C134" t="s">
+        <v>39</v>
+      </c>
+      <c r="D134" t="s">
+        <v>42</v>
+      </c>
+      <c r="E134" t="s">
+        <v>43</v>
+      </c>
+      <c r="F134" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135" t="s">
+        <v>540</v>
+      </c>
+      <c r="C135" t="s">
+        <v>39</v>
+      </c>
+      <c r="D135" t="s">
+        <v>42</v>
+      </c>
+      <c r="E135" t="s">
+        <v>43</v>
+      </c>
+      <c r="F135" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" t="s">
+        <v>541</v>
+      </c>
+      <c r="C136" t="s">
+        <v>39</v>
+      </c>
+      <c r="D136" t="s">
+        <v>42</v>
+      </c>
+      <c r="E136" t="s">
+        <v>43</v>
+      </c>
+      <c r="F136" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137" t="s">
+        <v>544</v>
+      </c>
+      <c r="C137" t="s">
+        <v>39</v>
+      </c>
+      <c r="D137" t="s">
+        <v>42</v>
+      </c>
+      <c r="E137" t="s">
+        <v>43</v>
+      </c>
+      <c r="F137" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" t="s">
+        <v>545</v>
+      </c>
+      <c r="C138" t="s">
+        <v>39</v>
+      </c>
+      <c r="D138" t="s">
+        <v>42</v>
+      </c>
+      <c r="E138" t="s">
+        <v>43</v>
+      </c>
+      <c r="F138" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="B139" t="s">
+        <v>546</v>
+      </c>
+      <c r="C139" t="s">
+        <v>37</v>
+      </c>
+      <c r="D139" t="s">
+        <v>55</v>
+      </c>
+      <c r="E139" t="s">
+        <v>43</v>
+      </c>
+      <c r="F139" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="140"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
changed "type" field to "function" field in UART frame
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147317" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148125" uniqueCount="556">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3346,7 +3346,7 @@
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C14" t="s">
         <v>39</v>
@@ -3358,12 +3358,12 @@
         <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>506</v>
+        <v>553</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
@@ -3380,7 +3380,7 @@
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C16" t="s">
         <v>39</v>
@@ -3392,12 +3392,12 @@
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
@@ -3414,7 +3414,7 @@
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -3426,12 +3426,12 @@
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -3448,78 +3448,78 @@
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>303</v>
+        <v>357</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
         <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>552</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>304</v>
+        <v>360</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="C22" t="s">
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E22" t="s">
         <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>375</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C23" t="s">
         <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
@@ -3528,15 +3528,15 @@
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>223</v>
+        <v>371</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
         <v>42</v>
@@ -3545,29 +3545,29 @@
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>109</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>371</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
@@ -3579,29 +3579,29 @@
         <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>370</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
         <v>43</v>
       </c>
       <c r="F28" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
@@ -3613,12 +3613,12 @@
         <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
@@ -3630,15 +3630,15 @@
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>336</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
         <v>42</v>
@@ -3647,12 +3647,12 @@
         <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>347</v>
+        <v>385</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C32" t="s">
         <v>39</v>
@@ -3664,15 +3664,15 @@
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>109</v>
+        <v>383</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
@@ -3681,12 +3681,12 @@
         <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="C34" t="s">
         <v>39</v>
@@ -3698,80 +3698,80 @@
         <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
         <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E36" t="s">
         <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>388</v>
+        <v>401</v>
       </c>
       <c r="C37" t="s">
         <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E37" t="s">
         <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>392</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="C38" t="s">
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E38" t="s">
         <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>400</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C39" t="s">
         <v>37</v>
@@ -3788,7 +3788,7 @@
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C40" t="s">
         <v>37</v>
@@ -3805,7 +3805,7 @@
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="C41" t="s">
         <v>37</v>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="C42" t="s">
         <v>37</v>
@@ -3839,24 +3839,24 @@
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C43" t="s">
         <v>37</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E43" t="s">
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>223</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C44" t="s">
         <v>37</v>
@@ -3868,32 +3868,32 @@
         <v>43</v>
       </c>
       <c r="F44" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C45" t="s">
         <v>37</v>
       </c>
       <c r="D45" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E45" t="s">
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D46" t="s">
         <v>42</v>
@@ -3902,15 +3902,15 @@
         <v>43</v>
       </c>
       <c r="F46" t="s">
-        <v>223</v>
+        <v>396</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D47" t="s">
         <v>42</v>
@@ -3924,7 +3924,7 @@
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C48" t="s">
         <v>39</v>
@@ -3936,12 +3936,12 @@
         <v>43</v>
       </c>
       <c r="F48" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C49" t="s">
         <v>39</v>
@@ -3958,7 +3958,7 @@
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C50" t="s">
         <v>39</v>
@@ -3970,12 +3970,12 @@
         <v>43</v>
       </c>
       <c r="F50" t="s">
-        <v>398</v>
+        <v>263</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C51" t="s">
         <v>39</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C52" t="s">
         <v>39</v>
@@ -4004,12 +4004,12 @@
         <v>43</v>
       </c>
       <c r="F52" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C53" t="s">
         <v>39</v>
@@ -4026,7 +4026,7 @@
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
@@ -4038,46 +4038,46 @@
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C55" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D55" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E55" t="s">
         <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>109</v>
+        <v>400</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C56" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D56" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E56" t="s">
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>225</v>
+        <v>359</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C57" t="s">
         <v>37</v>
@@ -4089,12 +4089,12 @@
         <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>400</v>
+        <v>359</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C58" t="s">
         <v>37</v>
@@ -4106,46 +4106,46 @@
         <v>43</v>
       </c>
       <c r="F58" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D59" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E59" t="s">
         <v>43</v>
       </c>
       <c r="F59" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D60" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E60" t="s">
         <v>43</v>
       </c>
       <c r="F60" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C61" t="s">
         <v>39</v>
@@ -4157,12 +4157,12 @@
         <v>43</v>
       </c>
       <c r="F61" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C62" t="s">
         <v>39</v>
@@ -4174,12 +4174,12 @@
         <v>43</v>
       </c>
       <c r="F62" t="s">
-        <v>336</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C63" t="s">
         <v>39</v>
@@ -4191,12 +4191,12 @@
         <v>43</v>
       </c>
       <c r="F63" t="s">
-        <v>347</v>
+        <v>385</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C64" t="s">
         <v>39</v>
@@ -4208,12 +4208,12 @@
         <v>43</v>
       </c>
       <c r="F64" t="s">
-        <v>109</v>
+        <v>442</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C65" t="s">
         <v>39</v>
@@ -4225,12 +4225,12 @@
         <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C66" t="s">
         <v>39</v>
@@ -4242,32 +4242,32 @@
         <v>43</v>
       </c>
       <c r="F66" t="s">
-        <v>442</v>
+        <v>390</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C67" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D67" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E67" t="s">
         <v>43</v>
       </c>
       <c r="F67" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C68" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D68" t="s">
         <v>42</v>
@@ -4276,97 +4276,97 @@
         <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>390</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C69" t="s">
         <v>37</v>
       </c>
       <c r="D69" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E69" t="s">
         <v>43</v>
       </c>
       <c r="F69" t="s">
-        <v>392</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C70" t="s">
         <v>37</v>
       </c>
       <c r="D70" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E70" t="s">
         <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>223</v>
+        <v>392</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C71" t="s">
         <v>37</v>
       </c>
       <c r="D71" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E71" t="s">
         <v>43</v>
       </c>
       <c r="F71" t="s">
-        <v>109</v>
+        <v>392</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="C72" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D72" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E72" t="s">
         <v>43</v>
       </c>
       <c r="F72" t="s">
-        <v>392</v>
+        <v>450</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="C73" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D73" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E73" t="s">
         <v>43</v>
       </c>
       <c r="F73" t="s">
-        <v>392</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C74" t="s">
         <v>39</v>
@@ -4378,12 +4378,12 @@
         <v>43</v>
       </c>
       <c r="F74" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="C75" t="s">
         <v>39</v>
@@ -4400,7 +4400,7 @@
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="C76" t="s">
         <v>39</v>
@@ -4412,12 +4412,12 @@
         <v>43</v>
       </c>
       <c r="F76" t="s">
-        <v>452</v>
+        <v>555</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="C77" t="s">
         <v>39</v>
@@ -4434,7 +4434,7 @@
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="C78" t="s">
         <v>39</v>
@@ -4446,12 +4446,12 @@
         <v>43</v>
       </c>
       <c r="F78" t="s">
-        <v>555</v>
+        <v>391</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="C79" t="s">
         <v>39</v>
@@ -4463,12 +4463,12 @@
         <v>43</v>
       </c>
       <c r="F79" t="s">
-        <v>109</v>
+        <v>460</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="C80" t="s">
         <v>39</v>
@@ -4480,12 +4480,12 @@
         <v>43</v>
       </c>
       <c r="F80" t="s">
-        <v>507</v>
+        <v>461</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="C81" t="s">
         <v>39</v>
@@ -4497,49 +4497,49 @@
         <v>43</v>
       </c>
       <c r="F81" t="s">
-        <v>109</v>
+        <v>463</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="C82" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D82" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E82" t="s">
         <v>43</v>
       </c>
       <c r="F82" t="s">
-        <v>391</v>
+        <v>548</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="C83" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D83" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E83" t="s">
         <v>43</v>
       </c>
       <c r="F83" t="s">
-        <v>460</v>
+        <v>75</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>459</v>
+        <v>470</v>
       </c>
       <c r="C84" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D84" t="s">
         <v>42</v>
@@ -4548,15 +4548,15 @@
         <v>43</v>
       </c>
       <c r="F84" t="s">
-        <v>461</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="C85" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D85" t="s">
         <v>42</v>
@@ -4565,49 +4565,49 @@
         <v>43</v>
       </c>
       <c r="F85" t="s">
-        <v>463</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="C86" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D86" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E86" t="s">
         <v>43</v>
       </c>
       <c r="F86" t="s">
-        <v>548</v>
+        <v>396</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="C87" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D87" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E87" t="s">
         <v>43</v>
       </c>
       <c r="F87" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="C88" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D88" t="s">
         <v>42</v>
@@ -4616,15 +4616,15 @@
         <v>43</v>
       </c>
       <c r="F88" t="s">
-        <v>223</v>
+        <v>398</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C89" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D89" t="s">
         <v>42</v>
@@ -4638,7 +4638,7 @@
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="C90" t="s">
         <v>39</v>
@@ -4650,12 +4650,12 @@
         <v>43</v>
       </c>
       <c r="F90" t="s">
-        <v>396</v>
+        <v>263</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="C91" t="s">
         <v>39</v>
@@ -4672,7 +4672,7 @@
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="C92" t="s">
         <v>39</v>
@@ -4684,12 +4684,12 @@
         <v>43</v>
       </c>
       <c r="F92" t="s">
-        <v>398</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="C93" t="s">
         <v>39</v>
@@ -4706,7 +4706,7 @@
     </row>
     <row r="94">
       <c r="B94" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="C94" t="s">
         <v>39</v>
@@ -4718,12 +4718,12 @@
         <v>43</v>
       </c>
       <c r="F94" t="s">
-        <v>263</v>
+        <v>488</v>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="C95" t="s">
         <v>39</v>
@@ -4735,12 +4735,12 @@
         <v>43</v>
       </c>
       <c r="F95" t="s">
-        <v>109</v>
+        <v>450</v>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="C96" t="s">
         <v>39</v>
@@ -4752,12 +4752,12 @@
         <v>43</v>
       </c>
       <c r="F96" t="s">
-        <v>262</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="C97" t="s">
         <v>39</v>
@@ -4769,12 +4769,12 @@
         <v>43</v>
       </c>
       <c r="F97" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="C98" t="s">
         <v>39</v>
@@ -4786,12 +4786,12 @@
         <v>43</v>
       </c>
       <c r="F98" t="s">
-        <v>488</v>
+        <v>109</v>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="s">
-        <v>484</v>
+        <v>508</v>
       </c>
       <c r="C99" t="s">
         <v>39</v>
@@ -4803,12 +4803,12 @@
         <v>43</v>
       </c>
       <c r="F99" t="s">
-        <v>450</v>
+        <v>506</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="s">
-        <v>485</v>
+        <v>509</v>
       </c>
       <c r="C100" t="s">
         <v>39</v>
@@ -4825,7 +4825,7 @@
     </row>
     <row r="101">
       <c r="B101" t="s">
-        <v>486</v>
+        <v>510</v>
       </c>
       <c r="C101" t="s">
         <v>39</v>
@@ -4837,12 +4837,12 @@
         <v>43</v>
       </c>
       <c r="F101" t="s">
-        <v>452</v>
+        <v>507</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="s">
-        <v>487</v>
+        <v>511</v>
       </c>
       <c r="C102" t="s">
         <v>39</v>
@@ -4859,7 +4859,7 @@
     </row>
     <row r="103">
       <c r="B103" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="C103" t="s">
         <v>39</v>
@@ -4871,12 +4871,12 @@
         <v>43</v>
       </c>
       <c r="F103" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="C104" t="s">
         <v>39</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="105">
       <c r="B105" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="C105" t="s">
         <v>39</v>
@@ -4905,12 +4905,12 @@
         <v>43</v>
       </c>
       <c r="F105" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="C106" t="s">
         <v>39</v>
@@ -4927,7 +4927,7 @@
     </row>
     <row r="107">
       <c r="B107" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="C107" t="s">
         <v>39</v>
@@ -4939,12 +4939,12 @@
         <v>43</v>
       </c>
       <c r="F107" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
     </row>
     <row r="108">
       <c r="B108" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="C108" t="s">
         <v>39</v>
@@ -4961,7 +4961,7 @@
     </row>
     <row r="109">
       <c r="B109" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="C109" t="s">
         <v>39</v>
@@ -4973,12 +4973,12 @@
         <v>43</v>
       </c>
       <c r="F109" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="110">
       <c r="B110" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="C110" t="s">
         <v>39</v>
@@ -4995,7 +4995,7 @@
     </row>
     <row r="111">
       <c r="B111" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="C111" t="s">
         <v>39</v>
@@ -5007,12 +5007,12 @@
         <v>43</v>
       </c>
       <c r="F111" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
     </row>
     <row r="112">
       <c r="B112" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="C112" t="s">
         <v>39</v>
@@ -5029,7 +5029,7 @@
     </row>
     <row r="113">
       <c r="B113" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="C113" t="s">
         <v>39</v>
@@ -5041,12 +5041,12 @@
         <v>43</v>
       </c>
       <c r="F113" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="114">
       <c r="B114" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="C114" t="s">
         <v>39</v>
@@ -5063,7 +5063,7 @@
     </row>
     <row r="115">
       <c r="B115" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="C115" t="s">
         <v>39</v>
@@ -5075,12 +5075,12 @@
         <v>43</v>
       </c>
       <c r="F115" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="116">
       <c r="B116" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="C116" t="s">
         <v>39</v>
@@ -5097,7 +5097,7 @@
     </row>
     <row r="117">
       <c r="B117" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="C117" t="s">
         <v>39</v>
@@ -5109,12 +5109,12 @@
         <v>43</v>
       </c>
       <c r="F117" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="118">
       <c r="B118" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="C118" t="s">
         <v>39</v>
@@ -5131,7 +5131,7 @@
     </row>
     <row r="119">
       <c r="B119" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="C119" t="s">
         <v>39</v>
@@ -5143,12 +5143,12 @@
         <v>43</v>
       </c>
       <c r="F119" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
     </row>
     <row r="120">
       <c r="B120" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="C120" t="s">
         <v>39</v>
@@ -5165,7 +5165,7 @@
     </row>
     <row r="121">
       <c r="B121" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="C121" t="s">
         <v>39</v>
@@ -5177,12 +5177,12 @@
         <v>43</v>
       </c>
       <c r="F121" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="122">
       <c r="B122" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="C122" t="s">
         <v>39</v>
@@ -5199,7 +5199,7 @@
     </row>
     <row r="123">
       <c r="B123" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="C123" t="s">
         <v>39</v>
@@ -5211,12 +5211,12 @@
         <v>43</v>
       </c>
       <c r="F123" t="s">
-        <v>496</v>
+        <v>338</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="C124" t="s">
         <v>39</v>
@@ -5228,12 +5228,12 @@
         <v>43</v>
       </c>
       <c r="F124" t="s">
-        <v>109</v>
+        <v>336</v>
       </c>
     </row>
     <row r="125">
       <c r="B125" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="C125" t="s">
         <v>39</v>
@@ -5245,12 +5245,12 @@
         <v>43</v>
       </c>
       <c r="F125" t="s">
-        <v>504</v>
+        <v>389</v>
       </c>
     </row>
     <row r="126">
       <c r="B126" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="C126" t="s">
         <v>39</v>
@@ -5262,12 +5262,12 @@
         <v>43</v>
       </c>
       <c r="F126" t="s">
-        <v>109</v>
+        <v>390</v>
       </c>
     </row>
     <row r="127">
       <c r="B127" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="C127" t="s">
         <v>39</v>
@@ -5279,12 +5279,12 @@
         <v>43</v>
       </c>
       <c r="F127" t="s">
-        <v>338</v>
+        <v>391</v>
       </c>
     </row>
     <row r="128">
       <c r="B128" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="C128" t="s">
         <v>39</v>
@@ -5296,12 +5296,12 @@
         <v>43</v>
       </c>
       <c r="F128" t="s">
-        <v>336</v>
+        <v>460</v>
       </c>
     </row>
     <row r="129">
       <c r="B129" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="C129" t="s">
         <v>39</v>
@@ -5313,12 +5313,12 @@
         <v>43</v>
       </c>
       <c r="F129" t="s">
-        <v>389</v>
+        <v>461</v>
       </c>
     </row>
     <row r="130">
       <c r="B130" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="C130" t="s">
         <v>39</v>
@@ -5330,12 +5330,12 @@
         <v>43</v>
       </c>
       <c r="F130" t="s">
-        <v>390</v>
+        <v>463</v>
       </c>
     </row>
     <row r="131">
       <c r="B131" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="C131" t="s">
         <v>39</v>
@@ -5347,12 +5347,12 @@
         <v>43</v>
       </c>
       <c r="F131" t="s">
-        <v>391</v>
+        <v>542</v>
       </c>
     </row>
     <row r="132">
       <c r="B132" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="C132" t="s">
         <v>39</v>
@@ -5364,12 +5364,12 @@
         <v>43</v>
       </c>
       <c r="F132" t="s">
-        <v>460</v>
+        <v>543</v>
       </c>
     </row>
     <row r="133">
       <c r="B133" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="C133" t="s">
         <v>39</v>
@@ -5381,12 +5381,12 @@
         <v>43</v>
       </c>
       <c r="F133" t="s">
-        <v>461</v>
+        <v>542</v>
       </c>
     </row>
     <row r="134">
       <c r="B134" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
       <c r="C134" t="s">
         <v>39</v>
@@ -5398,94 +5398,30 @@
         <v>43</v>
       </c>
       <c r="F134" t="s">
-        <v>463</v>
+        <v>543</v>
       </c>
     </row>
     <row r="135">
       <c r="B135" t="s">
-        <v>540</v>
+        <v>546</v>
       </c>
       <c r="C135" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D135" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E135" t="s">
         <v>43</v>
       </c>
       <c r="F135" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="B136" t="s">
-        <v>541</v>
-      </c>
-      <c r="C136" t="s">
-        <v>39</v>
-      </c>
-      <c r="D136" t="s">
-        <v>42</v>
-      </c>
-      <c r="E136" t="s">
-        <v>43</v>
-      </c>
-      <c r="F136" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="B137" t="s">
-        <v>544</v>
-      </c>
-      <c r="C137" t="s">
-        <v>39</v>
-      </c>
-      <c r="D137" t="s">
-        <v>42</v>
-      </c>
-      <c r="E137" t="s">
-        <v>43</v>
-      </c>
-      <c r="F137" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="B138" t="s">
-        <v>545</v>
-      </c>
-      <c r="C138" t="s">
-        <v>39</v>
-      </c>
-      <c r="D138" t="s">
-        <v>42</v>
-      </c>
-      <c r="E138" t="s">
-        <v>43</v>
-      </c>
-      <c r="F138" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="B139" t="s">
-        <v>546</v>
-      </c>
-      <c r="C139" t="s">
-        <v>37</v>
-      </c>
-      <c r="D139" t="s">
-        <v>55</v>
-      </c>
-      <c r="E139" t="s">
-        <v>43</v>
-      </c>
-      <c r="F139" t="s">
         <v>549</v>
       </c>
     </row>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
     <row r="140"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
removed unused red parameter dots in GUI
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150549" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151297" uniqueCount="558">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -5205,7 +5205,7 @@
     </row>
     <row r="123">
       <c r="B123" t="s">
-        <v>532</v>
+        <v>544</v>
       </c>
       <c r="C123" t="s">
         <v>39</v>
@@ -5217,12 +5217,12 @@
         <v>43</v>
       </c>
       <c r="F123" t="s">
-        <v>338</v>
+        <v>542</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" t="s">
-        <v>533</v>
+        <v>545</v>
       </c>
       <c r="C124" t="s">
         <v>39</v>
@@ -5234,196 +5234,36 @@
         <v>43</v>
       </c>
       <c r="F124" t="s">
-        <v>336</v>
+        <v>543</v>
       </c>
     </row>
     <row r="125">
       <c r="B125" t="s">
-        <v>534</v>
+        <v>546</v>
       </c>
       <c r="C125" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D125" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E125" t="s">
         <v>43</v>
       </c>
       <c r="F125" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="B126" t="s">
-        <v>535</v>
-      </c>
-      <c r="C126" t="s">
-        <v>39</v>
-      </c>
-      <c r="D126" t="s">
-        <v>42</v>
-      </c>
-      <c r="E126" t="s">
-        <v>43</v>
-      </c>
-      <c r="F126" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="B127" t="s">
-        <v>536</v>
-      </c>
-      <c r="C127" t="s">
-        <v>39</v>
-      </c>
-      <c r="D127" t="s">
-        <v>42</v>
-      </c>
-      <c r="E127" t="s">
-        <v>43</v>
-      </c>
-      <c r="F127" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="B128" t="s">
-        <v>537</v>
-      </c>
-      <c r="C128" t="s">
-        <v>39</v>
-      </c>
-      <c r="D128" t="s">
-        <v>42</v>
-      </c>
-      <c r="E128" t="s">
-        <v>43</v>
-      </c>
-      <c r="F128" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="B129" t="s">
-        <v>538</v>
-      </c>
-      <c r="C129" t="s">
-        <v>39</v>
-      </c>
-      <c r="D129" t="s">
-        <v>42</v>
-      </c>
-      <c r="E129" t="s">
-        <v>43</v>
-      </c>
-      <c r="F129" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="B130" t="s">
-        <v>539</v>
-      </c>
-      <c r="C130" t="s">
-        <v>39</v>
-      </c>
-      <c r="D130" t="s">
-        <v>42</v>
-      </c>
-      <c r="E130" t="s">
-        <v>43</v>
-      </c>
-      <c r="F130" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="B131" t="s">
-        <v>540</v>
-      </c>
-      <c r="C131" t="s">
-        <v>39</v>
-      </c>
-      <c r="D131" t="s">
-        <v>42</v>
-      </c>
-      <c r="E131" t="s">
-        <v>43</v>
-      </c>
-      <c r="F131" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="B132" t="s">
-        <v>541</v>
-      </c>
-      <c r="C132" t="s">
-        <v>39</v>
-      </c>
-      <c r="D132" t="s">
-        <v>42</v>
-      </c>
-      <c r="E132" t="s">
-        <v>43</v>
-      </c>
-      <c r="F132" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="B133" t="s">
-        <v>544</v>
-      </c>
-      <c r="C133" t="s">
-        <v>39</v>
-      </c>
-      <c r="D133" t="s">
-        <v>42</v>
-      </c>
-      <c r="E133" t="s">
-        <v>43</v>
-      </c>
-      <c r="F133" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="B134" t="s">
-        <v>545</v>
-      </c>
-      <c r="C134" t="s">
-        <v>39</v>
-      </c>
-      <c r="D134" t="s">
-        <v>42</v>
-      </c>
-      <c r="E134" t="s">
-        <v>43</v>
-      </c>
-      <c r="F134" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="B135" t="s">
-        <v>546</v>
-      </c>
-      <c r="C135" t="s">
-        <v>37</v>
-      </c>
-      <c r="D135" t="s">
-        <v>55</v>
-      </c>
-      <c r="E135" t="s">
-        <v>43</v>
-      </c>
-      <c r="F135" t="s">
         <v>549</v>
       </c>
     </row>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
     <row r="136"/>
     <row r="137"/>
     <row r="138"/>

</xml_diff>

<commit_message>
added support for connection initialization with sending device specification to STM32
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151297" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164393" uniqueCount="588">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1735,6 +1735,96 @@
   </si>
   <si>
     <t xml:space="preserve">Value to set:   &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor:      &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type:      &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model:          &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed:  &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version:             &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed:             &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor:       &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type:                  &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor:               &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model:                &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version:              &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed:                &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId267</t>
   </si>
 </sst>
 </file>
@@ -5254,21 +5344,261 @@
         <v>549</v>
       </c>
     </row>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
+    <row r="126">
+      <c r="B126" t="s">
+        <v>558</v>
+      </c>
+      <c r="C126" t="s">
+        <v>37</v>
+      </c>
+      <c r="D126" t="s">
+        <v>55</v>
+      </c>
+      <c r="E126" t="s">
+        <v>43</v>
+      </c>
+      <c r="F126" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" t="s">
+        <v>560</v>
+      </c>
+      <c r="C127" t="s">
+        <v>39</v>
+      </c>
+      <c r="D127" t="s">
+        <v>42</v>
+      </c>
+      <c r="E127" t="s">
+        <v>43</v>
+      </c>
+      <c r="F127" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128" t="s">
+        <v>561</v>
+      </c>
+      <c r="C128" t="s">
+        <v>39</v>
+      </c>
+      <c r="D128" t="s">
+        <v>42</v>
+      </c>
+      <c r="E128" t="s">
+        <v>43</v>
+      </c>
+      <c r="F128" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" t="s">
+        <v>562</v>
+      </c>
+      <c r="C129" t="s">
+        <v>39</v>
+      </c>
+      <c r="D129" t="s">
+        <v>42</v>
+      </c>
+      <c r="E129" t="s">
+        <v>43</v>
+      </c>
+      <c r="F129" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" t="s">
+        <v>563</v>
+      </c>
+      <c r="C130" t="s">
+        <v>39</v>
+      </c>
+      <c r="D130" t="s">
+        <v>42</v>
+      </c>
+      <c r="E130" t="s">
+        <v>43</v>
+      </c>
+      <c r="F130" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" t="s">
+        <v>564</v>
+      </c>
+      <c r="C131" t="s">
+        <v>39</v>
+      </c>
+      <c r="D131" t="s">
+        <v>42</v>
+      </c>
+      <c r="E131" t="s">
+        <v>43</v>
+      </c>
+      <c r="F131" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" t="s">
+        <v>565</v>
+      </c>
+      <c r="C132" t="s">
+        <v>39</v>
+      </c>
+      <c r="D132" t="s">
+        <v>42</v>
+      </c>
+      <c r="E132" t="s">
+        <v>43</v>
+      </c>
+      <c r="F132" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" t="s">
+        <v>566</v>
+      </c>
+      <c r="C133" t="s">
+        <v>39</v>
+      </c>
+      <c r="D133" t="s">
+        <v>42</v>
+      </c>
+      <c r="E133" t="s">
+        <v>43</v>
+      </c>
+      <c r="F133" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" t="s">
+        <v>567</v>
+      </c>
+      <c r="C134" t="s">
+        <v>39</v>
+      </c>
+      <c r="D134" t="s">
+        <v>42</v>
+      </c>
+      <c r="E134" t="s">
+        <v>43</v>
+      </c>
+      <c r="F134" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135" t="s">
+        <v>568</v>
+      </c>
+      <c r="C135" t="s">
+        <v>39</v>
+      </c>
+      <c r="D135" t="s">
+        <v>42</v>
+      </c>
+      <c r="E135" t="s">
+        <v>43</v>
+      </c>
+      <c r="F135" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" t="s">
+        <v>569</v>
+      </c>
+      <c r="C136" t="s">
+        <v>39</v>
+      </c>
+      <c r="D136" t="s">
+        <v>42</v>
+      </c>
+      <c r="E136" t="s">
+        <v>43</v>
+      </c>
+      <c r="F136" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137" t="s">
+        <v>572</v>
+      </c>
+      <c r="C137" t="s">
+        <v>39</v>
+      </c>
+      <c r="D137" t="s">
+        <v>42</v>
+      </c>
+      <c r="E137" t="s">
+        <v>43</v>
+      </c>
+      <c r="F137" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" t="s">
+        <v>585</v>
+      </c>
+      <c r="C138" t="s">
+        <v>37</v>
+      </c>
+      <c r="D138" t="s">
+        <v>42</v>
+      </c>
+      <c r="E138" t="s">
+        <v>43</v>
+      </c>
+      <c r="F138" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="B139" t="s">
+        <v>586</v>
+      </c>
+      <c r="C139" t="s">
+        <v>37</v>
+      </c>
+      <c r="D139" t="s">
+        <v>42</v>
+      </c>
+      <c r="E139" t="s">
+        <v>43</v>
+      </c>
+      <c r="F139" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="B140" t="s">
+        <v>587</v>
+      </c>
+      <c r="C140" t="s">
+        <v>37</v>
+      </c>
+      <c r="D140" t="s">
+        <v>55</v>
+      </c>
+      <c r="E140" t="s">
+        <v>43</v>
+      </c>
+      <c r="F140" t="s">
+        <v>392</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
added graph visible scale
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164393" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171217" uniqueCount="597">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1825,6 +1825,33 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdasdasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdasdasd&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -5599,6 +5626,74 @@
         <v>392</v>
       </c>
     </row>
+    <row r="141">
+      <c r="B141" t="s">
+        <v>588</v>
+      </c>
+      <c r="C141" t="s">
+        <v>37</v>
+      </c>
+      <c r="D141" t="s">
+        <v>42</v>
+      </c>
+      <c r="E141" t="s">
+        <v>43</v>
+      </c>
+      <c r="F141" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="B142" t="s">
+        <v>590</v>
+      </c>
+      <c r="C142" t="s">
+        <v>37</v>
+      </c>
+      <c r="D142" t="s">
+        <v>42</v>
+      </c>
+      <c r="E142" t="s">
+        <v>43</v>
+      </c>
+      <c r="F142" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="B143" t="s">
+        <v>592</v>
+      </c>
+      <c r="C143" t="s">
+        <v>37</v>
+      </c>
+      <c r="D143" t="s">
+        <v>42</v>
+      </c>
+      <c r="E143" t="s">
+        <v>43</v>
+      </c>
+      <c r="F143" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="B144" t="s">
+        <v>594</v>
+      </c>
+      <c r="C144" t="s">
+        <v>37</v>
+      </c>
+      <c r="D144" t="s">
+        <v>42</v>
+      </c>
+      <c r="E144" t="s">
+        <v>43</v>
+      </c>
+      <c r="F144" t="s">
+        <v>595</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
added automatic vertical range adjustment toggling option
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207124" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216954" uniqueCount="652">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2002,6 +2002,21 @@
   </si>
   <si>
     <t xml:space="preserve">Y-axis min:-&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Y range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Y range&lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -6013,7 +6028,7 @@
         <v>43</v>
       </c>
       <c r="F154" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
     </row>
     <row r="155">
@@ -6098,7 +6113,7 @@
         <v>43</v>
       </c>
       <c r="F159" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
     </row>
     <row r="160">
@@ -6167,6 +6182,23 @@
       </c>
       <c r="F163" t="s">
         <v>623</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="B164" t="s">
+        <v>647</v>
+      </c>
+      <c r="C164" t="s">
+        <v>37</v>
+      </c>
+      <c r="D164" t="s">
+        <v>42</v>
+      </c>
+      <c r="E164" t="s">
+        <v>43</v>
+      </c>
+      <c r="F164" t="s">
+        <v>650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-custom parameter names can be received from Qt GUI and displayed in Module Data Screen and Graph Signals Screen
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217937" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242698" uniqueCount="697">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2017,6 +2017,141 @@
   </si>
   <si>
     <t xml:space="preserve">Auto Y range&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P&lt;value&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non&lt;value&gt;A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Par1 &lt;value&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None &lt;value&gt;A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None &lt;value&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None &lt;value&gt;Hz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None              &lt;value&gt;W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None             &lt;value&gt;A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None              &lt;value&gt;Hz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None              &lt;value&gt;A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None              &lt;value&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None              &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId313</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId317</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId327</t>
   </si>
 </sst>
 </file>
@@ -3636,7 +3771,7 @@
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C14" t="s">
         <v>39</v>
@@ -3648,49 +3783,49 @@
         <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>553</v>
+        <v>596</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>300</v>
+        <v>357</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
         <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>109</v>
+        <v>375</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>301</v>
+        <v>360</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>554</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>302</v>
+        <v>361</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
         <v>42</v>
@@ -3699,15 +3834,15 @@
         <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>303</v>
+        <v>362</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
@@ -3716,12 +3851,12 @@
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>552</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>304</v>
+        <v>365</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -3733,29 +3868,29 @@
         <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>109</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
         <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>360</v>
+        <v>376</v>
       </c>
       <c r="C21" t="s">
         <v>37</v>
@@ -3767,15 +3902,15 @@
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>75</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>361</v>
+        <v>377</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
@@ -3784,15 +3919,15 @@
         <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>223</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>362</v>
+        <v>378</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
         <v>42</v>
@@ -3801,12 +3936,12 @@
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>109</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="C24" t="s">
         <v>39</v>
@@ -3818,12 +3953,12 @@
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="C25" t="s">
         <v>39</v>
@@ -3835,29 +3970,29 @@
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>370</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E26" t="s">
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>340</v>
+        <v>385</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
@@ -3869,12 +4004,12 @@
         <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>338</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
@@ -3886,12 +4021,12 @@
         <v>43</v>
       </c>
       <c r="F28" t="s">
-        <v>336</v>
+        <v>389</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
@@ -3903,49 +4038,49 @@
         <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>347</v>
+        <v>390</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E30" t="s">
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>109</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>381</v>
+        <v>399</v>
       </c>
       <c r="C31" t="s">
         <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
         <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>385</v>
+        <v>400</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>382</v>
+        <v>401</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
         <v>42</v>
@@ -3954,15 +4089,15 @@
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>383</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>386</v>
+        <v>402</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
@@ -3971,15 +4106,15 @@
         <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>389</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>387</v>
+        <v>403</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
@@ -3988,46 +4123,46 @@
         <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>390</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>388</v>
+        <v>404</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E35" t="s">
         <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>392</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="C36" t="s">
         <v>37</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E36" t="s">
         <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>400</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="C37" t="s">
         <v>37</v>
@@ -4039,29 +4174,29 @@
         <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C38" t="s">
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E38" t="s">
         <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="C39" t="s">
         <v>37</v>
@@ -4078,7 +4213,7 @@
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="C40" t="s">
         <v>37</v>
@@ -4095,10 +4230,10 @@
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D41" t="s">
         <v>42</v>
@@ -4107,15 +4242,15 @@
         <v>43</v>
       </c>
       <c r="F41" t="s">
-        <v>223</v>
+        <v>396</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
         <v>42</v>
@@ -4129,27 +4264,27 @@
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D43" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E43" t="s">
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>75</v>
+        <v>398</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="C44" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D44" t="s">
         <v>42</v>
@@ -4158,15 +4293,15 @@
         <v>43</v>
       </c>
       <c r="F44" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D45" t="s">
         <v>42</v>
@@ -4175,12 +4310,12 @@
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="C46" t="s">
         <v>39</v>
@@ -4192,12 +4327,12 @@
         <v>43</v>
       </c>
       <c r="F46" t="s">
-        <v>396</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="C47" t="s">
         <v>39</v>
@@ -4209,12 +4344,12 @@
         <v>43</v>
       </c>
       <c r="F47" t="s">
-        <v>109</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="C48" t="s">
         <v>39</v>
@@ -4226,12 +4361,12 @@
         <v>43</v>
       </c>
       <c r="F48" t="s">
-        <v>398</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="C49" t="s">
         <v>39</v>
@@ -4243,80 +4378,80 @@
         <v>43</v>
       </c>
       <c r="F49" t="s">
-        <v>109</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D50" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E50" t="s">
         <v>43</v>
       </c>
       <c r="F50" t="s">
-        <v>263</v>
+        <v>400</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="C51" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D51" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E51" t="s">
         <v>43</v>
       </c>
       <c r="F51" t="s">
-        <v>109</v>
+        <v>359</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D52" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E52" t="s">
         <v>43</v>
       </c>
       <c r="F52" t="s">
-        <v>262</v>
+        <v>359</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="C53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D53" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E53" t="s">
         <v>43</v>
       </c>
       <c r="F53" t="s">
-        <v>109</v>
+        <v>340</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
@@ -4328,80 +4463,80 @@
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>225</v>
+        <v>338</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="C55" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E55" t="s">
         <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>400</v>
+        <v>336</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E56" t="s">
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="C57" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D57" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E57" t="s">
         <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>359</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="C58" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D58" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E58" t="s">
         <v>43</v>
       </c>
       <c r="F58" t="s">
-        <v>340</v>
+        <v>385</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="C59" t="s">
         <v>39</v>
@@ -4413,12 +4548,12 @@
         <v>43</v>
       </c>
       <c r="F59" t="s">
-        <v>338</v>
+        <v>442</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="C60" t="s">
         <v>39</v>
@@ -4430,12 +4565,12 @@
         <v>43</v>
       </c>
       <c r="F60" t="s">
-        <v>336</v>
+        <v>389</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="C61" t="s">
         <v>39</v>
@@ -4447,32 +4582,32 @@
         <v>43</v>
       </c>
       <c r="F61" t="s">
-        <v>347</v>
+        <v>390</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="C62" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D62" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E62" t="s">
         <v>43</v>
       </c>
       <c r="F62" t="s">
-        <v>109</v>
+        <v>392</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="C63" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D63" t="s">
         <v>42</v>
@@ -4481,15 +4616,15 @@
         <v>43</v>
       </c>
       <c r="F63" t="s">
-        <v>385</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="C64" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D64" t="s">
         <v>42</v>
@@ -4498,66 +4633,66 @@
         <v>43</v>
       </c>
       <c r="F64" t="s">
-        <v>442</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="C65" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D65" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E65" t="s">
         <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="C66" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D66" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E66" t="s">
         <v>43</v>
       </c>
       <c r="F66" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="C67" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D67" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E67" t="s">
         <v>43</v>
       </c>
       <c r="F67" t="s">
-        <v>392</v>
+        <v>450</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="C68" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D68" t="s">
         <v>42</v>
@@ -4566,15 +4701,15 @@
         <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="C69" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D69" t="s">
         <v>42</v>
@@ -4583,46 +4718,46 @@
         <v>43</v>
       </c>
       <c r="F69" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
       <c r="C70" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D70" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E70" t="s">
         <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>392</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="C71" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D71" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E71" t="s">
         <v>43</v>
       </c>
       <c r="F71" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>443</v>
+        <v>458</v>
       </c>
       <c r="C72" t="s">
         <v>39</v>
@@ -4634,12 +4769,12 @@
         <v>43</v>
       </c>
       <c r="F72" t="s">
-        <v>450</v>
+        <v>460</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>444</v>
+        <v>459</v>
       </c>
       <c r="C73" t="s">
         <v>39</v>
@@ -4651,12 +4786,12 @@
         <v>43</v>
       </c>
       <c r="F73" t="s">
-        <v>109</v>
+        <v>461</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>446</v>
+        <v>462</v>
       </c>
       <c r="C74" t="s">
         <v>39</v>
@@ -4668,49 +4803,49 @@
         <v>43</v>
       </c>
       <c r="F74" t="s">
-        <v>452</v>
+        <v>463</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>447</v>
+        <v>467</v>
       </c>
       <c r="C75" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D75" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E75" t="s">
         <v>43</v>
       </c>
       <c r="F75" t="s">
-        <v>109</v>
+        <v>548</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>453</v>
+        <v>469</v>
       </c>
       <c r="C76" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D76" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E76" t="s">
         <v>43</v>
       </c>
       <c r="F76" t="s">
-        <v>555</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>454</v>
+        <v>470</v>
       </c>
       <c r="C77" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D77" t="s">
         <v>42</v>
@@ -4719,15 +4854,15 @@
         <v>43</v>
       </c>
       <c r="F77" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="C78" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D78" t="s">
         <v>42</v>
@@ -4736,12 +4871,12 @@
         <v>43</v>
       </c>
       <c r="F78" t="s">
-        <v>391</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="C79" t="s">
         <v>39</v>
@@ -4753,12 +4888,12 @@
         <v>43</v>
       </c>
       <c r="F79" t="s">
-        <v>460</v>
+        <v>396</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>459</v>
+        <v>473</v>
       </c>
       <c r="C80" t="s">
         <v>39</v>
@@ -4770,12 +4905,12 @@
         <v>43</v>
       </c>
       <c r="F80" t="s">
-        <v>461</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="C81" t="s">
         <v>39</v>
@@ -4787,49 +4922,49 @@
         <v>43</v>
       </c>
       <c r="F81" t="s">
-        <v>463</v>
+        <v>398</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="C82" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D82" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E82" t="s">
         <v>43</v>
       </c>
       <c r="F82" t="s">
-        <v>548</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="C83" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D83" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E83" t="s">
         <v>43</v>
       </c>
       <c r="F83" t="s">
-        <v>75</v>
+        <v>263</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="C84" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D84" t="s">
         <v>42</v>
@@ -4838,15 +4973,15 @@
         <v>43</v>
       </c>
       <c r="F84" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="C85" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D85" t="s">
         <v>42</v>
@@ -4855,12 +4990,12 @@
         <v>43</v>
       </c>
       <c r="F85" t="s">
-        <v>109</v>
+        <v>262</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="C86" t="s">
         <v>39</v>
@@ -4872,12 +5007,12 @@
         <v>43</v>
       </c>
       <c r="F86" t="s">
-        <v>396</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="C87" t="s">
         <v>39</v>
@@ -4889,12 +5024,12 @@
         <v>43</v>
       </c>
       <c r="F87" t="s">
-        <v>109</v>
+        <v>488</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="C88" t="s">
         <v>39</v>
@@ -4906,12 +5041,12 @@
         <v>43</v>
       </c>
       <c r="F88" t="s">
-        <v>398</v>
+        <v>450</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C89" t="s">
         <v>39</v>
@@ -4928,7 +5063,7 @@
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="C90" t="s">
         <v>39</v>
@@ -4940,12 +5075,12 @@
         <v>43</v>
       </c>
       <c r="F90" t="s">
-        <v>263</v>
+        <v>452</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C91" t="s">
         <v>39</v>
@@ -4962,7 +5097,7 @@
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>478</v>
+        <v>508</v>
       </c>
       <c r="C92" t="s">
         <v>39</v>
@@ -4974,12 +5109,12 @@
         <v>43</v>
       </c>
       <c r="F92" t="s">
-        <v>262</v>
+        <v>506</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>479</v>
+        <v>509</v>
       </c>
       <c r="C93" t="s">
         <v>39</v>
@@ -4996,7 +5131,7 @@
     </row>
     <row r="94">
       <c r="B94" t="s">
-        <v>480</v>
+        <v>510</v>
       </c>
       <c r="C94" t="s">
         <v>39</v>
@@ -5008,12 +5143,12 @@
         <v>43</v>
       </c>
       <c r="F94" t="s">
-        <v>488</v>
+        <v>507</v>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="s">
-        <v>484</v>
+        <v>511</v>
       </c>
       <c r="C95" t="s">
         <v>39</v>
@@ -5025,12 +5160,12 @@
         <v>43</v>
       </c>
       <c r="F95" t="s">
-        <v>450</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="s">
-        <v>485</v>
+        <v>512</v>
       </c>
       <c r="C96" t="s">
         <v>39</v>
@@ -5042,12 +5177,12 @@
         <v>43</v>
       </c>
       <c r="F96" t="s">
-        <v>109</v>
+        <v>503</v>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="s">
-        <v>486</v>
+        <v>513</v>
       </c>
       <c r="C97" t="s">
         <v>39</v>
@@ -5059,12 +5194,12 @@
         <v>43</v>
       </c>
       <c r="F97" t="s">
-        <v>452</v>
+        <v>109</v>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="s">
-        <v>487</v>
+        <v>514</v>
       </c>
       <c r="C98" t="s">
         <v>39</v>
@@ -5076,12 +5211,12 @@
         <v>43</v>
       </c>
       <c r="F98" t="s">
-        <v>109</v>
+        <v>505</v>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="C99" t="s">
         <v>39</v>
@@ -5093,12 +5228,12 @@
         <v>43</v>
       </c>
       <c r="F99" t="s">
-        <v>506</v>
+        <v>109</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="C100" t="s">
         <v>39</v>
@@ -5110,12 +5245,12 @@
         <v>43</v>
       </c>
       <c r="F100" t="s">
-        <v>109</v>
+        <v>496</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="C101" t="s">
         <v>39</v>
@@ -5127,12 +5262,12 @@
         <v>43</v>
       </c>
       <c r="F101" t="s">
-        <v>507</v>
+        <v>109</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="C102" t="s">
         <v>39</v>
@@ -5144,12 +5279,12 @@
         <v>43</v>
       </c>
       <c r="F102" t="s">
-        <v>109</v>
+        <v>504</v>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="C103" t="s">
         <v>39</v>
@@ -5161,12 +5296,12 @@
         <v>43</v>
       </c>
       <c r="F103" t="s">
-        <v>503</v>
+        <v>109</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="C104" t="s">
         <v>39</v>
@@ -5178,12 +5313,12 @@
         <v>43</v>
       </c>
       <c r="F104" t="s">
-        <v>109</v>
+        <v>506</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="C105" t="s">
         <v>39</v>
@@ -5195,12 +5330,12 @@
         <v>43</v>
       </c>
       <c r="F105" t="s">
-        <v>505</v>
+        <v>109</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="C106" t="s">
         <v>39</v>
@@ -5212,12 +5347,12 @@
         <v>43</v>
       </c>
       <c r="F106" t="s">
-        <v>109</v>
+        <v>507</v>
       </c>
     </row>
     <row r="107">
       <c r="B107" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="C107" t="s">
         <v>39</v>
@@ -5229,12 +5364,12 @@
         <v>43</v>
       </c>
       <c r="F107" t="s">
-        <v>496</v>
+        <v>109</v>
       </c>
     </row>
     <row r="108">
       <c r="B108" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="C108" t="s">
         <v>39</v>
@@ -5246,12 +5381,12 @@
         <v>43</v>
       </c>
       <c r="F108" t="s">
-        <v>109</v>
+        <v>503</v>
       </c>
     </row>
     <row r="109">
       <c r="B109" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="C109" t="s">
         <v>39</v>
@@ -5263,12 +5398,12 @@
         <v>43</v>
       </c>
       <c r="F109" t="s">
-        <v>504</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110">
       <c r="B110" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="C110" t="s">
         <v>39</v>
@@ -5280,12 +5415,12 @@
         <v>43</v>
       </c>
       <c r="F110" t="s">
-        <v>109</v>
+        <v>505</v>
       </c>
     </row>
     <row r="111">
       <c r="B111" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="C111" t="s">
         <v>39</v>
@@ -5297,12 +5432,12 @@
         <v>43</v>
       </c>
       <c r="F111" t="s">
-        <v>506</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112">
       <c r="B112" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="C112" t="s">
         <v>39</v>
@@ -5314,12 +5449,12 @@
         <v>43</v>
       </c>
       <c r="F112" t="s">
-        <v>109</v>
+        <v>496</v>
       </c>
     </row>
     <row r="113">
       <c r="B113" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="C113" t="s">
         <v>39</v>
@@ -5331,12 +5466,12 @@
         <v>43</v>
       </c>
       <c r="F113" t="s">
-        <v>507</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114">
       <c r="B114" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="C114" t="s">
         <v>39</v>
@@ -5348,12 +5483,12 @@
         <v>43</v>
       </c>
       <c r="F114" t="s">
-        <v>109</v>
+        <v>504</v>
       </c>
     </row>
     <row r="115">
       <c r="B115" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="C115" t="s">
         <v>39</v>
@@ -5365,12 +5500,12 @@
         <v>43</v>
       </c>
       <c r="F115" t="s">
-        <v>503</v>
+        <v>109</v>
       </c>
     </row>
     <row r="116">
       <c r="B116" t="s">
-        <v>525</v>
+        <v>544</v>
       </c>
       <c r="C116" t="s">
         <v>39</v>
@@ -5382,12 +5517,12 @@
         <v>43</v>
       </c>
       <c r="F116" t="s">
-        <v>109</v>
+        <v>542</v>
       </c>
     </row>
     <row r="117">
       <c r="B117" t="s">
-        <v>526</v>
+        <v>545</v>
       </c>
       <c r="C117" t="s">
         <v>39</v>
@@ -5399,46 +5534,46 @@
         <v>43</v>
       </c>
       <c r="F117" t="s">
-        <v>505</v>
+        <v>543</v>
       </c>
     </row>
     <row r="118">
       <c r="B118" t="s">
-        <v>527</v>
+        <v>546</v>
       </c>
       <c r="C118" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D118" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E118" t="s">
         <v>43</v>
       </c>
       <c r="F118" t="s">
-        <v>109</v>
+        <v>549</v>
       </c>
     </row>
     <row r="119">
       <c r="B119" t="s">
-        <v>528</v>
+        <v>558</v>
       </c>
       <c r="C119" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D119" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E119" t="s">
         <v>43</v>
       </c>
       <c r="F119" t="s">
-        <v>496</v>
+        <v>559</v>
       </c>
     </row>
     <row r="120">
       <c r="B120" t="s">
-        <v>529</v>
+        <v>560</v>
       </c>
       <c r="C120" t="s">
         <v>39</v>
@@ -5450,12 +5585,12 @@
         <v>43</v>
       </c>
       <c r="F120" t="s">
-        <v>109</v>
+        <v>583</v>
       </c>
     </row>
     <row r="121">
       <c r="B121" t="s">
-        <v>530</v>
+        <v>562</v>
       </c>
       <c r="C121" t="s">
         <v>39</v>
@@ -5467,12 +5602,12 @@
         <v>43</v>
       </c>
       <c r="F121" t="s">
-        <v>504</v>
+        <v>584</v>
       </c>
     </row>
     <row r="122">
       <c r="B122" t="s">
-        <v>531</v>
+        <v>564</v>
       </c>
       <c r="C122" t="s">
         <v>39</v>
@@ -5484,12 +5619,12 @@
         <v>43</v>
       </c>
       <c r="F122" t="s">
-        <v>109</v>
+        <v>580</v>
       </c>
     </row>
     <row r="123">
       <c r="B123" t="s">
-        <v>544</v>
+        <v>566</v>
       </c>
       <c r="C123" t="s">
         <v>39</v>
@@ -5501,12 +5636,12 @@
         <v>43</v>
       </c>
       <c r="F123" t="s">
-        <v>542</v>
+        <v>581</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" t="s">
-        <v>545</v>
+        <v>567</v>
       </c>
       <c r="C124" t="s">
         <v>39</v>
@@ -5518,35 +5653,35 @@
         <v>43</v>
       </c>
       <c r="F124" t="s">
-        <v>543</v>
+        <v>370</v>
       </c>
     </row>
     <row r="125">
       <c r="B125" t="s">
-        <v>546</v>
+        <v>568</v>
       </c>
       <c r="C125" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D125" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E125" t="s">
         <v>43</v>
       </c>
       <c r="F125" t="s">
-        <v>549</v>
+        <v>582</v>
       </c>
     </row>
     <row r="126">
       <c r="B126" t="s">
-        <v>558</v>
+        <v>572</v>
       </c>
       <c r="C126" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D126" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E126" t="s">
         <v>43</v>
@@ -5557,10 +5692,10 @@
     </row>
     <row r="127">
       <c r="B127" t="s">
-        <v>560</v>
+        <v>585</v>
       </c>
       <c r="C127" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D127" t="s">
         <v>42</v>
@@ -5569,15 +5704,15 @@
         <v>43</v>
       </c>
       <c r="F127" t="s">
-        <v>583</v>
+        <v>223</v>
       </c>
     </row>
     <row r="128">
       <c r="B128" t="s">
-        <v>561</v>
+        <v>586</v>
       </c>
       <c r="C128" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D128" t="s">
         <v>42</v>
@@ -5591,27 +5726,27 @@
     </row>
     <row r="129">
       <c r="B129" t="s">
-        <v>562</v>
+        <v>587</v>
       </c>
       <c r="C129" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D129" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E129" t="s">
         <v>43</v>
       </c>
       <c r="F129" t="s">
-        <v>584</v>
+        <v>392</v>
       </c>
     </row>
     <row r="130">
       <c r="B130" t="s">
-        <v>563</v>
+        <v>588</v>
       </c>
       <c r="C130" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D130" t="s">
         <v>42</v>
@@ -5620,15 +5755,15 @@
         <v>43</v>
       </c>
       <c r="F130" t="s">
-        <v>109</v>
+        <v>596</v>
       </c>
     </row>
     <row r="131">
       <c r="B131" t="s">
-        <v>564</v>
+        <v>590</v>
       </c>
       <c r="C131" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D131" t="s">
         <v>42</v>
@@ -5637,15 +5772,15 @@
         <v>43</v>
       </c>
       <c r="F131" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
     </row>
     <row r="132">
       <c r="B132" t="s">
-        <v>565</v>
+        <v>592</v>
       </c>
       <c r="C132" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D132" t="s">
         <v>42</v>
@@ -5654,15 +5789,15 @@
         <v>43</v>
       </c>
       <c r="F132" t="s">
-        <v>109</v>
+        <v>593</v>
       </c>
     </row>
     <row r="133">
       <c r="B133" t="s">
-        <v>566</v>
+        <v>594</v>
       </c>
       <c r="C133" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D133" t="s">
         <v>42</v>
@@ -5671,15 +5806,15 @@
         <v>43</v>
       </c>
       <c r="F133" t="s">
-        <v>581</v>
+        <v>595</v>
       </c>
     </row>
     <row r="134">
       <c r="B134" t="s">
-        <v>567</v>
+        <v>597</v>
       </c>
       <c r="C134" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D134" t="s">
         <v>42</v>
@@ -5688,15 +5823,15 @@
         <v>43</v>
       </c>
       <c r="F134" t="s">
-        <v>109</v>
+        <v>596</v>
       </c>
     </row>
     <row r="135">
       <c r="B135" t="s">
-        <v>568</v>
+        <v>598</v>
       </c>
       <c r="C135" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D135" t="s">
         <v>42</v>
@@ -5705,15 +5840,15 @@
         <v>43</v>
       </c>
       <c r="F135" t="s">
-        <v>582</v>
+        <v>109</v>
       </c>
     </row>
     <row r="136">
       <c r="B136" t="s">
-        <v>569</v>
+        <v>599</v>
       </c>
       <c r="C136" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D136" t="s">
         <v>42</v>
@@ -5722,15 +5857,15 @@
         <v>43</v>
       </c>
       <c r="F136" t="s">
-        <v>109</v>
+        <v>596</v>
       </c>
     </row>
     <row r="137">
       <c r="B137" t="s">
-        <v>572</v>
+        <v>600</v>
       </c>
       <c r="C137" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D137" t="s">
         <v>42</v>
@@ -5739,32 +5874,32 @@
         <v>43</v>
       </c>
       <c r="F137" t="s">
-        <v>559</v>
+        <v>623</v>
       </c>
     </row>
     <row r="138">
       <c r="B138" t="s">
-        <v>585</v>
+        <v>602</v>
       </c>
       <c r="C138" t="s">
         <v>37</v>
       </c>
       <c r="D138" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E138" t="s">
         <v>43</v>
       </c>
       <c r="F138" t="s">
-        <v>223</v>
+        <v>603</v>
       </c>
     </row>
     <row r="139">
       <c r="B139" t="s">
-        <v>586</v>
+        <v>612</v>
       </c>
       <c r="C139" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D139" t="s">
         <v>42</v>
@@ -5773,32 +5908,32 @@
         <v>43</v>
       </c>
       <c r="F139" t="s">
-        <v>109</v>
+        <v>603</v>
       </c>
     </row>
     <row r="140">
       <c r="B140" t="s">
-        <v>587</v>
+        <v>619</v>
       </c>
       <c r="C140" t="s">
         <v>37</v>
       </c>
       <c r="D140" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E140" t="s">
         <v>43</v>
       </c>
       <c r="F140" t="s">
-        <v>392</v>
+        <v>223</v>
       </c>
     </row>
     <row r="141">
       <c r="B141" t="s">
-        <v>588</v>
+        <v>620</v>
       </c>
       <c r="C141" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D141" t="s">
         <v>42</v>
@@ -5807,32 +5942,32 @@
         <v>43</v>
       </c>
       <c r="F141" t="s">
-        <v>596</v>
+        <v>109</v>
       </c>
     </row>
     <row r="142">
       <c r="B142" t="s">
-        <v>590</v>
+        <v>621</v>
       </c>
       <c r="C142" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D142" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E142" t="s">
         <v>43</v>
       </c>
       <c r="F142" t="s">
-        <v>596</v>
+        <v>392</v>
       </c>
     </row>
     <row r="143">
       <c r="B143" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
       <c r="C143" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D143" t="s">
         <v>42</v>
@@ -5841,15 +5976,15 @@
         <v>43</v>
       </c>
       <c r="F143" t="s">
-        <v>593</v>
+        <v>644</v>
       </c>
     </row>
     <row r="144">
       <c r="B144" t="s">
-        <v>594</v>
+        <v>625</v>
       </c>
       <c r="C144" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D144" t="s">
         <v>42</v>
@@ -5858,15 +5993,15 @@
         <v>43</v>
       </c>
       <c r="F144" t="s">
-        <v>595</v>
+        <v>642</v>
       </c>
     </row>
     <row r="145">
       <c r="B145" t="s">
-        <v>597</v>
+        <v>631</v>
       </c>
       <c r="C145" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D145" t="s">
         <v>42</v>
@@ -5875,15 +6010,15 @@
         <v>43</v>
       </c>
       <c r="F145" t="s">
-        <v>596</v>
+        <v>639</v>
       </c>
     </row>
     <row r="146">
       <c r="B146" t="s">
-        <v>598</v>
+        <v>640</v>
       </c>
       <c r="C146" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D146" t="s">
         <v>42</v>
@@ -5892,15 +6027,15 @@
         <v>43</v>
       </c>
       <c r="F146" t="s">
-        <v>109</v>
+        <v>641</v>
       </c>
     </row>
     <row r="147">
       <c r="B147" t="s">
-        <v>599</v>
+        <v>643</v>
       </c>
       <c r="C147" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D147" t="s">
         <v>42</v>
@@ -5909,15 +6044,15 @@
         <v>43</v>
       </c>
       <c r="F147" t="s">
-        <v>596</v>
+        <v>336</v>
       </c>
     </row>
     <row r="148">
       <c r="B148" t="s">
-        <v>600</v>
+        <v>645</v>
       </c>
       <c r="C148" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D148" t="s">
         <v>42</v>
@@ -5931,24 +6066,24 @@
     </row>
     <row r="149">
       <c r="B149" t="s">
-        <v>602</v>
+        <v>647</v>
       </c>
       <c r="C149" t="s">
         <v>37</v>
       </c>
       <c r="D149" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E149" t="s">
         <v>43</v>
       </c>
       <c r="F149" t="s">
-        <v>603</v>
+        <v>650</v>
       </c>
     </row>
     <row r="150">
       <c r="B150" t="s">
-        <v>604</v>
+        <v>652</v>
       </c>
       <c r="C150" t="s">
         <v>39</v>
@@ -5960,12 +6095,12 @@
         <v>43</v>
       </c>
       <c r="F150" t="s">
-        <v>615</v>
+        <v>370</v>
       </c>
     </row>
     <row r="151">
       <c r="B151" t="s">
-        <v>606</v>
+        <v>653</v>
       </c>
       <c r="C151" t="s">
         <v>39</v>
@@ -5977,12 +6112,12 @@
         <v>43</v>
       </c>
       <c r="F151" t="s">
-        <v>616</v>
+        <v>370</v>
       </c>
     </row>
     <row r="152">
       <c r="B152" t="s">
-        <v>608</v>
+        <v>654</v>
       </c>
       <c r="C152" t="s">
         <v>39</v>
@@ -5994,12 +6129,12 @@
         <v>43</v>
       </c>
       <c r="F152" t="s">
-        <v>617</v>
+        <v>370</v>
       </c>
     </row>
     <row r="153">
       <c r="B153" t="s">
-        <v>610</v>
+        <v>655</v>
       </c>
       <c r="C153" t="s">
         <v>39</v>
@@ -6011,12 +6146,12 @@
         <v>43</v>
       </c>
       <c r="F153" t="s">
-        <v>618</v>
+        <v>370</v>
       </c>
     </row>
     <row r="154">
       <c r="B154" t="s">
-        <v>612</v>
+        <v>674</v>
       </c>
       <c r="C154" t="s">
         <v>39</v>
@@ -6028,15 +6163,15 @@
         <v>43</v>
       </c>
       <c r="F154" t="s">
-        <v>603</v>
+        <v>370</v>
       </c>
     </row>
     <row r="155">
       <c r="B155" t="s">
-        <v>619</v>
+        <v>675</v>
       </c>
       <c r="C155" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D155" t="s">
         <v>42</v>
@@ -6045,15 +6180,15 @@
         <v>43</v>
       </c>
       <c r="F155" t="s">
-        <v>223</v>
+        <v>596</v>
       </c>
     </row>
     <row r="156">
       <c r="B156" t="s">
-        <v>620</v>
+        <v>676</v>
       </c>
       <c r="C156" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D156" t="s">
         <v>42</v>
@@ -6062,29 +6197,29 @@
         <v>43</v>
       </c>
       <c r="F156" t="s">
-        <v>109</v>
+        <v>370</v>
       </c>
     </row>
     <row r="157">
       <c r="B157" t="s">
-        <v>621</v>
+        <v>677</v>
       </c>
       <c r="C157" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D157" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E157" t="s">
         <v>43</v>
       </c>
       <c r="F157" t="s">
-        <v>392</v>
+        <v>596</v>
       </c>
     </row>
     <row r="158">
       <c r="B158" t="s">
-        <v>624</v>
+        <v>678</v>
       </c>
       <c r="C158" t="s">
         <v>39</v>
@@ -6096,12 +6231,12 @@
         <v>43</v>
       </c>
       <c r="F158" t="s">
-        <v>644</v>
+        <v>370</v>
       </c>
     </row>
     <row r="159">
       <c r="B159" t="s">
-        <v>625</v>
+        <v>679</v>
       </c>
       <c r="C159" t="s">
         <v>39</v>
@@ -6113,12 +6248,12 @@
         <v>43</v>
       </c>
       <c r="F159" t="s">
-        <v>642</v>
+        <v>596</v>
       </c>
     </row>
     <row r="160">
       <c r="B160" t="s">
-        <v>631</v>
+        <v>680</v>
       </c>
       <c r="C160" t="s">
         <v>39</v>
@@ -6130,12 +6265,12 @@
         <v>43</v>
       </c>
       <c r="F160" t="s">
-        <v>639</v>
+        <v>370</v>
       </c>
     </row>
     <row r="161">
       <c r="B161" t="s">
-        <v>640</v>
+        <v>681</v>
       </c>
       <c r="C161" t="s">
         <v>39</v>
@@ -6147,12 +6282,12 @@
         <v>43</v>
       </c>
       <c r="F161" t="s">
-        <v>641</v>
+        <v>596</v>
       </c>
     </row>
     <row r="162">
       <c r="B162" t="s">
-        <v>643</v>
+        <v>682</v>
       </c>
       <c r="C162" t="s">
         <v>39</v>
@@ -6164,12 +6299,12 @@
         <v>43</v>
       </c>
       <c r="F162" t="s">
-        <v>336</v>
+        <v>370</v>
       </c>
     </row>
     <row r="163">
       <c r="B163" t="s">
-        <v>645</v>
+        <v>683</v>
       </c>
       <c r="C163" t="s">
         <v>39</v>
@@ -6181,15 +6316,15 @@
         <v>43</v>
       </c>
       <c r="F163" t="s">
-        <v>623</v>
+        <v>596</v>
       </c>
     </row>
     <row r="164">
       <c r="B164" t="s">
-        <v>647</v>
+        <v>684</v>
       </c>
       <c r="C164" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D164" t="s">
         <v>42</v>
@@ -6198,7 +6333,211 @@
         <v>43</v>
       </c>
       <c r="F164" t="s">
-        <v>650</v>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="B165" t="s">
+        <v>685</v>
+      </c>
+      <c r="C165" t="s">
+        <v>39</v>
+      </c>
+      <c r="D165" t="s">
+        <v>42</v>
+      </c>
+      <c r="E165" t="s">
+        <v>43</v>
+      </c>
+      <c r="F165" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="B166" t="s">
+        <v>686</v>
+      </c>
+      <c r="C166" t="s">
+        <v>39</v>
+      </c>
+      <c r="D166" t="s">
+        <v>42</v>
+      </c>
+      <c r="E166" t="s">
+        <v>43</v>
+      </c>
+      <c r="F166" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" t="s">
+        <v>687</v>
+      </c>
+      <c r="C167" t="s">
+        <v>39</v>
+      </c>
+      <c r="D167" t="s">
+        <v>42</v>
+      </c>
+      <c r="E167" t="s">
+        <v>43</v>
+      </c>
+      <c r="F167" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="B168" t="s">
+        <v>688</v>
+      </c>
+      <c r="C168" t="s">
+        <v>39</v>
+      </c>
+      <c r="D168" t="s">
+        <v>42</v>
+      </c>
+      <c r="E168" t="s">
+        <v>43</v>
+      </c>
+      <c r="F168" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="B169" t="s">
+        <v>689</v>
+      </c>
+      <c r="C169" t="s">
+        <v>39</v>
+      </c>
+      <c r="D169" t="s">
+        <v>42</v>
+      </c>
+      <c r="E169" t="s">
+        <v>43</v>
+      </c>
+      <c r="F169" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="B170" t="s">
+        <v>690</v>
+      </c>
+      <c r="C170" t="s">
+        <v>39</v>
+      </c>
+      <c r="D170" t="s">
+        <v>42</v>
+      </c>
+      <c r="E170" t="s">
+        <v>43</v>
+      </c>
+      <c r="F170" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="B171" t="s">
+        <v>691</v>
+      </c>
+      <c r="C171" t="s">
+        <v>39</v>
+      </c>
+      <c r="D171" t="s">
+        <v>42</v>
+      </c>
+      <c r="E171" t="s">
+        <v>43</v>
+      </c>
+      <c r="F171" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="B172" t="s">
+        <v>692</v>
+      </c>
+      <c r="C172" t="s">
+        <v>39</v>
+      </c>
+      <c r="D172" t="s">
+        <v>42</v>
+      </c>
+      <c r="E172" t="s">
+        <v>43</v>
+      </c>
+      <c r="F172" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="B173" t="s">
+        <v>693</v>
+      </c>
+      <c r="C173" t="s">
+        <v>39</v>
+      </c>
+      <c r="D173" t="s">
+        <v>42</v>
+      </c>
+      <c r="E173" t="s">
+        <v>43</v>
+      </c>
+      <c r="F173" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="B174" t="s">
+        <v>694</v>
+      </c>
+      <c r="C174" t="s">
+        <v>39</v>
+      </c>
+      <c r="D174" t="s">
+        <v>42</v>
+      </c>
+      <c r="E174" t="s">
+        <v>43</v>
+      </c>
+      <c r="F174" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="B175" t="s">
+        <v>695</v>
+      </c>
+      <c r="C175" t="s">
+        <v>39</v>
+      </c>
+      <c r="D175" t="s">
+        <v>42</v>
+      </c>
+      <c r="E175" t="s">
+        <v>43</v>
+      </c>
+      <c r="F175" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="B176" t="s">
+        <v>696</v>
+      </c>
+      <c r="C176" t="s">
+        <v>39</v>
+      </c>
+      <c r="D176" t="s">
+        <v>42</v>
+      </c>
+      <c r="E176" t="s">
+        <v>43</v>
+      </c>
+      <c r="F176" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-custom parameter names are now initialized from Qt GUI
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242698" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259578" uniqueCount="726">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2152,6 +2152,93 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId329</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId338</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId352</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId355</t>
   </si>
 </sst>
 </file>
@@ -5573,7 +5660,7 @@
     </row>
     <row r="120">
       <c r="B120" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="C120" t="s">
         <v>39</v>
@@ -5585,12 +5672,12 @@
         <v>43</v>
       </c>
       <c r="F120" t="s">
-        <v>583</v>
+        <v>596</v>
       </c>
     </row>
     <row r="121">
       <c r="B121" t="s">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="C121" t="s">
         <v>39</v>
@@ -5602,15 +5689,15 @@
         <v>43</v>
       </c>
       <c r="F121" t="s">
-        <v>584</v>
+        <v>559</v>
       </c>
     </row>
     <row r="122">
       <c r="B122" t="s">
-        <v>564</v>
+        <v>585</v>
       </c>
       <c r="C122" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D122" t="s">
         <v>42</v>
@@ -5619,15 +5706,15 @@
         <v>43</v>
       </c>
       <c r="F122" t="s">
-        <v>580</v>
+        <v>223</v>
       </c>
     </row>
     <row r="123">
       <c r="B123" t="s">
-        <v>566</v>
+        <v>586</v>
       </c>
       <c r="C123" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D123" t="s">
         <v>42</v>
@@ -5636,32 +5723,32 @@
         <v>43</v>
       </c>
       <c r="F123" t="s">
-        <v>581</v>
+        <v>109</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" t="s">
-        <v>567</v>
+        <v>587</v>
       </c>
       <c r="C124" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D124" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E124" t="s">
         <v>43</v>
       </c>
       <c r="F124" t="s">
-        <v>370</v>
+        <v>392</v>
       </c>
     </row>
     <row r="125">
       <c r="B125" t="s">
-        <v>568</v>
+        <v>588</v>
       </c>
       <c r="C125" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D125" t="s">
         <v>42</v>
@@ -5670,15 +5757,15 @@
         <v>43</v>
       </c>
       <c r="F125" t="s">
-        <v>582</v>
+        <v>596</v>
       </c>
     </row>
     <row r="126">
       <c r="B126" t="s">
-        <v>572</v>
+        <v>590</v>
       </c>
       <c r="C126" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D126" t="s">
         <v>42</v>
@@ -5687,15 +5774,15 @@
         <v>43</v>
       </c>
       <c r="F126" t="s">
-        <v>559</v>
+        <v>596</v>
       </c>
     </row>
     <row r="127">
       <c r="B127" t="s">
-        <v>585</v>
+        <v>592</v>
       </c>
       <c r="C127" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D127" t="s">
         <v>42</v>
@@ -5704,15 +5791,15 @@
         <v>43</v>
       </c>
       <c r="F127" t="s">
-        <v>223</v>
+        <v>593</v>
       </c>
     </row>
     <row r="128">
       <c r="B128" t="s">
-        <v>586</v>
+        <v>594</v>
       </c>
       <c r="C128" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D128" t="s">
         <v>42</v>
@@ -5721,29 +5808,29 @@
         <v>43</v>
       </c>
       <c r="F128" t="s">
-        <v>109</v>
+        <v>595</v>
       </c>
     </row>
     <row r="129">
       <c r="B129" t="s">
-        <v>587</v>
+        <v>597</v>
       </c>
       <c r="C129" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D129" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E129" t="s">
         <v>43</v>
       </c>
       <c r="F129" t="s">
-        <v>392</v>
+        <v>596</v>
       </c>
     </row>
     <row r="130">
       <c r="B130" t="s">
-        <v>588</v>
+        <v>598</v>
       </c>
       <c r="C130" t="s">
         <v>40</v>
@@ -5755,12 +5842,12 @@
         <v>43</v>
       </c>
       <c r="F130" t="s">
-        <v>596</v>
+        <v>109</v>
       </c>
     </row>
     <row r="131">
       <c r="B131" t="s">
-        <v>590</v>
+        <v>599</v>
       </c>
       <c r="C131" t="s">
         <v>40</v>
@@ -5777,7 +5864,7 @@
     </row>
     <row r="132">
       <c r="B132" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
       <c r="C132" t="s">
         <v>40</v>
@@ -5789,32 +5876,32 @@
         <v>43</v>
       </c>
       <c r="F132" t="s">
-        <v>593</v>
+        <v>623</v>
       </c>
     </row>
     <row r="133">
       <c r="B133" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="C133" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D133" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E133" t="s">
         <v>43</v>
       </c>
       <c r="F133" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
     </row>
     <row r="134">
       <c r="B134" t="s">
-        <v>597</v>
+        <v>612</v>
       </c>
       <c r="C134" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D134" t="s">
         <v>42</v>
@@ -5823,15 +5910,15 @@
         <v>43</v>
       </c>
       <c r="F134" t="s">
-        <v>596</v>
+        <v>603</v>
       </c>
     </row>
     <row r="135">
       <c r="B135" t="s">
-        <v>598</v>
+        <v>619</v>
       </c>
       <c r="C135" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D135" t="s">
         <v>42</v>
@@ -5840,15 +5927,15 @@
         <v>43</v>
       </c>
       <c r="F135" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
     </row>
     <row r="136">
       <c r="B136" t="s">
-        <v>599</v>
+        <v>620</v>
       </c>
       <c r="C136" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D136" t="s">
         <v>42</v>
@@ -5857,46 +5944,46 @@
         <v>43</v>
       </c>
       <c r="F136" t="s">
-        <v>596</v>
+        <v>109</v>
       </c>
     </row>
     <row r="137">
       <c r="B137" t="s">
-        <v>600</v>
+        <v>621</v>
       </c>
       <c r="C137" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D137" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E137" t="s">
         <v>43</v>
       </c>
       <c r="F137" t="s">
-        <v>623</v>
+        <v>392</v>
       </c>
     </row>
     <row r="138">
       <c r="B138" t="s">
-        <v>602</v>
+        <v>624</v>
       </c>
       <c r="C138" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D138" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E138" t="s">
         <v>43</v>
       </c>
       <c r="F138" t="s">
-        <v>603</v>
+        <v>644</v>
       </c>
     </row>
     <row r="139">
       <c r="B139" t="s">
-        <v>612</v>
+        <v>625</v>
       </c>
       <c r="C139" t="s">
         <v>39</v>
@@ -5908,15 +5995,15 @@
         <v>43</v>
       </c>
       <c r="F139" t="s">
-        <v>603</v>
+        <v>642</v>
       </c>
     </row>
     <row r="140">
       <c r="B140" t="s">
-        <v>619</v>
+        <v>631</v>
       </c>
       <c r="C140" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D140" t="s">
         <v>42</v>
@@ -5925,15 +6012,15 @@
         <v>43</v>
       </c>
       <c r="F140" t="s">
-        <v>223</v>
+        <v>639</v>
       </c>
     </row>
     <row r="141">
       <c r="B141" t="s">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="C141" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D141" t="s">
         <v>42</v>
@@ -5942,29 +6029,29 @@
         <v>43</v>
       </c>
       <c r="F141" t="s">
-        <v>109</v>
+        <v>641</v>
       </c>
     </row>
     <row r="142">
       <c r="B142" t="s">
-        <v>621</v>
+        <v>643</v>
       </c>
       <c r="C142" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D142" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E142" t="s">
         <v>43</v>
       </c>
       <c r="F142" t="s">
-        <v>392</v>
+        <v>336</v>
       </c>
     </row>
     <row r="143">
       <c r="B143" t="s">
-        <v>624</v>
+        <v>645</v>
       </c>
       <c r="C143" t="s">
         <v>39</v>
@@ -5976,15 +6063,15 @@
         <v>43</v>
       </c>
       <c r="F143" t="s">
-        <v>644</v>
+        <v>623</v>
       </c>
     </row>
     <row r="144">
       <c r="B144" t="s">
-        <v>625</v>
+        <v>647</v>
       </c>
       <c r="C144" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D144" t="s">
         <v>42</v>
@@ -5993,12 +6080,12 @@
         <v>43</v>
       </c>
       <c r="F144" t="s">
-        <v>642</v>
+        <v>650</v>
       </c>
     </row>
     <row r="145">
       <c r="B145" t="s">
-        <v>631</v>
+        <v>674</v>
       </c>
       <c r="C145" t="s">
         <v>39</v>
@@ -6010,12 +6097,12 @@
         <v>43</v>
       </c>
       <c r="F145" t="s">
-        <v>639</v>
+        <v>370</v>
       </c>
     </row>
     <row r="146">
       <c r="B146" t="s">
-        <v>640</v>
+        <v>675</v>
       </c>
       <c r="C146" t="s">
         <v>39</v>
@@ -6027,12 +6114,12 @@
         <v>43</v>
       </c>
       <c r="F146" t="s">
-        <v>641</v>
+        <v>596</v>
       </c>
     </row>
     <row r="147">
       <c r="B147" t="s">
-        <v>643</v>
+        <v>676</v>
       </c>
       <c r="C147" t="s">
         <v>39</v>
@@ -6044,12 +6131,12 @@
         <v>43</v>
       </c>
       <c r="F147" t="s">
-        <v>336</v>
+        <v>370</v>
       </c>
     </row>
     <row r="148">
       <c r="B148" t="s">
-        <v>645</v>
+        <v>677</v>
       </c>
       <c r="C148" t="s">
         <v>39</v>
@@ -6061,15 +6148,15 @@
         <v>43</v>
       </c>
       <c r="F148" t="s">
-        <v>623</v>
+        <v>596</v>
       </c>
     </row>
     <row r="149">
       <c r="B149" t="s">
-        <v>647</v>
+        <v>678</v>
       </c>
       <c r="C149" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D149" t="s">
         <v>42</v>
@@ -6078,12 +6165,12 @@
         <v>43</v>
       </c>
       <c r="F149" t="s">
-        <v>650</v>
+        <v>370</v>
       </c>
     </row>
     <row r="150">
       <c r="B150" t="s">
-        <v>652</v>
+        <v>679</v>
       </c>
       <c r="C150" t="s">
         <v>39</v>
@@ -6095,12 +6182,12 @@
         <v>43</v>
       </c>
       <c r="F150" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="151">
       <c r="B151" t="s">
-        <v>653</v>
+        <v>680</v>
       </c>
       <c r="C151" t="s">
         <v>39</v>
@@ -6117,7 +6204,7 @@
     </row>
     <row r="152">
       <c r="B152" t="s">
-        <v>654</v>
+        <v>681</v>
       </c>
       <c r="C152" t="s">
         <v>39</v>
@@ -6129,12 +6216,12 @@
         <v>43</v>
       </c>
       <c r="F152" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="153">
       <c r="B153" t="s">
-        <v>655</v>
+        <v>682</v>
       </c>
       <c r="C153" t="s">
         <v>39</v>
@@ -6151,7 +6238,7 @@
     </row>
     <row r="154">
       <c r="B154" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="C154" t="s">
         <v>39</v>
@@ -6163,12 +6250,12 @@
         <v>43</v>
       </c>
       <c r="F154" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="155">
       <c r="B155" t="s">
-        <v>675</v>
+        <v>684</v>
       </c>
       <c r="C155" t="s">
         <v>39</v>
@@ -6180,12 +6267,12 @@
         <v>43</v>
       </c>
       <c r="F155" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="156">
       <c r="B156" t="s">
-        <v>676</v>
+        <v>685</v>
       </c>
       <c r="C156" t="s">
         <v>39</v>
@@ -6197,12 +6284,12 @@
         <v>43</v>
       </c>
       <c r="F156" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="157">
       <c r="B157" t="s">
-        <v>677</v>
+        <v>686</v>
       </c>
       <c r="C157" t="s">
         <v>39</v>
@@ -6214,12 +6301,12 @@
         <v>43</v>
       </c>
       <c r="F157" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="158">
       <c r="B158" t="s">
-        <v>678</v>
+        <v>687</v>
       </c>
       <c r="C158" t="s">
         <v>39</v>
@@ -6231,12 +6318,12 @@
         <v>43</v>
       </c>
       <c r="F158" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="159">
       <c r="B159" t="s">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="C159" t="s">
         <v>39</v>
@@ -6248,12 +6335,12 @@
         <v>43</v>
       </c>
       <c r="F159" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="160">
       <c r="B160" t="s">
-        <v>680</v>
+        <v>689</v>
       </c>
       <c r="C160" t="s">
         <v>39</v>
@@ -6265,12 +6352,12 @@
         <v>43</v>
       </c>
       <c r="F160" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="161">
       <c r="B161" t="s">
-        <v>681</v>
+        <v>690</v>
       </c>
       <c r="C161" t="s">
         <v>39</v>
@@ -6282,12 +6369,12 @@
         <v>43</v>
       </c>
       <c r="F161" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="162">
       <c r="B162" t="s">
-        <v>682</v>
+        <v>691</v>
       </c>
       <c r="C162" t="s">
         <v>39</v>
@@ -6299,12 +6386,12 @@
         <v>43</v>
       </c>
       <c r="F162" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="163">
       <c r="B163" t="s">
-        <v>683</v>
+        <v>692</v>
       </c>
       <c r="C163" t="s">
         <v>39</v>
@@ -6316,12 +6403,12 @@
         <v>43</v>
       </c>
       <c r="F163" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="164">
       <c r="B164" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="C164" t="s">
         <v>39</v>
@@ -6333,12 +6420,12 @@
         <v>43</v>
       </c>
       <c r="F164" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="165">
       <c r="B165" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="C165" t="s">
         <v>39</v>
@@ -6350,12 +6437,12 @@
         <v>43</v>
       </c>
       <c r="F165" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="166">
       <c r="B166" t="s">
-        <v>686</v>
+        <v>695</v>
       </c>
       <c r="C166" t="s">
         <v>39</v>
@@ -6367,12 +6454,12 @@
         <v>43</v>
       </c>
       <c r="F166" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="167">
       <c r="B167" t="s">
-        <v>687</v>
+        <v>696</v>
       </c>
       <c r="C167" t="s">
         <v>39</v>
@@ -6384,12 +6471,12 @@
         <v>43</v>
       </c>
       <c r="F167" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="168">
       <c r="B168" t="s">
-        <v>688</v>
+        <v>707</v>
       </c>
       <c r="C168" t="s">
         <v>39</v>
@@ -6406,7 +6493,7 @@
     </row>
     <row r="169">
       <c r="B169" t="s">
-        <v>689</v>
+        <v>708</v>
       </c>
       <c r="C169" t="s">
         <v>39</v>
@@ -6423,7 +6510,7 @@
     </row>
     <row r="170">
       <c r="B170" t="s">
-        <v>690</v>
+        <v>709</v>
       </c>
       <c r="C170" t="s">
         <v>39</v>
@@ -6440,7 +6527,7 @@
     </row>
     <row r="171">
       <c r="B171" t="s">
-        <v>691</v>
+        <v>710</v>
       </c>
       <c r="C171" t="s">
         <v>39</v>
@@ -6457,7 +6544,7 @@
     </row>
     <row r="172">
       <c r="B172" t="s">
-        <v>692</v>
+        <v>711</v>
       </c>
       <c r="C172" t="s">
         <v>39</v>
@@ -6474,7 +6561,7 @@
     </row>
     <row r="173">
       <c r="B173" t="s">
-        <v>693</v>
+        <v>712</v>
       </c>
       <c r="C173" t="s">
         <v>39</v>
@@ -6491,7 +6578,7 @@
     </row>
     <row r="174">
       <c r="B174" t="s">
-        <v>694</v>
+        <v>713</v>
       </c>
       <c r="C174" t="s">
         <v>39</v>
@@ -6508,7 +6595,7 @@
     </row>
     <row r="175">
       <c r="B175" t="s">
-        <v>695</v>
+        <v>714</v>
       </c>
       <c r="C175" t="s">
         <v>39</v>
@@ -6525,7 +6612,7 @@
     </row>
     <row r="176">
       <c r="B176" t="s">
-        <v>696</v>
+        <v>715</v>
       </c>
       <c r="C176" t="s">
         <v>39</v>
@@ -6537,6 +6624,176 @@
         <v>43</v>
       </c>
       <c r="F176" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="B177" t="s">
+        <v>716</v>
+      </c>
+      <c r="C177" t="s">
+        <v>39</v>
+      </c>
+      <c r="D177" t="s">
+        <v>42</v>
+      </c>
+      <c r="E177" t="s">
+        <v>43</v>
+      </c>
+      <c r="F177" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="B178" t="s">
+        <v>717</v>
+      </c>
+      <c r="C178" t="s">
+        <v>39</v>
+      </c>
+      <c r="D178" t="s">
+        <v>42</v>
+      </c>
+      <c r="E178" t="s">
+        <v>43</v>
+      </c>
+      <c r="F178" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="B179" t="s">
+        <v>718</v>
+      </c>
+      <c r="C179" t="s">
+        <v>39</v>
+      </c>
+      <c r="D179" t="s">
+        <v>42</v>
+      </c>
+      <c r="E179" t="s">
+        <v>43</v>
+      </c>
+      <c r="F179" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="B180" t="s">
+        <v>719</v>
+      </c>
+      <c r="C180" t="s">
+        <v>39</v>
+      </c>
+      <c r="D180" t="s">
+        <v>42</v>
+      </c>
+      <c r="E180" t="s">
+        <v>43</v>
+      </c>
+      <c r="F180" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="B181" t="s">
+        <v>720</v>
+      </c>
+      <c r="C181" t="s">
+        <v>39</v>
+      </c>
+      <c r="D181" t="s">
+        <v>42</v>
+      </c>
+      <c r="E181" t="s">
+        <v>43</v>
+      </c>
+      <c r="F181" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="B182" t="s">
+        <v>721</v>
+      </c>
+      <c r="C182" t="s">
+        <v>39</v>
+      </c>
+      <c r="D182" t="s">
+        <v>42</v>
+      </c>
+      <c r="E182" t="s">
+        <v>43</v>
+      </c>
+      <c r="F182" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="B183" t="s">
+        <v>722</v>
+      </c>
+      <c r="C183" t="s">
+        <v>39</v>
+      </c>
+      <c r="D183" t="s">
+        <v>42</v>
+      </c>
+      <c r="E183" t="s">
+        <v>43</v>
+      </c>
+      <c r="F183" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="B184" t="s">
+        <v>723</v>
+      </c>
+      <c r="C184" t="s">
+        <v>39</v>
+      </c>
+      <c r="D184" t="s">
+        <v>42</v>
+      </c>
+      <c r="E184" t="s">
+        <v>43</v>
+      </c>
+      <c r="F184" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="B185" t="s">
+        <v>724</v>
+      </c>
+      <c r="C185" t="s">
+        <v>39</v>
+      </c>
+      <c r="D185" t="s">
+        <v>42</v>
+      </c>
+      <c r="E185" t="s">
+        <v>43</v>
+      </c>
+      <c r="F185" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="B186" t="s">
+        <v>725</v>
+      </c>
+      <c r="C186" t="s">
+        <v>39</v>
+      </c>
+      <c r="D186" t="s">
+        <v>42</v>
+      </c>
+      <c r="E186" t="s">
+        <v>43</v>
+      </c>
+      <c r="F186" t="s">
         <v>370</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-settable parameter names are now initialized from Qt GUI
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259578" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270776" uniqueCount="746">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2239,6 +2239,66 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId357</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId362</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId363</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId369</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId373</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId374</t>
   </si>
 </sst>
 </file>
@@ -3994,7 +4054,7 @@
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C22" t="s">
         <v>39</v>
@@ -4006,12 +4066,12 @@
         <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>338</v>
+        <v>596</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C23" t="s">
         <v>39</v>
@@ -4023,12 +4083,12 @@
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C24" t="s">
         <v>39</v>
@@ -4040,15 +4100,15 @@
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>347</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
         <v>42</v>
@@ -4057,15 +4117,15 @@
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>109</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
         <v>42</v>
@@ -4074,49 +4134,49 @@
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
         <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>386</v>
+        <v>399</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
         <v>43</v>
       </c>
       <c r="F28" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
         <v>42</v>
@@ -4125,46 +4185,46 @@
         <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>390</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="C30" t="s">
         <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>392</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="C31" t="s">
         <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s">
         <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>400</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
@@ -4176,12 +4236,12 @@
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -4193,12 +4253,12 @@
         <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="C34" t="s">
         <v>37</v>
@@ -4210,29 +4270,29 @@
         <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
         <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C36" t="s">
         <v>37</v>
@@ -4249,7 +4309,7 @@
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="C37" t="s">
         <v>37</v>
@@ -4266,27 +4326,27 @@
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E38" t="s">
         <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>75</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
         <v>42</v>
@@ -4295,15 +4355,15 @@
         <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -4312,12 +4372,12 @@
         <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>109</v>
+        <v>398</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C41" t="s">
         <v>39</v>
@@ -4329,12 +4389,12 @@
         <v>43</v>
       </c>
       <c r="F41" t="s">
-        <v>396</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="C42" t="s">
         <v>39</v>
@@ -4346,12 +4406,12 @@
         <v>43</v>
       </c>
       <c r="F42" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="C43" t="s">
         <v>39</v>
@@ -4363,12 +4423,12 @@
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>398</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C44" t="s">
         <v>39</v>
@@ -4380,12 +4440,12 @@
         <v>43</v>
       </c>
       <c r="F44" t="s">
-        <v>109</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="C45" t="s">
         <v>39</v>
@@ -4397,12 +4457,12 @@
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>263</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="C46" t="s">
         <v>39</v>
@@ -4414,63 +4474,63 @@
         <v>43</v>
       </c>
       <c r="F46" t="s">
-        <v>109</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E47" t="s">
         <v>43</v>
       </c>
       <c r="F47" t="s">
-        <v>262</v>
+        <v>400</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D48" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E48" t="s">
         <v>43</v>
       </c>
       <c r="F48" t="s">
-        <v>109</v>
+        <v>359</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E49" t="s">
         <v>43</v>
       </c>
       <c r="F49" t="s">
-        <v>225</v>
+        <v>359</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="C50" t="s">
         <v>37</v>
@@ -4482,63 +4542,63 @@
         <v>43</v>
       </c>
       <c r="F50" t="s">
-        <v>400</v>
+        <v>340</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C51" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E51" t="s">
         <v>43</v>
       </c>
       <c r="F51" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D52" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E52" t="s">
         <v>43</v>
       </c>
       <c r="F52" t="s">
-        <v>359</v>
+        <v>336</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="C53" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E53" t="s">
         <v>43</v>
       </c>
       <c r="F53" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
@@ -4550,12 +4610,12 @@
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>338</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C55" t="s">
         <v>39</v>
@@ -4567,12 +4627,12 @@
         <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>336</v>
+        <v>385</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C56" t="s">
         <v>39</v>
@@ -4584,12 +4644,12 @@
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>347</v>
+        <v>442</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C57" t="s">
         <v>39</v>
@@ -4601,12 +4661,12 @@
         <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>109</v>
+        <v>389</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C58" t="s">
         <v>39</v>
@@ -4618,32 +4678,32 @@
         <v>43</v>
       </c>
       <c r="F58" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D59" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E59" t="s">
         <v>43</v>
       </c>
       <c r="F59" t="s">
-        <v>442</v>
+        <v>392</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C60" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D60" t="s">
         <v>42</v>
@@ -4652,15 +4712,15 @@
         <v>43</v>
       </c>
       <c r="F60" t="s">
-        <v>389</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C61" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D61" t="s">
         <v>42</v>
@@ -4669,12 +4729,12 @@
         <v>43</v>
       </c>
       <c r="F61" t="s">
-        <v>390</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="C62" t="s">
         <v>37</v>
@@ -4691,27 +4751,27 @@
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="C63" t="s">
         <v>37</v>
       </c>
       <c r="D63" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E63" t="s">
         <v>43</v>
       </c>
       <c r="F63" t="s">
-        <v>223</v>
+        <v>392</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="C64" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D64" t="s">
         <v>42</v>
@@ -4720,46 +4780,46 @@
         <v>43</v>
       </c>
       <c r="F64" t="s">
-        <v>109</v>
+        <v>450</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="C65" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D65" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E65" t="s">
         <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>392</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="C66" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D66" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E66" t="s">
         <v>43</v>
       </c>
       <c r="F66" t="s">
-        <v>392</v>
+        <v>452</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="C67" t="s">
         <v>39</v>
@@ -4771,49 +4831,49 @@
         <v>43</v>
       </c>
       <c r="F67" t="s">
-        <v>450</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>444</v>
+        <v>467</v>
       </c>
       <c r="C68" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D68" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E68" t="s">
         <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>109</v>
+        <v>548</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>446</v>
+        <v>469</v>
       </c>
       <c r="C69" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D69" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E69" t="s">
         <v>43</v>
       </c>
       <c r="F69" t="s">
-        <v>452</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>447</v>
+        <v>470</v>
       </c>
       <c r="C70" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D70" t="s">
         <v>42</v>
@@ -4822,15 +4882,15 @@
         <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="C71" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D71" t="s">
         <v>42</v>
@@ -4839,12 +4899,12 @@
         <v>43</v>
       </c>
       <c r="F71" t="s">
-        <v>391</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="C72" t="s">
         <v>39</v>
@@ -4856,12 +4916,12 @@
         <v>43</v>
       </c>
       <c r="F72" t="s">
-        <v>460</v>
+        <v>396</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>459</v>
+        <v>473</v>
       </c>
       <c r="C73" t="s">
         <v>39</v>
@@ -4873,12 +4933,12 @@
         <v>43</v>
       </c>
       <c r="F73" t="s">
-        <v>461</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="C74" t="s">
         <v>39</v>
@@ -4890,49 +4950,49 @@
         <v>43</v>
       </c>
       <c r="F74" t="s">
-        <v>463</v>
+        <v>398</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="C75" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D75" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E75" t="s">
         <v>43</v>
       </c>
       <c r="F75" t="s">
-        <v>548</v>
+        <v>109</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="C76" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D76" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E76" t="s">
         <v>43</v>
       </c>
       <c r="F76" t="s">
-        <v>75</v>
+        <v>263</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="C77" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D77" t="s">
         <v>42</v>
@@ -4941,15 +5001,15 @@
         <v>43</v>
       </c>
       <c r="F77" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="C78" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D78" t="s">
         <v>42</v>
@@ -4958,12 +5018,12 @@
         <v>43</v>
       </c>
       <c r="F78" t="s">
-        <v>109</v>
+        <v>262</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="C79" t="s">
         <v>39</v>
@@ -4975,12 +5035,12 @@
         <v>43</v>
       </c>
       <c r="F79" t="s">
-        <v>396</v>
+        <v>109</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="C80" t="s">
         <v>39</v>
@@ -4992,12 +5052,12 @@
         <v>43</v>
       </c>
       <c r="F80" t="s">
-        <v>109</v>
+        <v>488</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="C81" t="s">
         <v>39</v>
@@ -5009,12 +5069,12 @@
         <v>43</v>
       </c>
       <c r="F81" t="s">
-        <v>398</v>
+        <v>450</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C82" t="s">
         <v>39</v>
@@ -5031,7 +5091,7 @@
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="C83" t="s">
         <v>39</v>
@@ -5043,12 +5103,12 @@
         <v>43</v>
       </c>
       <c r="F83" t="s">
-        <v>263</v>
+        <v>452</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C84" t="s">
         <v>39</v>
@@ -5065,7 +5125,7 @@
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>478</v>
+        <v>508</v>
       </c>
       <c r="C85" t="s">
         <v>39</v>
@@ -5077,12 +5137,12 @@
         <v>43</v>
       </c>
       <c r="F85" t="s">
-        <v>262</v>
+        <v>506</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>479</v>
+        <v>509</v>
       </c>
       <c r="C86" t="s">
         <v>39</v>
@@ -5099,7 +5159,7 @@
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>480</v>
+        <v>510</v>
       </c>
       <c r="C87" t="s">
         <v>39</v>
@@ -5111,12 +5171,12 @@
         <v>43</v>
       </c>
       <c r="F87" t="s">
-        <v>488</v>
+        <v>507</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>484</v>
+        <v>511</v>
       </c>
       <c r="C88" t="s">
         <v>39</v>
@@ -5128,12 +5188,12 @@
         <v>43</v>
       </c>
       <c r="F88" t="s">
-        <v>450</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>485</v>
+        <v>512</v>
       </c>
       <c r="C89" t="s">
         <v>39</v>
@@ -5145,12 +5205,12 @@
         <v>43</v>
       </c>
       <c r="F89" t="s">
-        <v>109</v>
+        <v>503</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>486</v>
+        <v>513</v>
       </c>
       <c r="C90" t="s">
         <v>39</v>
@@ -5162,12 +5222,12 @@
         <v>43</v>
       </c>
       <c r="F90" t="s">
-        <v>452</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>487</v>
+        <v>514</v>
       </c>
       <c r="C91" t="s">
         <v>39</v>
@@ -5179,12 +5239,12 @@
         <v>43</v>
       </c>
       <c r="F91" t="s">
-        <v>109</v>
+        <v>505</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="C92" t="s">
         <v>39</v>
@@ -5196,12 +5256,12 @@
         <v>43</v>
       </c>
       <c r="F92" t="s">
-        <v>506</v>
+        <v>109</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="C93" t="s">
         <v>39</v>
@@ -5213,12 +5273,12 @@
         <v>43</v>
       </c>
       <c r="F93" t="s">
-        <v>109</v>
+        <v>496</v>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="C94" t="s">
         <v>39</v>
@@ -5230,12 +5290,12 @@
         <v>43</v>
       </c>
       <c r="F94" t="s">
-        <v>507</v>
+        <v>109</v>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="C95" t="s">
         <v>39</v>
@@ -5247,12 +5307,12 @@
         <v>43</v>
       </c>
       <c r="F95" t="s">
-        <v>109</v>
+        <v>504</v>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="C96" t="s">
         <v>39</v>
@@ -5264,12 +5324,12 @@
         <v>43</v>
       </c>
       <c r="F96" t="s">
-        <v>503</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="C97" t="s">
         <v>39</v>
@@ -5281,12 +5341,12 @@
         <v>43</v>
       </c>
       <c r="F97" t="s">
-        <v>109</v>
+        <v>506</v>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="C98" t="s">
         <v>39</v>
@@ -5298,12 +5358,12 @@
         <v>43</v>
       </c>
       <c r="F98" t="s">
-        <v>505</v>
+        <v>109</v>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="C99" t="s">
         <v>39</v>
@@ -5315,12 +5375,12 @@
         <v>43</v>
       </c>
       <c r="F99" t="s">
-        <v>109</v>
+        <v>507</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="C100" t="s">
         <v>39</v>
@@ -5332,12 +5392,12 @@
         <v>43</v>
       </c>
       <c r="F100" t="s">
-        <v>496</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="C101" t="s">
         <v>39</v>
@@ -5349,12 +5409,12 @@
         <v>43</v>
       </c>
       <c r="F101" t="s">
-        <v>109</v>
+        <v>503</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="C102" t="s">
         <v>39</v>
@@ -5366,12 +5426,12 @@
         <v>43</v>
       </c>
       <c r="F102" t="s">
-        <v>504</v>
+        <v>109</v>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="C103" t="s">
         <v>39</v>
@@ -5383,12 +5443,12 @@
         <v>43</v>
       </c>
       <c r="F103" t="s">
-        <v>109</v>
+        <v>505</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="C104" t="s">
         <v>39</v>
@@ -5400,12 +5460,12 @@
         <v>43</v>
       </c>
       <c r="F104" t="s">
-        <v>506</v>
+        <v>109</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="C105" t="s">
         <v>39</v>
@@ -5417,12 +5477,12 @@
         <v>43</v>
       </c>
       <c r="F105" t="s">
-        <v>109</v>
+        <v>496</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="C106" t="s">
         <v>39</v>
@@ -5434,12 +5494,12 @@
         <v>43</v>
       </c>
       <c r="F106" t="s">
-        <v>507</v>
+        <v>109</v>
       </c>
     </row>
     <row r="107">
       <c r="B107" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="C107" t="s">
         <v>39</v>
@@ -5451,12 +5511,12 @@
         <v>43</v>
       </c>
       <c r="F107" t="s">
-        <v>109</v>
+        <v>504</v>
       </c>
     </row>
     <row r="108">
       <c r="B108" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="C108" t="s">
         <v>39</v>
@@ -5468,46 +5528,46 @@
         <v>43</v>
       </c>
       <c r="F108" t="s">
-        <v>503</v>
+        <v>109</v>
       </c>
     </row>
     <row r="109">
       <c r="B109" t="s">
-        <v>525</v>
+        <v>546</v>
       </c>
       <c r="C109" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D109" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E109" t="s">
         <v>43</v>
       </c>
       <c r="F109" t="s">
-        <v>109</v>
+        <v>549</v>
       </c>
     </row>
     <row r="110">
       <c r="B110" t="s">
-        <v>526</v>
+        <v>558</v>
       </c>
       <c r="C110" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D110" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E110" t="s">
         <v>43</v>
       </c>
       <c r="F110" t="s">
-        <v>505</v>
+        <v>559</v>
       </c>
     </row>
     <row r="111">
       <c r="B111" t="s">
-        <v>527</v>
+        <v>566</v>
       </c>
       <c r="C111" t="s">
         <v>39</v>
@@ -5519,12 +5579,12 @@
         <v>43</v>
       </c>
       <c r="F111" t="s">
-        <v>109</v>
+        <v>596</v>
       </c>
     </row>
     <row r="112">
       <c r="B112" t="s">
-        <v>528</v>
+        <v>572</v>
       </c>
       <c r="C112" t="s">
         <v>39</v>
@@ -5536,15 +5596,15 @@
         <v>43</v>
       </c>
       <c r="F112" t="s">
-        <v>496</v>
+        <v>559</v>
       </c>
     </row>
     <row r="113">
       <c r="B113" t="s">
-        <v>529</v>
+        <v>585</v>
       </c>
       <c r="C113" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D113" t="s">
         <v>42</v>
@@ -5553,15 +5613,15 @@
         <v>43</v>
       </c>
       <c r="F113" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
     </row>
     <row r="114">
       <c r="B114" t="s">
-        <v>530</v>
+        <v>586</v>
       </c>
       <c r="C114" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D114" t="s">
         <v>42</v>
@@ -5570,32 +5630,32 @@
         <v>43</v>
       </c>
       <c r="F114" t="s">
-        <v>504</v>
+        <v>109</v>
       </c>
     </row>
     <row r="115">
       <c r="B115" t="s">
-        <v>531</v>
+        <v>587</v>
       </c>
       <c r="C115" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D115" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E115" t="s">
         <v>43</v>
       </c>
       <c r="F115" t="s">
-        <v>109</v>
+        <v>392</v>
       </c>
     </row>
     <row r="116">
       <c r="B116" t="s">
-        <v>544</v>
+        <v>588</v>
       </c>
       <c r="C116" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D116" t="s">
         <v>42</v>
@@ -5604,15 +5664,15 @@
         <v>43</v>
       </c>
       <c r="F116" t="s">
-        <v>542</v>
+        <v>596</v>
       </c>
     </row>
     <row r="117">
       <c r="B117" t="s">
-        <v>545</v>
+        <v>590</v>
       </c>
       <c r="C117" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D117" t="s">
         <v>42</v>
@@ -5621,49 +5681,49 @@
         <v>43</v>
       </c>
       <c r="F117" t="s">
-        <v>543</v>
+        <v>596</v>
       </c>
     </row>
     <row r="118">
       <c r="B118" t="s">
-        <v>546</v>
+        <v>592</v>
       </c>
       <c r="C118" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D118" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E118" t="s">
         <v>43</v>
       </c>
       <c r="F118" t="s">
-        <v>549</v>
+        <v>593</v>
       </c>
     </row>
     <row r="119">
       <c r="B119" t="s">
-        <v>558</v>
+        <v>594</v>
       </c>
       <c r="C119" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D119" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E119" t="s">
         <v>43</v>
       </c>
       <c r="F119" t="s">
-        <v>559</v>
+        <v>595</v>
       </c>
     </row>
     <row r="120">
       <c r="B120" t="s">
-        <v>566</v>
+        <v>597</v>
       </c>
       <c r="C120" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D120" t="s">
         <v>42</v>
@@ -5677,10 +5737,10 @@
     </row>
     <row r="121">
       <c r="B121" t="s">
-        <v>572</v>
+        <v>598</v>
       </c>
       <c r="C121" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D121" t="s">
         <v>42</v>
@@ -5689,15 +5749,15 @@
         <v>43</v>
       </c>
       <c r="F121" t="s">
-        <v>559</v>
+        <v>109</v>
       </c>
     </row>
     <row r="122">
       <c r="B122" t="s">
-        <v>585</v>
+        <v>599</v>
       </c>
       <c r="C122" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D122" t="s">
         <v>42</v>
@@ -5706,15 +5766,15 @@
         <v>43</v>
       </c>
       <c r="F122" t="s">
-        <v>223</v>
+        <v>596</v>
       </c>
     </row>
     <row r="123">
       <c r="B123" t="s">
-        <v>586</v>
+        <v>600</v>
       </c>
       <c r="C123" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D123" t="s">
         <v>42</v>
@@ -5723,12 +5783,12 @@
         <v>43</v>
       </c>
       <c r="F123" t="s">
-        <v>109</v>
+        <v>623</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" t="s">
-        <v>587</v>
+        <v>602</v>
       </c>
       <c r="C124" t="s">
         <v>37</v>
@@ -5740,15 +5800,15 @@
         <v>43</v>
       </c>
       <c r="F124" t="s">
-        <v>392</v>
+        <v>603</v>
       </c>
     </row>
     <row r="125">
       <c r="B125" t="s">
-        <v>588</v>
+        <v>612</v>
       </c>
       <c r="C125" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D125" t="s">
         <v>42</v>
@@ -5757,15 +5817,15 @@
         <v>43</v>
       </c>
       <c r="F125" t="s">
-        <v>596</v>
+        <v>603</v>
       </c>
     </row>
     <row r="126">
       <c r="B126" t="s">
-        <v>590</v>
+        <v>619</v>
       </c>
       <c r="C126" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D126" t="s">
         <v>42</v>
@@ -5774,15 +5834,15 @@
         <v>43</v>
       </c>
       <c r="F126" t="s">
-        <v>596</v>
+        <v>223</v>
       </c>
     </row>
     <row r="127">
       <c r="B127" t="s">
-        <v>592</v>
+        <v>620</v>
       </c>
       <c r="C127" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D127" t="s">
         <v>42</v>
@@ -5791,32 +5851,32 @@
         <v>43</v>
       </c>
       <c r="F127" t="s">
-        <v>593</v>
+        <v>109</v>
       </c>
     </row>
     <row r="128">
       <c r="B128" t="s">
-        <v>594</v>
+        <v>621</v>
       </c>
       <c r="C128" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D128" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E128" t="s">
         <v>43</v>
       </c>
       <c r="F128" t="s">
-        <v>595</v>
+        <v>392</v>
       </c>
     </row>
     <row r="129">
       <c r="B129" t="s">
-        <v>597</v>
+        <v>624</v>
       </c>
       <c r="C129" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D129" t="s">
         <v>42</v>
@@ -5825,15 +5885,15 @@
         <v>43</v>
       </c>
       <c r="F129" t="s">
-        <v>596</v>
+        <v>644</v>
       </c>
     </row>
     <row r="130">
       <c r="B130" t="s">
-        <v>598</v>
+        <v>625</v>
       </c>
       <c r="C130" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D130" t="s">
         <v>42</v>
@@ -5842,15 +5902,15 @@
         <v>43</v>
       </c>
       <c r="F130" t="s">
-        <v>109</v>
+        <v>642</v>
       </c>
     </row>
     <row r="131">
       <c r="B131" t="s">
-        <v>599</v>
+        <v>631</v>
       </c>
       <c r="C131" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D131" t="s">
         <v>42</v>
@@ -5859,15 +5919,15 @@
         <v>43</v>
       </c>
       <c r="F131" t="s">
-        <v>596</v>
+        <v>639</v>
       </c>
     </row>
     <row r="132">
       <c r="B132" t="s">
-        <v>600</v>
+        <v>640</v>
       </c>
       <c r="C132" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D132" t="s">
         <v>42</v>
@@ -5876,29 +5936,29 @@
         <v>43</v>
       </c>
       <c r="F132" t="s">
-        <v>623</v>
+        <v>641</v>
       </c>
     </row>
     <row r="133">
       <c r="B133" t="s">
-        <v>602</v>
+        <v>643</v>
       </c>
       <c r="C133" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D133" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E133" t="s">
         <v>43</v>
       </c>
       <c r="F133" t="s">
-        <v>603</v>
+        <v>336</v>
       </c>
     </row>
     <row r="134">
       <c r="B134" t="s">
-        <v>612</v>
+        <v>645</v>
       </c>
       <c r="C134" t="s">
         <v>39</v>
@@ -5910,12 +5970,12 @@
         <v>43</v>
       </c>
       <c r="F134" t="s">
-        <v>603</v>
+        <v>623</v>
       </c>
     </row>
     <row r="135">
       <c r="B135" t="s">
-        <v>619</v>
+        <v>647</v>
       </c>
       <c r="C135" t="s">
         <v>37</v>
@@ -5927,15 +5987,15 @@
         <v>43</v>
       </c>
       <c r="F135" t="s">
-        <v>223</v>
+        <v>650</v>
       </c>
     </row>
     <row r="136">
       <c r="B136" t="s">
-        <v>620</v>
+        <v>674</v>
       </c>
       <c r="C136" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D136" t="s">
         <v>42</v>
@@ -5944,29 +6004,29 @@
         <v>43</v>
       </c>
       <c r="F136" t="s">
-        <v>109</v>
+        <v>370</v>
       </c>
     </row>
     <row r="137">
       <c r="B137" t="s">
-        <v>621</v>
+        <v>675</v>
       </c>
       <c r="C137" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D137" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E137" t="s">
         <v>43</v>
       </c>
       <c r="F137" t="s">
-        <v>392</v>
+        <v>596</v>
       </c>
     </row>
     <row r="138">
       <c r="B138" t="s">
-        <v>624</v>
+        <v>676</v>
       </c>
       <c r="C138" t="s">
         <v>39</v>
@@ -5978,12 +6038,12 @@
         <v>43</v>
       </c>
       <c r="F138" t="s">
-        <v>644</v>
+        <v>370</v>
       </c>
     </row>
     <row r="139">
       <c r="B139" t="s">
-        <v>625</v>
+        <v>677</v>
       </c>
       <c r="C139" t="s">
         <v>39</v>
@@ -5995,12 +6055,12 @@
         <v>43</v>
       </c>
       <c r="F139" t="s">
-        <v>642</v>
+        <v>596</v>
       </c>
     </row>
     <row r="140">
       <c r="B140" t="s">
-        <v>631</v>
+        <v>678</v>
       </c>
       <c r="C140" t="s">
         <v>39</v>
@@ -6012,12 +6072,12 @@
         <v>43</v>
       </c>
       <c r="F140" t="s">
-        <v>639</v>
+        <v>370</v>
       </c>
     </row>
     <row r="141">
       <c r="B141" t="s">
-        <v>640</v>
+        <v>679</v>
       </c>
       <c r="C141" t="s">
         <v>39</v>
@@ -6029,12 +6089,12 @@
         <v>43</v>
       </c>
       <c r="F141" t="s">
-        <v>641</v>
+        <v>596</v>
       </c>
     </row>
     <row r="142">
       <c r="B142" t="s">
-        <v>643</v>
+        <v>680</v>
       </c>
       <c r="C142" t="s">
         <v>39</v>
@@ -6046,12 +6106,12 @@
         <v>43</v>
       </c>
       <c r="F142" t="s">
-        <v>336</v>
+        <v>370</v>
       </c>
     </row>
     <row r="143">
       <c r="B143" t="s">
-        <v>645</v>
+        <v>681</v>
       </c>
       <c r="C143" t="s">
         <v>39</v>
@@ -6063,15 +6123,15 @@
         <v>43</v>
       </c>
       <c r="F143" t="s">
-        <v>623</v>
+        <v>596</v>
       </c>
     </row>
     <row r="144">
       <c r="B144" t="s">
-        <v>647</v>
+        <v>682</v>
       </c>
       <c r="C144" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D144" t="s">
         <v>42</v>
@@ -6080,12 +6140,12 @@
         <v>43</v>
       </c>
       <c r="F144" t="s">
-        <v>650</v>
+        <v>370</v>
       </c>
     </row>
     <row r="145">
       <c r="B145" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="C145" t="s">
         <v>39</v>
@@ -6097,12 +6157,12 @@
         <v>43</v>
       </c>
       <c r="F145" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="146">
       <c r="B146" t="s">
-        <v>675</v>
+        <v>684</v>
       </c>
       <c r="C146" t="s">
         <v>39</v>
@@ -6114,12 +6174,12 @@
         <v>43</v>
       </c>
       <c r="F146" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="147">
       <c r="B147" t="s">
-        <v>676</v>
+        <v>685</v>
       </c>
       <c r="C147" t="s">
         <v>39</v>
@@ -6131,12 +6191,12 @@
         <v>43</v>
       </c>
       <c r="F147" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="148">
       <c r="B148" t="s">
-        <v>677</v>
+        <v>686</v>
       </c>
       <c r="C148" t="s">
         <v>39</v>
@@ -6148,12 +6208,12 @@
         <v>43</v>
       </c>
       <c r="F148" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="149">
       <c r="B149" t="s">
-        <v>678</v>
+        <v>687</v>
       </c>
       <c r="C149" t="s">
         <v>39</v>
@@ -6165,12 +6225,12 @@
         <v>43</v>
       </c>
       <c r="F149" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="150">
       <c r="B150" t="s">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="C150" t="s">
         <v>39</v>
@@ -6182,12 +6242,12 @@
         <v>43</v>
       </c>
       <c r="F150" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="151">
       <c r="B151" t="s">
-        <v>680</v>
+        <v>689</v>
       </c>
       <c r="C151" t="s">
         <v>39</v>
@@ -6199,12 +6259,12 @@
         <v>43</v>
       </c>
       <c r="F151" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="152">
       <c r="B152" t="s">
-        <v>681</v>
+        <v>690</v>
       </c>
       <c r="C152" t="s">
         <v>39</v>
@@ -6216,12 +6276,12 @@
         <v>43</v>
       </c>
       <c r="F152" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="153">
       <c r="B153" t="s">
-        <v>682</v>
+        <v>691</v>
       </c>
       <c r="C153" t="s">
         <v>39</v>
@@ -6233,12 +6293,12 @@
         <v>43</v>
       </c>
       <c r="F153" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="154">
       <c r="B154" t="s">
-        <v>683</v>
+        <v>692</v>
       </c>
       <c r="C154" t="s">
         <v>39</v>
@@ -6250,12 +6310,12 @@
         <v>43</v>
       </c>
       <c r="F154" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="155">
       <c r="B155" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="C155" t="s">
         <v>39</v>
@@ -6267,12 +6327,12 @@
         <v>43</v>
       </c>
       <c r="F155" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="156">
       <c r="B156" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="C156" t="s">
         <v>39</v>
@@ -6284,12 +6344,12 @@
         <v>43</v>
       </c>
       <c r="F156" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="157">
       <c r="B157" t="s">
-        <v>686</v>
+        <v>695</v>
       </c>
       <c r="C157" t="s">
         <v>39</v>
@@ -6301,12 +6361,12 @@
         <v>43</v>
       </c>
       <c r="F157" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="158">
       <c r="B158" t="s">
-        <v>687</v>
+        <v>696</v>
       </c>
       <c r="C158" t="s">
         <v>39</v>
@@ -6318,12 +6378,12 @@
         <v>43</v>
       </c>
       <c r="F158" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="159">
       <c r="B159" t="s">
-        <v>688</v>
+        <v>707</v>
       </c>
       <c r="C159" t="s">
         <v>39</v>
@@ -6340,7 +6400,7 @@
     </row>
     <row r="160">
       <c r="B160" t="s">
-        <v>689</v>
+        <v>708</v>
       </c>
       <c r="C160" t="s">
         <v>39</v>
@@ -6357,7 +6417,7 @@
     </row>
     <row r="161">
       <c r="B161" t="s">
-        <v>690</v>
+        <v>709</v>
       </c>
       <c r="C161" t="s">
         <v>39</v>
@@ -6374,7 +6434,7 @@
     </row>
     <row r="162">
       <c r="B162" t="s">
-        <v>691</v>
+        <v>710</v>
       </c>
       <c r="C162" t="s">
         <v>39</v>
@@ -6391,7 +6451,7 @@
     </row>
     <row r="163">
       <c r="B163" t="s">
-        <v>692</v>
+        <v>711</v>
       </c>
       <c r="C163" t="s">
         <v>39</v>
@@ -6408,7 +6468,7 @@
     </row>
     <row r="164">
       <c r="B164" t="s">
-        <v>693</v>
+        <v>712</v>
       </c>
       <c r="C164" t="s">
         <v>39</v>
@@ -6425,7 +6485,7 @@
     </row>
     <row r="165">
       <c r="B165" t="s">
-        <v>694</v>
+        <v>713</v>
       </c>
       <c r="C165" t="s">
         <v>39</v>
@@ -6442,7 +6502,7 @@
     </row>
     <row r="166">
       <c r="B166" t="s">
-        <v>695</v>
+        <v>714</v>
       </c>
       <c r="C166" t="s">
         <v>39</v>
@@ -6459,7 +6519,7 @@
     </row>
     <row r="167">
       <c r="B167" t="s">
-        <v>696</v>
+        <v>715</v>
       </c>
       <c r="C167" t="s">
         <v>39</v>
@@ -6476,7 +6536,7 @@
     </row>
     <row r="168">
       <c r="B168" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="C168" t="s">
         <v>39</v>
@@ -6488,12 +6548,12 @@
         <v>43</v>
       </c>
       <c r="F168" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="169">
       <c r="B169" t="s">
-        <v>708</v>
+        <v>717</v>
       </c>
       <c r="C169" t="s">
         <v>39</v>
@@ -6505,12 +6565,12 @@
         <v>43</v>
       </c>
       <c r="F169" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="170">
       <c r="B170" t="s">
-        <v>709</v>
+        <v>718</v>
       </c>
       <c r="C170" t="s">
         <v>39</v>
@@ -6522,12 +6582,12 @@
         <v>43</v>
       </c>
       <c r="F170" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="171">
       <c r="B171" t="s">
-        <v>710</v>
+        <v>719</v>
       </c>
       <c r="C171" t="s">
         <v>39</v>
@@ -6539,12 +6599,12 @@
         <v>43</v>
       </c>
       <c r="F171" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="172">
       <c r="B172" t="s">
-        <v>711</v>
+        <v>720</v>
       </c>
       <c r="C172" t="s">
         <v>39</v>
@@ -6556,12 +6616,12 @@
         <v>43</v>
       </c>
       <c r="F172" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="173">
       <c r="B173" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="C173" t="s">
         <v>39</v>
@@ -6573,12 +6633,12 @@
         <v>43</v>
       </c>
       <c r="F173" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="174">
       <c r="B174" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="C174" t="s">
         <v>39</v>
@@ -6590,12 +6650,12 @@
         <v>43</v>
       </c>
       <c r="F174" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="175">
       <c r="B175" t="s">
-        <v>714</v>
+        <v>723</v>
       </c>
       <c r="C175" t="s">
         <v>39</v>
@@ -6607,12 +6667,12 @@
         <v>43</v>
       </c>
       <c r="F175" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="176">
       <c r="B176" t="s">
-        <v>715</v>
+        <v>724</v>
       </c>
       <c r="C176" t="s">
         <v>39</v>
@@ -6624,12 +6684,12 @@
         <v>43</v>
       </c>
       <c r="F176" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="177">
       <c r="B177" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="C177" t="s">
         <v>39</v>
@@ -6641,12 +6701,12 @@
         <v>43</v>
       </c>
       <c r="F177" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="178">
       <c r="B178" t="s">
-        <v>717</v>
+        <v>727</v>
       </c>
       <c r="C178" t="s">
         <v>39</v>
@@ -6663,7 +6723,7 @@
     </row>
     <row r="179">
       <c r="B179" t="s">
-        <v>718</v>
+        <v>728</v>
       </c>
       <c r="C179" t="s">
         <v>39</v>
@@ -6680,7 +6740,7 @@
     </row>
     <row r="180">
       <c r="B180" t="s">
-        <v>719</v>
+        <v>729</v>
       </c>
       <c r="C180" t="s">
         <v>39</v>
@@ -6697,7 +6757,7 @@
     </row>
     <row r="181">
       <c r="B181" t="s">
-        <v>720</v>
+        <v>730</v>
       </c>
       <c r="C181" t="s">
         <v>39</v>
@@ -6714,7 +6774,7 @@
     </row>
     <row r="182">
       <c r="B182" t="s">
-        <v>721</v>
+        <v>731</v>
       </c>
       <c r="C182" t="s">
         <v>39</v>
@@ -6731,7 +6791,7 @@
     </row>
     <row r="183">
       <c r="B183" t="s">
-        <v>722</v>
+        <v>732</v>
       </c>
       <c r="C183" t="s">
         <v>39</v>
@@ -6748,7 +6808,7 @@
     </row>
     <row r="184">
       <c r="B184" t="s">
-        <v>723</v>
+        <v>733</v>
       </c>
       <c r="C184" t="s">
         <v>39</v>
@@ -6765,7 +6825,7 @@
     </row>
     <row r="185">
       <c r="B185" t="s">
-        <v>724</v>
+        <v>734</v>
       </c>
       <c r="C185" t="s">
         <v>39</v>
@@ -6782,7 +6842,7 @@
     </row>
     <row r="186">
       <c r="B186" t="s">
-        <v>725</v>
+        <v>735</v>
       </c>
       <c r="C186" t="s">
         <v>39</v>
@@ -6794,6 +6854,176 @@
         <v>43</v>
       </c>
       <c r="F186" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="B187" t="s">
+        <v>736</v>
+      </c>
+      <c r="C187" t="s">
+        <v>39</v>
+      </c>
+      <c r="D187" t="s">
+        <v>42</v>
+      </c>
+      <c r="E187" t="s">
+        <v>43</v>
+      </c>
+      <c r="F187" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="B188" t="s">
+        <v>737</v>
+      </c>
+      <c r="C188" t="s">
+        <v>39</v>
+      </c>
+      <c r="D188" t="s">
+        <v>42</v>
+      </c>
+      <c r="E188" t="s">
+        <v>43</v>
+      </c>
+      <c r="F188" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" t="s">
+        <v>738</v>
+      </c>
+      <c r="C189" t="s">
+        <v>39</v>
+      </c>
+      <c r="D189" t="s">
+        <v>42</v>
+      </c>
+      <c r="E189" t="s">
+        <v>43</v>
+      </c>
+      <c r="F189" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="B190" t="s">
+        <v>739</v>
+      </c>
+      <c r="C190" t="s">
+        <v>39</v>
+      </c>
+      <c r="D190" t="s">
+        <v>42</v>
+      </c>
+      <c r="E190" t="s">
+        <v>43</v>
+      </c>
+      <c r="F190" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="B191" t="s">
+        <v>740</v>
+      </c>
+      <c r="C191" t="s">
+        <v>39</v>
+      </c>
+      <c r="D191" t="s">
+        <v>42</v>
+      </c>
+      <c r="E191" t="s">
+        <v>43</v>
+      </c>
+      <c r="F191" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="B192" t="s">
+        <v>741</v>
+      </c>
+      <c r="C192" t="s">
+        <v>39</v>
+      </c>
+      <c r="D192" t="s">
+        <v>42</v>
+      </c>
+      <c r="E192" t="s">
+        <v>43</v>
+      </c>
+      <c r="F192" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="B193" t="s">
+        <v>742</v>
+      </c>
+      <c r="C193" t="s">
+        <v>39</v>
+      </c>
+      <c r="D193" t="s">
+        <v>42</v>
+      </c>
+      <c r="E193" t="s">
+        <v>43</v>
+      </c>
+      <c r="F193" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="B194" t="s">
+        <v>743</v>
+      </c>
+      <c r="C194" t="s">
+        <v>39</v>
+      </c>
+      <c r="D194" t="s">
+        <v>42</v>
+      </c>
+      <c r="E194" t="s">
+        <v>43</v>
+      </c>
+      <c r="F194" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="B195" t="s">
+        <v>744</v>
+      </c>
+      <c r="C195" t="s">
+        <v>39</v>
+      </c>
+      <c r="D195" t="s">
+        <v>42</v>
+      </c>
+      <c r="E195" t="s">
+        <v>43</v>
+      </c>
+      <c r="F195" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="B196" t="s">
+        <v>745</v>
+      </c>
+      <c r="C196" t="s">
+        <v>39</v>
+      </c>
+      <c r="D196" t="s">
+        <v>42</v>
+      </c>
+      <c r="E196" t="s">
+        <v>43</v>
+      </c>
+      <c r="F196" t="s">
         <v>370</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Scroll Wheel for choosing exponents
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270776" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294588" uniqueCount="761">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2299,6 +2299,51 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId374</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId376</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId379</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exp&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exp(&lt;value&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value to st: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId381</t>
   </si>
 </sst>
 </file>
@@ -4083,7 +4128,7 @@
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>347</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24">
@@ -7027,6 +7072,59 @@
         <v>370</v>
       </c>
     </row>
+    <row r="197">
+      <c r="B197" t="s">
+        <v>752</v>
+      </c>
+      <c r="C197" t="s">
+        <v>39</v>
+      </c>
+      <c r="D197" t="s">
+        <v>42</v>
+      </c>
+      <c r="E197" t="s">
+        <v>43</v>
+      </c>
+      <c r="F197" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="B198" t="s">
+        <v>758</v>
+      </c>
+      <c r="C198" t="s">
+        <v>39</v>
+      </c>
+      <c r="D198" t="s">
+        <v>42</v>
+      </c>
+      <c r="E198" t="s">
+        <v>43</v>
+      </c>
+      <c r="F198" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="B199" t="s">
+        <v>760</v>
+      </c>
+      <c r="C199" t="s">
+        <v>39</v>
+      </c>
+      <c r="D199" t="s">
+        <v>42</v>
+      </c>
+      <c r="E199" t="s">
+        <v>43</v>
+      </c>
+      <c r="F199" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="200"/>
+    <row r="201"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
implemented new value choosing mechanism
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294588" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310897" uniqueCount="791">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2344,6 +2344,96 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId381</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widget Wildcard Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExtraLarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId383</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId385</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId391</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId393</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId396</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId397</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId398</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId407</t>
   </si>
 </sst>
 </file>
@@ -3552,6 +3642,9 @@
       <c r="I3" s="20" t="s">
         <v>28</v>
       </c>
+      <c r="J3" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
@@ -3574,6 +3667,7 @@
         <v>292</v>
       </c>
       <c r="I4"/>
+      <c r="J4"/>
       <c r="K4" s="4" t="s">
         <v>9</v>
       </c>
@@ -3611,6 +3705,7 @@
         <v>292</v>
       </c>
       <c r="I5"/>
+      <c r="J5"/>
       <c r="K5" s="7" t="s">
         <v>1</v>
       </c>
@@ -3646,6 +3741,7 @@
         <v>292</v>
       </c>
       <c r="I6"/>
+      <c r="J6"/>
       <c r="K6" s="7" t="s">
         <v>2</v>
       </c>
@@ -3661,6 +3757,27 @@
       <c r="O6" s="10"/>
     </row>
     <row r="7" spans="2:15">
+      <c r="B7" t="s">
+        <v>762</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" t="s">
+        <v>292</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
       <c r="K7" s="7" t="s">
         <v>7</v>
       </c>
@@ -4119,7 +4236,7 @@
         <v>379</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>762</v>
       </c>
       <c r="D23" t="s">
         <v>42</v>
@@ -4128,15 +4245,15 @@
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>258</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
@@ -4145,15 +4262,15 @@
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>109</v>
+        <v>385</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
         <v>42</v>
@@ -4162,29 +4279,29 @@
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="C27" t="s">
         <v>37</v>
@@ -4196,29 +4313,29 @@
         <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C28" t="s">
         <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
         <v>43</v>
       </c>
       <c r="F28" t="s">
-        <v>400</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C29" t="s">
         <v>37</v>
@@ -4230,12 +4347,12 @@
         <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C30" t="s">
         <v>37</v>
@@ -4247,12 +4364,12 @@
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C31" t="s">
         <v>37</v>
@@ -4264,12 +4381,12 @@
         <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
@@ -4281,12 +4398,12 @@
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -4298,46 +4415,46 @@
         <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C34" t="s">
         <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E34" t="s">
         <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E35" t="s">
         <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C36" t="s">
         <v>37</v>
@@ -4349,15 +4466,15 @@
         <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D37" t="s">
         <v>42</v>
@@ -4366,12 +4483,12 @@
         <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>109</v>
+        <v>396</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C38" t="s">
         <v>39</v>
@@ -4383,12 +4500,12 @@
         <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>396</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C39" t="s">
         <v>39</v>
@@ -4400,12 +4517,12 @@
         <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>398</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C40" t="s">
         <v>39</v>
@@ -4417,12 +4534,12 @@
         <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>398</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C41" t="s">
         <v>39</v>
@@ -4434,12 +4551,12 @@
         <v>43</v>
       </c>
       <c r="F41" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C42" t="s">
         <v>39</v>
@@ -4451,12 +4568,12 @@
         <v>43</v>
       </c>
       <c r="F42" t="s">
-        <v>263</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C43" t="s">
         <v>39</v>
@@ -4468,12 +4585,12 @@
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>109</v>
+        <v>262</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C44" t="s">
         <v>39</v>
@@ -4485,12 +4602,12 @@
         <v>43</v>
       </c>
       <c r="F44" t="s">
-        <v>262</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C45" t="s">
         <v>39</v>
@@ -4502,29 +4619,29 @@
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>109</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D46" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E46" t="s">
         <v>43</v>
       </c>
       <c r="F46" t="s">
-        <v>225</v>
+        <v>400</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C47" t="s">
         <v>37</v>
@@ -4536,12 +4653,12 @@
         <v>43</v>
       </c>
       <c r="F47" t="s">
-        <v>400</v>
+        <v>359</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C48" t="s">
         <v>37</v>
@@ -4558,7 +4675,7 @@
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C49" t="s">
         <v>37</v>
@@ -4570,29 +4687,29 @@
         <v>43</v>
       </c>
       <c r="F49" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C50" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E50" t="s">
         <v>43</v>
       </c>
       <c r="F50" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C51" t="s">
         <v>39</v>
@@ -4604,12 +4721,12 @@
         <v>43</v>
       </c>
       <c r="F51" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C52" t="s">
         <v>39</v>
@@ -4621,12 +4738,12 @@
         <v>43</v>
       </c>
       <c r="F52" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C53" t="s">
         <v>39</v>
@@ -4638,12 +4755,12 @@
         <v>43</v>
       </c>
       <c r="F53" t="s">
-        <v>347</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
@@ -4655,12 +4772,12 @@
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>109</v>
+        <v>385</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C55" t="s">
         <v>39</v>
@@ -4672,12 +4789,12 @@
         <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>385</v>
+        <v>442</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C56" t="s">
         <v>39</v>
@@ -4689,12 +4806,12 @@
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>442</v>
+        <v>389</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C57" t="s">
         <v>39</v>
@@ -4706,46 +4823,46 @@
         <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C58" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D58" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E58" t="s">
         <v>43</v>
       </c>
       <c r="F58" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C59" t="s">
         <v>37</v>
       </c>
       <c r="D59" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E59" t="s">
         <v>43</v>
       </c>
       <c r="F59" t="s">
-        <v>392</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C60" t="s">
         <v>37</v>
@@ -4757,29 +4874,29 @@
         <v>43</v>
       </c>
       <c r="F60" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C61" t="s">
         <v>37</v>
       </c>
       <c r="D61" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E61" t="s">
         <v>43</v>
       </c>
       <c r="F61" t="s">
-        <v>109</v>
+        <v>392</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C62" t="s">
         <v>37</v>
@@ -4796,24 +4913,24 @@
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="C63" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D63" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E63" t="s">
         <v>43</v>
       </c>
       <c r="F63" t="s">
-        <v>392</v>
+        <v>450</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C64" t="s">
         <v>39</v>
@@ -4825,12 +4942,12 @@
         <v>43</v>
       </c>
       <c r="F64" t="s">
-        <v>450</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C65" t="s">
         <v>39</v>
@@ -4842,12 +4959,12 @@
         <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C66" t="s">
         <v>39</v>
@@ -4859,29 +4976,29 @@
         <v>43</v>
       </c>
       <c r="F66" t="s">
-        <v>452</v>
+        <v>109</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>447</v>
+        <v>467</v>
       </c>
       <c r="C67" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D67" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E67" t="s">
         <v>43</v>
       </c>
       <c r="F67" t="s">
-        <v>109</v>
+        <v>548</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C68" t="s">
         <v>37</v>
@@ -4893,29 +5010,29 @@
         <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>548</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C69" t="s">
         <v>37</v>
       </c>
       <c r="D69" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E69" t="s">
         <v>43</v>
       </c>
       <c r="F69" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C70" t="s">
         <v>37</v>
@@ -4927,15 +5044,15 @@
         <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C71" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D71" t="s">
         <v>42</v>
@@ -4944,12 +5061,12 @@
         <v>43</v>
       </c>
       <c r="F71" t="s">
-        <v>109</v>
+        <v>396</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C72" t="s">
         <v>39</v>
@@ -4961,12 +5078,12 @@
         <v>43</v>
       </c>
       <c r="F72" t="s">
-        <v>396</v>
+        <v>109</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C73" t="s">
         <v>39</v>
@@ -4978,12 +5095,12 @@
         <v>43</v>
       </c>
       <c r="F73" t="s">
-        <v>109</v>
+        <v>398</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C74" t="s">
         <v>39</v>
@@ -4995,12 +5112,12 @@
         <v>43</v>
       </c>
       <c r="F74" t="s">
-        <v>398</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C75" t="s">
         <v>39</v>
@@ -5012,12 +5129,12 @@
         <v>43</v>
       </c>
       <c r="F75" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C76" t="s">
         <v>39</v>
@@ -5029,12 +5146,12 @@
         <v>43</v>
       </c>
       <c r="F76" t="s">
-        <v>263</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C77" t="s">
         <v>39</v>
@@ -5046,12 +5163,12 @@
         <v>43</v>
       </c>
       <c r="F77" t="s">
-        <v>109</v>
+        <v>262</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C78" t="s">
         <v>39</v>
@@ -5063,12 +5180,12 @@
         <v>43</v>
       </c>
       <c r="F78" t="s">
-        <v>262</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C79" t="s">
         <v>39</v>
@@ -5080,12 +5197,12 @@
         <v>43</v>
       </c>
       <c r="F79" t="s">
-        <v>109</v>
+        <v>488</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="C80" t="s">
         <v>39</v>
@@ -5097,12 +5214,12 @@
         <v>43</v>
       </c>
       <c r="F80" t="s">
-        <v>488</v>
+        <v>450</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C81" t="s">
         <v>39</v>
@@ -5114,12 +5231,12 @@
         <v>43</v>
       </c>
       <c r="F81" t="s">
-        <v>450</v>
+        <v>109</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C82" t="s">
         <v>39</v>
@@ -5131,12 +5248,12 @@
         <v>43</v>
       </c>
       <c r="F82" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C83" t="s">
         <v>39</v>
@@ -5148,12 +5265,12 @@
         <v>43</v>
       </c>
       <c r="F83" t="s">
-        <v>452</v>
+        <v>109</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>487</v>
+        <v>508</v>
       </c>
       <c r="C84" t="s">
         <v>39</v>
@@ -5165,12 +5282,12 @@
         <v>43</v>
       </c>
       <c r="F84" t="s">
-        <v>109</v>
+        <v>506</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C85" t="s">
         <v>39</v>
@@ -5182,12 +5299,12 @@
         <v>43</v>
       </c>
       <c r="F85" t="s">
-        <v>506</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C86" t="s">
         <v>39</v>
@@ -5199,12 +5316,12 @@
         <v>43</v>
       </c>
       <c r="F86" t="s">
-        <v>109</v>
+        <v>507</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C87" t="s">
         <v>39</v>
@@ -5216,12 +5333,12 @@
         <v>43</v>
       </c>
       <c r="F87" t="s">
-        <v>507</v>
+        <v>109</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C88" t="s">
         <v>39</v>
@@ -5233,12 +5350,12 @@
         <v>43</v>
       </c>
       <c r="F88" t="s">
-        <v>109</v>
+        <v>503</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C89" t="s">
         <v>39</v>
@@ -5250,12 +5367,12 @@
         <v>43</v>
       </c>
       <c r="F89" t="s">
-        <v>503</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C90" t="s">
         <v>39</v>
@@ -5267,12 +5384,12 @@
         <v>43</v>
       </c>
       <c r="F90" t="s">
-        <v>109</v>
+        <v>505</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C91" t="s">
         <v>39</v>
@@ -5284,12 +5401,12 @@
         <v>43</v>
       </c>
       <c r="F91" t="s">
-        <v>505</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C92" t="s">
         <v>39</v>
@@ -5301,12 +5418,12 @@
         <v>43</v>
       </c>
       <c r="F92" t="s">
-        <v>109</v>
+        <v>496</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C93" t="s">
         <v>39</v>
@@ -5318,12 +5435,12 @@
         <v>43</v>
       </c>
       <c r="F93" t="s">
-        <v>496</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C94" t="s">
         <v>39</v>
@@ -5335,12 +5452,12 @@
         <v>43</v>
       </c>
       <c r="F94" t="s">
-        <v>109</v>
+        <v>504</v>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C95" t="s">
         <v>39</v>
@@ -5352,12 +5469,12 @@
         <v>43</v>
       </c>
       <c r="F95" t="s">
-        <v>504</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C96" t="s">
         <v>39</v>
@@ -5369,12 +5486,12 @@
         <v>43</v>
       </c>
       <c r="F96" t="s">
-        <v>109</v>
+        <v>506</v>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C97" t="s">
         <v>39</v>
@@ -5386,12 +5503,12 @@
         <v>43</v>
       </c>
       <c r="F97" t="s">
-        <v>506</v>
+        <v>109</v>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C98" t="s">
         <v>39</v>
@@ -5403,12 +5520,12 @@
         <v>43</v>
       </c>
       <c r="F98" t="s">
-        <v>109</v>
+        <v>507</v>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C99" t="s">
         <v>39</v>
@@ -5420,12 +5537,12 @@
         <v>43</v>
       </c>
       <c r="F99" t="s">
-        <v>507</v>
+        <v>109</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C100" t="s">
         <v>39</v>
@@ -5437,12 +5554,12 @@
         <v>43</v>
       </c>
       <c r="F100" t="s">
-        <v>109</v>
+        <v>503</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C101" t="s">
         <v>39</v>
@@ -5454,12 +5571,12 @@
         <v>43</v>
       </c>
       <c r="F101" t="s">
-        <v>503</v>
+        <v>109</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C102" t="s">
         <v>39</v>
@@ -5471,12 +5588,12 @@
         <v>43</v>
       </c>
       <c r="F102" t="s">
-        <v>109</v>
+        <v>505</v>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C103" t="s">
         <v>39</v>
@@ -5488,12 +5605,12 @@
         <v>43</v>
       </c>
       <c r="F103" t="s">
-        <v>505</v>
+        <v>109</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C104" t="s">
         <v>39</v>
@@ -5505,12 +5622,12 @@
         <v>43</v>
       </c>
       <c r="F104" t="s">
-        <v>109</v>
+        <v>496</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C105" t="s">
         <v>39</v>
@@ -5522,12 +5639,12 @@
         <v>43</v>
       </c>
       <c r="F105" t="s">
-        <v>496</v>
+        <v>109</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C106" t="s">
         <v>39</v>
@@ -5539,12 +5656,12 @@
         <v>43</v>
       </c>
       <c r="F106" t="s">
-        <v>109</v>
+        <v>504</v>
       </c>
     </row>
     <row r="107">
       <c r="B107" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C107" t="s">
         <v>39</v>
@@ -5556,29 +5673,29 @@
         <v>43</v>
       </c>
       <c r="F107" t="s">
-        <v>504</v>
+        <v>109</v>
       </c>
     </row>
     <row r="108">
       <c r="B108" t="s">
-        <v>531</v>
+        <v>546</v>
       </c>
       <c r="C108" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D108" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E108" t="s">
         <v>43</v>
       </c>
       <c r="F108" t="s">
-        <v>109</v>
+        <v>549</v>
       </c>
     </row>
     <row r="109">
       <c r="B109" t="s">
-        <v>546</v>
+        <v>558</v>
       </c>
       <c r="C109" t="s">
         <v>37</v>
@@ -5590,29 +5707,29 @@
         <v>43</v>
       </c>
       <c r="F109" t="s">
-        <v>549</v>
+        <v>559</v>
       </c>
     </row>
     <row r="110">
       <c r="B110" t="s">
-        <v>558</v>
+        <v>566</v>
       </c>
       <c r="C110" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D110" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E110" t="s">
         <v>43</v>
       </c>
       <c r="F110" t="s">
-        <v>559</v>
+        <v>596</v>
       </c>
     </row>
     <row r="111">
       <c r="B111" t="s">
-        <v>566</v>
+        <v>572</v>
       </c>
       <c r="C111" t="s">
         <v>39</v>
@@ -5624,15 +5741,15 @@
         <v>43</v>
       </c>
       <c r="F111" t="s">
-        <v>596</v>
+        <v>559</v>
       </c>
     </row>
     <row r="112">
       <c r="B112" t="s">
-        <v>572</v>
+        <v>585</v>
       </c>
       <c r="C112" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D112" t="s">
         <v>42</v>
@@ -5641,12 +5758,12 @@
         <v>43</v>
       </c>
       <c r="F112" t="s">
-        <v>559</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113">
       <c r="B113" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C113" t="s">
         <v>37</v>
@@ -5658,46 +5775,46 @@
         <v>43</v>
       </c>
       <c r="F113" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114">
       <c r="B114" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C114" t="s">
         <v>37</v>
       </c>
       <c r="D114" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E114" t="s">
         <v>43</v>
       </c>
       <c r="F114" t="s">
-        <v>109</v>
+        <v>392</v>
       </c>
     </row>
     <row r="115">
       <c r="B115" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C115" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D115" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E115" t="s">
         <v>43</v>
       </c>
       <c r="F115" t="s">
-        <v>392</v>
+        <v>596</v>
       </c>
     </row>
     <row r="116">
       <c r="B116" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="C116" t="s">
         <v>40</v>
@@ -5714,7 +5831,7 @@
     </row>
     <row r="117">
       <c r="B117" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C117" t="s">
         <v>40</v>
@@ -5726,12 +5843,12 @@
         <v>43</v>
       </c>
       <c r="F117" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="118">
       <c r="B118" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C118" t="s">
         <v>40</v>
@@ -5743,12 +5860,12 @@
         <v>43</v>
       </c>
       <c r="F118" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="119">
       <c r="B119" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="C119" t="s">
         <v>40</v>
@@ -5760,12 +5877,12 @@
         <v>43</v>
       </c>
       <c r="F119" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="120">
       <c r="B120" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C120" t="s">
         <v>40</v>
@@ -5777,12 +5894,12 @@
         <v>43</v>
       </c>
       <c r="F120" t="s">
-        <v>596</v>
+        <v>109</v>
       </c>
     </row>
     <row r="121">
       <c r="B121" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C121" t="s">
         <v>40</v>
@@ -5794,12 +5911,12 @@
         <v>43</v>
       </c>
       <c r="F121" t="s">
-        <v>109</v>
+        <v>596</v>
       </c>
     </row>
     <row r="122">
       <c r="B122" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C122" t="s">
         <v>40</v>
@@ -5811,35 +5928,35 @@
         <v>43</v>
       </c>
       <c r="F122" t="s">
-        <v>596</v>
+        <v>623</v>
       </c>
     </row>
     <row r="123">
       <c r="B123" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C123" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D123" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E123" t="s">
         <v>43</v>
       </c>
       <c r="F123" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" t="s">
-        <v>602</v>
+        <v>612</v>
       </c>
       <c r="C124" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D124" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E124" t="s">
         <v>43</v>
@@ -5850,10 +5967,10 @@
     </row>
     <row r="125">
       <c r="B125" t="s">
-        <v>612</v>
+        <v>619</v>
       </c>
       <c r="C125" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D125" t="s">
         <v>42</v>
@@ -5862,12 +5979,12 @@
         <v>43</v>
       </c>
       <c r="F125" t="s">
-        <v>603</v>
+        <v>223</v>
       </c>
     </row>
     <row r="126">
       <c r="B126" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C126" t="s">
         <v>37</v>
@@ -5879,46 +5996,46 @@
         <v>43</v>
       </c>
       <c r="F126" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="127">
       <c r="B127" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C127" t="s">
         <v>37</v>
       </c>
       <c r="D127" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E127" t="s">
         <v>43</v>
       </c>
       <c r="F127" t="s">
-        <v>109</v>
+        <v>392</v>
       </c>
     </row>
     <row r="128">
       <c r="B128" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="C128" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D128" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E128" t="s">
         <v>43</v>
       </c>
       <c r="F128" t="s">
-        <v>392</v>
+        <v>644</v>
       </c>
     </row>
     <row r="129">
       <c r="B129" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C129" t="s">
         <v>39</v>
@@ -5930,12 +6047,12 @@
         <v>43</v>
       </c>
       <c r="F129" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="130">
       <c r="B130" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="C130" t="s">
         <v>39</v>
@@ -5947,12 +6064,12 @@
         <v>43</v>
       </c>
       <c r="F130" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="131">
       <c r="B131" t="s">
-        <v>631</v>
+        <v>640</v>
       </c>
       <c r="C131" t="s">
         <v>39</v>
@@ -5964,12 +6081,12 @@
         <v>43</v>
       </c>
       <c r="F131" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="132">
       <c r="B132" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="C132" t="s">
         <v>39</v>
@@ -5981,12 +6098,12 @@
         <v>43</v>
       </c>
       <c r="F132" t="s">
-        <v>641</v>
+        <v>336</v>
       </c>
     </row>
     <row r="133">
       <c r="B133" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="C133" t="s">
         <v>39</v>
@@ -5998,15 +6115,15 @@
         <v>43</v>
       </c>
       <c r="F133" t="s">
-        <v>336</v>
+        <v>623</v>
       </c>
     </row>
     <row r="134">
       <c r="B134" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="C134" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D134" t="s">
         <v>42</v>
@@ -6015,15 +6132,15 @@
         <v>43</v>
       </c>
       <c r="F134" t="s">
-        <v>623</v>
+        <v>650</v>
       </c>
     </row>
     <row r="135">
       <c r="B135" t="s">
-        <v>647</v>
+        <v>674</v>
       </c>
       <c r="C135" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D135" t="s">
         <v>42</v>
@@ -6032,12 +6149,12 @@
         <v>43</v>
       </c>
       <c r="F135" t="s">
-        <v>650</v>
+        <v>370</v>
       </c>
     </row>
     <row r="136">
       <c r="B136" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C136" t="s">
         <v>39</v>
@@ -6049,12 +6166,12 @@
         <v>43</v>
       </c>
       <c r="F136" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="137">
       <c r="B137" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C137" t="s">
         <v>39</v>
@@ -6066,12 +6183,12 @@
         <v>43</v>
       </c>
       <c r="F137" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="138">
       <c r="B138" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C138" t="s">
         <v>39</v>
@@ -6083,12 +6200,12 @@
         <v>43</v>
       </c>
       <c r="F138" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="139">
       <c r="B139" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="C139" t="s">
         <v>39</v>
@@ -6100,12 +6217,12 @@
         <v>43</v>
       </c>
       <c r="F139" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="140">
       <c r="B140" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C140" t="s">
         <v>39</v>
@@ -6117,12 +6234,12 @@
         <v>43</v>
       </c>
       <c r="F140" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="141">
       <c r="B141" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C141" t="s">
         <v>39</v>
@@ -6134,12 +6251,12 @@
         <v>43</v>
       </c>
       <c r="F141" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="142">
       <c r="B142" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C142" t="s">
         <v>39</v>
@@ -6151,12 +6268,12 @@
         <v>43</v>
       </c>
       <c r="F142" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="143">
       <c r="B143" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C143" t="s">
         <v>39</v>
@@ -6168,12 +6285,12 @@
         <v>43</v>
       </c>
       <c r="F143" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="144">
       <c r="B144" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C144" t="s">
         <v>39</v>
@@ -6185,12 +6302,12 @@
         <v>43</v>
       </c>
       <c r="F144" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="145">
       <c r="B145" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C145" t="s">
         <v>39</v>
@@ -6202,12 +6319,12 @@
         <v>43</v>
       </c>
       <c r="F145" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="146">
       <c r="B146" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C146" t="s">
         <v>39</v>
@@ -6219,12 +6336,12 @@
         <v>43</v>
       </c>
       <c r="F146" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="147">
       <c r="B147" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="C147" t="s">
         <v>39</v>
@@ -6236,12 +6353,12 @@
         <v>43</v>
       </c>
       <c r="F147" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="148">
       <c r="B148" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C148" t="s">
         <v>39</v>
@@ -6253,12 +6370,12 @@
         <v>43</v>
       </c>
       <c r="F148" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="149">
       <c r="B149" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C149" t="s">
         <v>39</v>
@@ -6270,12 +6387,12 @@
         <v>43</v>
       </c>
       <c r="F149" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="150">
       <c r="B150" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C150" t="s">
         <v>39</v>
@@ -6287,12 +6404,12 @@
         <v>43</v>
       </c>
       <c r="F150" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="151">
       <c r="B151" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C151" t="s">
         <v>39</v>
@@ -6304,12 +6421,12 @@
         <v>43</v>
       </c>
       <c r="F151" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="152">
       <c r="B152" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="C152" t="s">
         <v>39</v>
@@ -6321,12 +6438,12 @@
         <v>43</v>
       </c>
       <c r="F152" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="153">
       <c r="B153" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C153" t="s">
         <v>39</v>
@@ -6338,12 +6455,12 @@
         <v>43</v>
       </c>
       <c r="F153" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="154">
       <c r="B154" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C154" t="s">
         <v>39</v>
@@ -6355,12 +6472,12 @@
         <v>43</v>
       </c>
       <c r="F154" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="155">
       <c r="B155" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="C155" t="s">
         <v>39</v>
@@ -6372,12 +6489,12 @@
         <v>43</v>
       </c>
       <c r="F155" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="156">
       <c r="B156" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="C156" t="s">
         <v>39</v>
@@ -6389,12 +6506,12 @@
         <v>43</v>
       </c>
       <c r="F156" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="157">
       <c r="B157" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C157" t="s">
         <v>39</v>
@@ -6406,12 +6523,12 @@
         <v>43</v>
       </c>
       <c r="F157" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="158">
       <c r="B158" t="s">
-        <v>696</v>
+        <v>707</v>
       </c>
       <c r="C158" t="s">
         <v>39</v>
@@ -6428,7 +6545,7 @@
     </row>
     <row r="159">
       <c r="B159" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C159" t="s">
         <v>39</v>
@@ -6440,12 +6557,12 @@
         <v>43</v>
       </c>
       <c r="F159" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="160">
       <c r="B160" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C160" t="s">
         <v>39</v>
@@ -6457,12 +6574,12 @@
         <v>43</v>
       </c>
       <c r="F160" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="161">
       <c r="B161" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C161" t="s">
         <v>39</v>
@@ -6474,12 +6591,12 @@
         <v>43</v>
       </c>
       <c r="F161" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="162">
       <c r="B162" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C162" t="s">
         <v>39</v>
@@ -6491,12 +6608,12 @@
         <v>43</v>
       </c>
       <c r="F162" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="163">
       <c r="B163" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C163" t="s">
         <v>39</v>
@@ -6508,12 +6625,12 @@
         <v>43</v>
       </c>
       <c r="F163" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="164">
       <c r="B164" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C164" t="s">
         <v>39</v>
@@ -6525,12 +6642,12 @@
         <v>43</v>
       </c>
       <c r="F164" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="165">
       <c r="B165" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C165" t="s">
         <v>39</v>
@@ -6542,12 +6659,12 @@
         <v>43</v>
       </c>
       <c r="F165" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="166">
       <c r="B166" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="C166" t="s">
         <v>39</v>
@@ -6559,12 +6676,12 @@
         <v>43</v>
       </c>
       <c r="F166" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="167">
       <c r="B167" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C167" t="s">
         <v>39</v>
@@ -6576,12 +6693,12 @@
         <v>43</v>
       </c>
       <c r="F167" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="168">
       <c r="B168" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C168" t="s">
         <v>39</v>
@@ -6593,12 +6710,12 @@
         <v>43</v>
       </c>
       <c r="F168" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="169">
       <c r="B169" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C169" t="s">
         <v>39</v>
@@ -6610,12 +6727,12 @@
         <v>43</v>
       </c>
       <c r="F169" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="170">
       <c r="B170" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C170" t="s">
         <v>39</v>
@@ -6627,12 +6744,12 @@
         <v>43</v>
       </c>
       <c r="F170" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="171">
       <c r="B171" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C171" t="s">
         <v>39</v>
@@ -6644,12 +6761,12 @@
         <v>43</v>
       </c>
       <c r="F171" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="172">
       <c r="B172" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C172" t="s">
         <v>39</v>
@@ -6661,12 +6778,12 @@
         <v>43</v>
       </c>
       <c r="F172" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="173">
       <c r="B173" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C173" t="s">
         <v>39</v>
@@ -6678,12 +6795,12 @@
         <v>43</v>
       </c>
       <c r="F173" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="174">
       <c r="B174" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C174" t="s">
         <v>39</v>
@@ -6695,12 +6812,12 @@
         <v>43</v>
       </c>
       <c r="F174" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="175">
       <c r="B175" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C175" t="s">
         <v>39</v>
@@ -6712,12 +6829,12 @@
         <v>43</v>
       </c>
       <c r="F175" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="176">
       <c r="B176" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C176" t="s">
         <v>39</v>
@@ -6729,12 +6846,12 @@
         <v>43</v>
       </c>
       <c r="F176" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="177">
       <c r="B177" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="C177" t="s">
         <v>39</v>
@@ -6751,7 +6868,7 @@
     </row>
     <row r="178">
       <c r="B178" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C178" t="s">
         <v>39</v>
@@ -6763,12 +6880,12 @@
         <v>43</v>
       </c>
       <c r="F178" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="179">
       <c r="B179" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C179" t="s">
         <v>39</v>
@@ -6780,12 +6897,12 @@
         <v>43</v>
       </c>
       <c r="F179" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="180">
       <c r="B180" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C180" t="s">
         <v>39</v>
@@ -6797,12 +6914,12 @@
         <v>43</v>
       </c>
       <c r="F180" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="181">
       <c r="B181" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C181" t="s">
         <v>39</v>
@@ -6814,12 +6931,12 @@
         <v>43</v>
       </c>
       <c r="F181" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="182">
       <c r="B182" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C182" t="s">
         <v>39</v>
@@ -6831,12 +6948,12 @@
         <v>43</v>
       </c>
       <c r="F182" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="183">
       <c r="B183" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C183" t="s">
         <v>39</v>
@@ -6848,12 +6965,12 @@
         <v>43</v>
       </c>
       <c r="F183" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="184">
       <c r="B184" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C184" t="s">
         <v>39</v>
@@ -6865,12 +6982,12 @@
         <v>43</v>
       </c>
       <c r="F184" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="185">
       <c r="B185" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C185" t="s">
         <v>39</v>
@@ -6882,12 +6999,12 @@
         <v>43</v>
       </c>
       <c r="F185" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="186">
       <c r="B186" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C186" t="s">
         <v>39</v>
@@ -6899,12 +7016,12 @@
         <v>43</v>
       </c>
       <c r="F186" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="187">
       <c r="B187" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C187" t="s">
         <v>39</v>
@@ -6916,12 +7033,12 @@
         <v>43</v>
       </c>
       <c r="F187" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="188">
       <c r="B188" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C188" t="s">
         <v>39</v>
@@ -6933,12 +7050,12 @@
         <v>43</v>
       </c>
       <c r="F188" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="189">
       <c r="B189" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C189" t="s">
         <v>39</v>
@@ -6950,12 +7067,12 @@
         <v>43</v>
       </c>
       <c r="F189" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="190">
       <c r="B190" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C190" t="s">
         <v>39</v>
@@ -6967,12 +7084,12 @@
         <v>43</v>
       </c>
       <c r="F190" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="191">
       <c r="B191" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C191" t="s">
         <v>39</v>
@@ -6984,12 +7101,12 @@
         <v>43</v>
       </c>
       <c r="F191" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="192">
       <c r="B192" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C192" t="s">
         <v>39</v>
@@ -7001,12 +7118,12 @@
         <v>43</v>
       </c>
       <c r="F192" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="193">
       <c r="B193" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C193" t="s">
         <v>39</v>
@@ -7018,12 +7135,12 @@
         <v>43</v>
       </c>
       <c r="F193" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="194">
       <c r="B194" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C194" t="s">
         <v>39</v>
@@ -7035,12 +7152,12 @@
         <v>43</v>
       </c>
       <c r="F194" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="195">
       <c r="B195" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C195" t="s">
         <v>39</v>
@@ -7052,15 +7169,15 @@
         <v>43</v>
       </c>
       <c r="F195" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="196">
       <c r="B196" t="s">
-        <v>745</v>
+        <v>750</v>
       </c>
       <c r="C196" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D196" t="s">
         <v>42</v>
@@ -7069,7 +7186,7 @@
         <v>43</v>
       </c>
       <c r="F196" t="s">
-        <v>370</v>
+        <v>45</v>
       </c>
     </row>
     <row r="197">
@@ -7077,7 +7194,7 @@
         <v>752</v>
       </c>
       <c r="C197" t="s">
-        <v>39</v>
+        <v>762</v>
       </c>
       <c r="D197" t="s">
         <v>42</v>
@@ -7086,15 +7203,15 @@
         <v>43</v>
       </c>
       <c r="F197" t="s">
-        <v>756</v>
+        <v>596</v>
       </c>
     </row>
     <row r="198">
       <c r="B198" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="C198" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D198" t="s">
         <v>42</v>
@@ -7103,15 +7220,15 @@
         <v>43</v>
       </c>
       <c r="F198" t="s">
-        <v>550</v>
+        <v>45</v>
       </c>
     </row>
     <row r="199">
       <c r="B199" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C199" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D199" t="s">
         <v>42</v>
@@ -7120,11 +7237,417 @@
         <v>43</v>
       </c>
       <c r="F199" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="B200" t="s">
+        <v>764</v>
+      </c>
+      <c r="C200" t="s">
+        <v>37</v>
+      </c>
+      <c r="D200" t="s">
+        <v>42</v>
+      </c>
+      <c r="E200" t="s">
+        <v>43</v>
+      </c>
+      <c r="F200" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="B201" t="s">
+        <v>765</v>
+      </c>
+      <c r="C201" t="s">
+        <v>37</v>
+      </c>
+      <c r="D201" t="s">
+        <v>42</v>
+      </c>
+      <c r="E201" t="s">
+        <v>43</v>
+      </c>
+      <c r="F201" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="B202" t="s">
+        <v>766</v>
+      </c>
+      <c r="C202" t="s">
+        <v>37</v>
+      </c>
+      <c r="D202" t="s">
+        <v>42</v>
+      </c>
+      <c r="E202" t="s">
+        <v>43</v>
+      </c>
+      <c r="F202" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="B203" t="s">
+        <v>767</v>
+      </c>
+      <c r="C203" t="s">
+        <v>37</v>
+      </c>
+      <c r="D203" t="s">
+        <v>42</v>
+      </c>
+      <c r="E203" t="s">
+        <v>43</v>
+      </c>
+      <c r="F203" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="B204" t="s">
+        <v>768</v>
+      </c>
+      <c r="C204" t="s">
+        <v>37</v>
+      </c>
+      <c r="D204" t="s">
+        <v>42</v>
+      </c>
+      <c r="E204" t="s">
+        <v>43</v>
+      </c>
+      <c r="F204" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="B205" t="s">
+        <v>769</v>
+      </c>
+      <c r="C205" t="s">
+        <v>37</v>
+      </c>
+      <c r="D205" t="s">
+        <v>42</v>
+      </c>
+      <c r="E205" t="s">
+        <v>43</v>
+      </c>
+      <c r="F205" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="B206" t="s">
+        <v>770</v>
+      </c>
+      <c r="C206" t="s">
+        <v>37</v>
+      </c>
+      <c r="D206" t="s">
+        <v>42</v>
+      </c>
+      <c r="E206" t="s">
+        <v>43</v>
+      </c>
+      <c r="F206" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="B207" t="s">
+        <v>771</v>
+      </c>
+      <c r="C207" t="s">
+        <v>37</v>
+      </c>
+      <c r="D207" t="s">
+        <v>42</v>
+      </c>
+      <c r="E207" t="s">
+        <v>43</v>
+      </c>
+      <c r="F207" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="B208" t="s">
+        <v>772</v>
+      </c>
+      <c r="C208" t="s">
+        <v>37</v>
+      </c>
+      <c r="D208" t="s">
+        <v>42</v>
+      </c>
+      <c r="E208" t="s">
+        <v>43</v>
+      </c>
+      <c r="F208" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="B209" t="s">
+        <v>773</v>
+      </c>
+      <c r="C209" t="s">
+        <v>37</v>
+      </c>
+      <c r="D209" t="s">
+        <v>42</v>
+      </c>
+      <c r="E209" t="s">
+        <v>43</v>
+      </c>
+      <c r="F209" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="B210" t="s">
+        <v>774</v>
+      </c>
+      <c r="C210" t="s">
+        <v>37</v>
+      </c>
+      <c r="D210" t="s">
+        <v>42</v>
+      </c>
+      <c r="E210" t="s">
+        <v>43</v>
+      </c>
+      <c r="F210" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="B211" t="s">
+        <v>775</v>
+      </c>
+      <c r="C211" t="s">
+        <v>37</v>
+      </c>
+      <c r="D211" t="s">
+        <v>42</v>
+      </c>
+      <c r="E211" t="s">
+        <v>43</v>
+      </c>
+      <c r="F211" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="B212" t="s">
+        <v>776</v>
+      </c>
+      <c r="C212" t="s">
+        <v>37</v>
+      </c>
+      <c r="D212" t="s">
+        <v>42</v>
+      </c>
+      <c r="E212" t="s">
+        <v>43</v>
+      </c>
+      <c r="F212" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="B213" t="s">
+        <v>777</v>
+      </c>
+      <c r="C213" t="s">
+        <v>762</v>
+      </c>
+      <c r="D213" t="s">
+        <v>42</v>
+      </c>
+      <c r="E213" t="s">
+        <v>43</v>
+      </c>
+      <c r="F213" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="B214" t="s">
+        <v>778</v>
+      </c>
+      <c r="C214" t="s">
+        <v>762</v>
+      </c>
+      <c r="D214" t="s">
+        <v>42</v>
+      </c>
+      <c r="E214" t="s">
+        <v>43</v>
+      </c>
+      <c r="F214" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="200"/>
-    <row r="201"/>
+    <row r="215">
+      <c r="B215" t="s">
+        <v>779</v>
+      </c>
+      <c r="C215" t="s">
+        <v>762</v>
+      </c>
+      <c r="D215" t="s">
+        <v>42</v>
+      </c>
+      <c r="E215" t="s">
+        <v>43</v>
+      </c>
+      <c r="F215" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="B216" t="s">
+        <v>780</v>
+      </c>
+      <c r="C216" t="s">
+        <v>762</v>
+      </c>
+      <c r="D216" t="s">
+        <v>42</v>
+      </c>
+      <c r="E216" t="s">
+        <v>43</v>
+      </c>
+      <c r="F216" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="B217" t="s">
+        <v>781</v>
+      </c>
+      <c r="C217" t="s">
+        <v>762</v>
+      </c>
+      <c r="D217" t="s">
+        <v>42</v>
+      </c>
+      <c r="E217" t="s">
+        <v>43</v>
+      </c>
+      <c r="F217" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="B218" t="s">
+        <v>782</v>
+      </c>
+      <c r="C218" t="s">
+        <v>762</v>
+      </c>
+      <c r="D218" t="s">
+        <v>42</v>
+      </c>
+      <c r="E218" t="s">
+        <v>43</v>
+      </c>
+      <c r="F218" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="B219" t="s">
+        <v>783</v>
+      </c>
+      <c r="C219" t="s">
+        <v>762</v>
+      </c>
+      <c r="D219" t="s">
+        <v>42</v>
+      </c>
+      <c r="E219" t="s">
+        <v>43</v>
+      </c>
+      <c r="F219" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="B220" t="s">
+        <v>784</v>
+      </c>
+      <c r="C220" t="s">
+        <v>762</v>
+      </c>
+      <c r="D220" t="s">
+        <v>42</v>
+      </c>
+      <c r="E220" t="s">
+        <v>43</v>
+      </c>
+      <c r="F220" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="B221" t="s">
+        <v>786</v>
+      </c>
+      <c r="C221" t="s">
+        <v>39</v>
+      </c>
+      <c r="D221" t="s">
+        <v>42</v>
+      </c>
+      <c r="E221" t="s">
+        <v>43</v>
+      </c>
+      <c r="F221" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="B222" t="s">
+        <v>789</v>
+      </c>
+      <c r="C222" t="s">
+        <v>762</v>
+      </c>
+      <c r="D222" t="s">
+        <v>42</v>
+      </c>
+      <c r="E222" t="s">
+        <v>43</v>
+      </c>
+      <c r="F222" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="B223" t="s">
+        <v>790</v>
+      </c>
+      <c r="C223" t="s">
+        <v>39</v>
+      </c>
+      <c r="D223" t="s">
+        <v>42</v>
+      </c>
+      <c r="E223" t="s">
+        <v>43</v>
+      </c>
+      <c r="F223" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
added module 3 stub
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310897" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312244" uniqueCount="792">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2434,6 +2434,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId408</t>
   </si>
 </sst>
 </file>
@@ -7648,6 +7651,23 @@
         <v>170</v>
       </c>
     </row>
+    <row r="224">
+      <c r="B224" t="s">
+        <v>791</v>
+      </c>
+      <c r="C224" t="s">
+        <v>37</v>
+      </c>
+      <c r="D224" t="s">
+        <v>55</v>
+      </c>
+      <c r="E224" t="s">
+        <v>43</v>
+      </c>
+      <c r="F224" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
added recovery after wrong CRC packet
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312244" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313597" uniqueCount="794">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2437,6 +2437,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId409</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear LEDs</t>
   </si>
 </sst>
 </file>
@@ -7668,6 +7674,23 @@
         <v>226</v>
       </c>
     </row>
+    <row r="225">
+      <c r="B225" t="s">
+        <v>792</v>
+      </c>
+      <c r="C225" t="s">
+        <v>37</v>
+      </c>
+      <c r="D225" t="s">
+        <v>55</v>
+      </c>
+      <c r="E225" t="s">
+        <v>43</v>
+      </c>
+      <c r="F225" t="s">
+        <v>793</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
added new Y-axis graph range changing mechanism
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313597" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327664" uniqueCount="840">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2443,6 +2443,144 @@
   </si>
   <si>
     <t xml:space="preserve">Clear LEDs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId417</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId418</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId422</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId423</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId424</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId426</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId435</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId436</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId439</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId442</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId448</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId449</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId452</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set ranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId453</t>
   </si>
 </sst>
 </file>
@@ -3737,7 +3875,7 @@
         <v>38</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -3804,6 +3942,27 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>794</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>292</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8"/>
       <c r="K8" s="7" t="s">
         <v>8</v>
       </c>
@@ -6030,7 +6189,7 @@
         <v>624</v>
       </c>
       <c r="C128" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D128" t="s">
         <v>42</v>
@@ -6044,10 +6203,10 @@
     </row>
     <row r="129">
       <c r="B129" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="C129" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D129" t="s">
         <v>42</v>
@@ -6056,15 +6215,15 @@
         <v>43</v>
       </c>
       <c r="F129" t="s">
-        <v>642</v>
+        <v>623</v>
       </c>
     </row>
     <row r="130">
       <c r="B130" t="s">
-        <v>631</v>
+        <v>647</v>
       </c>
       <c r="C130" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D130" t="s">
         <v>42</v>
@@ -6073,12 +6232,12 @@
         <v>43</v>
       </c>
       <c r="F130" t="s">
-        <v>639</v>
+        <v>650</v>
       </c>
     </row>
     <row r="131">
       <c r="B131" t="s">
-        <v>640</v>
+        <v>674</v>
       </c>
       <c r="C131" t="s">
         <v>39</v>
@@ -6090,12 +6249,12 @@
         <v>43</v>
       </c>
       <c r="F131" t="s">
-        <v>641</v>
+        <v>370</v>
       </c>
     </row>
     <row r="132">
       <c r="B132" t="s">
-        <v>643</v>
+        <v>675</v>
       </c>
       <c r="C132" t="s">
         <v>39</v>
@@ -6107,12 +6266,12 @@
         <v>43</v>
       </c>
       <c r="F132" t="s">
-        <v>336</v>
+        <v>596</v>
       </c>
     </row>
     <row r="133">
       <c r="B133" t="s">
-        <v>645</v>
+        <v>676</v>
       </c>
       <c r="C133" t="s">
         <v>39</v>
@@ -6124,15 +6283,15 @@
         <v>43</v>
       </c>
       <c r="F133" t="s">
-        <v>623</v>
+        <v>370</v>
       </c>
     </row>
     <row r="134">
       <c r="B134" t="s">
-        <v>647</v>
+        <v>677</v>
       </c>
       <c r="C134" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D134" t="s">
         <v>42</v>
@@ -6141,12 +6300,12 @@
         <v>43</v>
       </c>
       <c r="F134" t="s">
-        <v>650</v>
+        <v>596</v>
       </c>
     </row>
     <row r="135">
       <c r="B135" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="C135" t="s">
         <v>39</v>
@@ -6163,7 +6322,7 @@
     </row>
     <row r="136">
       <c r="B136" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="C136" t="s">
         <v>39</v>
@@ -6180,7 +6339,7 @@
     </row>
     <row r="137">
       <c r="B137" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="C137" t="s">
         <v>39</v>
@@ -6197,7 +6356,7 @@
     </row>
     <row r="138">
       <c r="B138" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="C138" t="s">
         <v>39</v>
@@ -6214,7 +6373,7 @@
     </row>
     <row r="139">
       <c r="B139" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="C139" t="s">
         <v>39</v>
@@ -6231,7 +6390,7 @@
     </row>
     <row r="140">
       <c r="B140" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="C140" t="s">
         <v>39</v>
@@ -6248,7 +6407,7 @@
     </row>
     <row r="141">
       <c r="B141" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="C141" t="s">
         <v>39</v>
@@ -6265,7 +6424,7 @@
     </row>
     <row r="142">
       <c r="B142" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="C142" t="s">
         <v>39</v>
@@ -6282,7 +6441,7 @@
     </row>
     <row r="143">
       <c r="B143" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="C143" t="s">
         <v>39</v>
@@ -6299,7 +6458,7 @@
     </row>
     <row r="144">
       <c r="B144" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="C144" t="s">
         <v>39</v>
@@ -6316,7 +6475,7 @@
     </row>
     <row r="145">
       <c r="B145" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="C145" t="s">
         <v>39</v>
@@ -6333,10 +6492,10 @@
     </row>
     <row r="146">
       <c r="B146" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="C146" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D146" t="s">
         <v>42</v>
@@ -6350,10 +6509,10 @@
     </row>
     <row r="147">
       <c r="B147" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="C147" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D147" t="s">
         <v>42</v>
@@ -6367,10 +6526,10 @@
     </row>
     <row r="148">
       <c r="B148" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="C148" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D148" t="s">
         <v>42</v>
@@ -6384,10 +6543,10 @@
     </row>
     <row r="149">
       <c r="B149" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="C149" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D149" t="s">
         <v>42</v>
@@ -6401,10 +6560,10 @@
     </row>
     <row r="150">
       <c r="B150" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="C150" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D150" t="s">
         <v>42</v>
@@ -6418,10 +6577,10 @@
     </row>
     <row r="151">
       <c r="B151" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="C151" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D151" t="s">
         <v>42</v>
@@ -6435,10 +6594,10 @@
     </row>
     <row r="152">
       <c r="B152" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="C152" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D152" t="s">
         <v>42</v>
@@ -6452,10 +6611,10 @@
     </row>
     <row r="153">
       <c r="B153" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="C153" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D153" t="s">
         <v>42</v>
@@ -6469,7 +6628,7 @@
     </row>
     <row r="154">
       <c r="B154" t="s">
-        <v>693</v>
+        <v>707</v>
       </c>
       <c r="C154" t="s">
         <v>39</v>
@@ -6481,12 +6640,12 @@
         <v>43</v>
       </c>
       <c r="F154" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="155">
       <c r="B155" t="s">
-        <v>694</v>
+        <v>708</v>
       </c>
       <c r="C155" t="s">
         <v>39</v>
@@ -6498,12 +6657,12 @@
         <v>43</v>
       </c>
       <c r="F155" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="156">
       <c r="B156" t="s">
-        <v>695</v>
+        <v>709</v>
       </c>
       <c r="C156" t="s">
         <v>39</v>
@@ -6515,12 +6674,12 @@
         <v>43</v>
       </c>
       <c r="F156" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="157">
       <c r="B157" t="s">
-        <v>696</v>
+        <v>710</v>
       </c>
       <c r="C157" t="s">
         <v>39</v>
@@ -6532,12 +6691,12 @@
         <v>43</v>
       </c>
       <c r="F157" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="158">
       <c r="B158" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
       <c r="C158" t="s">
         <v>39</v>
@@ -6554,7 +6713,7 @@
     </row>
     <row r="159">
       <c r="B159" t="s">
-        <v>708</v>
+        <v>712</v>
       </c>
       <c r="C159" t="s">
         <v>39</v>
@@ -6571,7 +6730,7 @@
     </row>
     <row r="160">
       <c r="B160" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
       <c r="C160" t="s">
         <v>39</v>
@@ -6588,7 +6747,7 @@
     </row>
     <row r="161">
       <c r="B161" t="s">
-        <v>710</v>
+        <v>714</v>
       </c>
       <c r="C161" t="s">
         <v>39</v>
@@ -6605,7 +6764,7 @@
     </row>
     <row r="162">
       <c r="B162" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C162" t="s">
         <v>39</v>
@@ -6622,7 +6781,7 @@
     </row>
     <row r="163">
       <c r="B163" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c r="C163" t="s">
         <v>39</v>
@@ -6639,7 +6798,7 @@
     </row>
     <row r="164">
       <c r="B164" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="C164" t="s">
         <v>39</v>
@@ -6656,7 +6815,7 @@
     </row>
     <row r="165">
       <c r="B165" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="C165" t="s">
         <v>39</v>
@@ -6673,7 +6832,7 @@
     </row>
     <row r="166">
       <c r="B166" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="C166" t="s">
         <v>39</v>
@@ -6690,7 +6849,7 @@
     </row>
     <row r="167">
       <c r="B167" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="C167" t="s">
         <v>39</v>
@@ -6707,7 +6866,7 @@
     </row>
     <row r="168">
       <c r="B168" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="C168" t="s">
         <v>39</v>
@@ -6724,7 +6883,7 @@
     </row>
     <row r="169">
       <c r="B169" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="C169" t="s">
         <v>39</v>
@@ -6741,7 +6900,7 @@
     </row>
     <row r="170">
       <c r="B170" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="C170" t="s">
         <v>39</v>
@@ -6758,7 +6917,7 @@
     </row>
     <row r="171">
       <c r="B171" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c r="C171" t="s">
         <v>39</v>
@@ -6775,7 +6934,7 @@
     </row>
     <row r="172">
       <c r="B172" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
       <c r="C172" t="s">
         <v>39</v>
@@ -6792,7 +6951,7 @@
     </row>
     <row r="173">
       <c r="B173" t="s">
-        <v>722</v>
+        <v>727</v>
       </c>
       <c r="C173" t="s">
         <v>39</v>
@@ -6804,12 +6963,12 @@
         <v>43</v>
       </c>
       <c r="F173" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="174">
       <c r="B174" t="s">
-        <v>723</v>
+        <v>728</v>
       </c>
       <c r="C174" t="s">
         <v>39</v>
@@ -6821,12 +6980,12 @@
         <v>43</v>
       </c>
       <c r="F174" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="175">
       <c r="B175" t="s">
-        <v>724</v>
+        <v>729</v>
       </c>
       <c r="C175" t="s">
         <v>39</v>
@@ -6838,12 +6997,12 @@
         <v>43</v>
       </c>
       <c r="F175" t="s">
-        <v>596</v>
+        <v>370</v>
       </c>
     </row>
     <row r="176">
       <c r="B176" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="C176" t="s">
         <v>39</v>
@@ -6855,12 +7014,12 @@
         <v>43</v>
       </c>
       <c r="F176" t="s">
-        <v>370</v>
+        <v>596</v>
       </c>
     </row>
     <row r="177">
       <c r="B177" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
       <c r="C177" t="s">
         <v>39</v>
@@ -6877,7 +7036,7 @@
     </row>
     <row r="178">
       <c r="B178" t="s">
-        <v>728</v>
+        <v>732</v>
       </c>
       <c r="C178" t="s">
         <v>39</v>
@@ -6894,7 +7053,7 @@
     </row>
     <row r="179">
       <c r="B179" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c r="C179" t="s">
         <v>39</v>
@@ -6911,7 +7070,7 @@
     </row>
     <row r="180">
       <c r="B180" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c r="C180" t="s">
         <v>39</v>
@@ -6928,7 +7087,7 @@
     </row>
     <row r="181">
       <c r="B181" t="s">
-        <v>731</v>
+        <v>735</v>
       </c>
       <c r="C181" t="s">
         <v>39</v>
@@ -6945,7 +7104,7 @@
     </row>
     <row r="182">
       <c r="B182" t="s">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="C182" t="s">
         <v>39</v>
@@ -6962,7 +7121,7 @@
     </row>
     <row r="183">
       <c r="B183" t="s">
-        <v>733</v>
+        <v>737</v>
       </c>
       <c r="C183" t="s">
         <v>39</v>
@@ -6979,7 +7138,7 @@
     </row>
     <row r="184">
       <c r="B184" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="C184" t="s">
         <v>39</v>
@@ -6996,7 +7155,7 @@
     </row>
     <row r="185">
       <c r="B185" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="C185" t="s">
         <v>39</v>
@@ -7013,7 +7172,7 @@
     </row>
     <row r="186">
       <c r="B186" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="C186" t="s">
         <v>39</v>
@@ -7030,7 +7189,7 @@
     </row>
     <row r="187">
       <c r="B187" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="C187" t="s">
         <v>39</v>
@@ -7047,7 +7206,7 @@
     </row>
     <row r="188">
       <c r="B188" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="C188" t="s">
         <v>39</v>
@@ -7064,7 +7223,7 @@
     </row>
     <row r="189">
       <c r="B189" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="C189" t="s">
         <v>39</v>
@@ -7081,7 +7240,7 @@
     </row>
     <row r="190">
       <c r="B190" t="s">
-        <v>740</v>
+        <v>744</v>
       </c>
       <c r="C190" t="s">
         <v>39</v>
@@ -7098,7 +7257,7 @@
     </row>
     <row r="191">
       <c r="B191" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="C191" t="s">
         <v>39</v>
@@ -7115,10 +7274,10 @@
     </row>
     <row r="192">
       <c r="B192" t="s">
-        <v>742</v>
+        <v>750</v>
       </c>
       <c r="C192" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D192" t="s">
         <v>42</v>
@@ -7127,15 +7286,15 @@
         <v>43</v>
       </c>
       <c r="F192" t="s">
-        <v>596</v>
+        <v>45</v>
       </c>
     </row>
     <row r="193">
       <c r="B193" t="s">
-        <v>743</v>
+        <v>753</v>
       </c>
       <c r="C193" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D193" t="s">
         <v>42</v>
@@ -7144,15 +7303,15 @@
         <v>43</v>
       </c>
       <c r="F193" t="s">
-        <v>370</v>
+        <v>45</v>
       </c>
     </row>
     <row r="194">
       <c r="B194" t="s">
-        <v>744</v>
+        <v>758</v>
       </c>
       <c r="C194" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D194" t="s">
         <v>42</v>
@@ -7161,15 +7320,15 @@
         <v>43</v>
       </c>
       <c r="F194" t="s">
-        <v>596</v>
+        <v>45</v>
       </c>
     </row>
     <row r="195">
       <c r="B195" t="s">
-        <v>745</v>
+        <v>764</v>
       </c>
       <c r="C195" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D195" t="s">
         <v>42</v>
@@ -7178,12 +7337,12 @@
         <v>43</v>
       </c>
       <c r="F195" t="s">
-        <v>370</v>
+        <v>45</v>
       </c>
     </row>
     <row r="196">
       <c r="B196" t="s">
-        <v>750</v>
+        <v>765</v>
       </c>
       <c r="C196" t="s">
         <v>37</v>
@@ -7200,10 +7359,10 @@
     </row>
     <row r="197">
       <c r="B197" t="s">
-        <v>752</v>
+        <v>766</v>
       </c>
       <c r="C197" t="s">
-        <v>762</v>
+        <v>37</v>
       </c>
       <c r="D197" t="s">
         <v>42</v>
@@ -7212,12 +7371,12 @@
         <v>43</v>
       </c>
       <c r="F197" t="s">
-        <v>596</v>
+        <v>45</v>
       </c>
     </row>
     <row r="198">
       <c r="B198" t="s">
-        <v>753</v>
+        <v>767</v>
       </c>
       <c r="C198" t="s">
         <v>37</v>
@@ -7234,7 +7393,7 @@
     </row>
     <row r="199">
       <c r="B199" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="C199" t="s">
         <v>37</v>
@@ -7251,7 +7410,7 @@
     </row>
     <row r="200">
       <c r="B200" t="s">
-        <v>764</v>
+        <v>769</v>
       </c>
       <c r="C200" t="s">
         <v>37</v>
@@ -7268,7 +7427,7 @@
     </row>
     <row r="201">
       <c r="B201" t="s">
-        <v>765</v>
+        <v>770</v>
       </c>
       <c r="C201" t="s">
         <v>37</v>
@@ -7285,7 +7444,7 @@
     </row>
     <row r="202">
       <c r="B202" t="s">
-        <v>766</v>
+        <v>771</v>
       </c>
       <c r="C202" t="s">
         <v>37</v>
@@ -7302,7 +7461,7 @@
     </row>
     <row r="203">
       <c r="B203" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
       <c r="C203" t="s">
         <v>37</v>
@@ -7319,7 +7478,7 @@
     </row>
     <row r="204">
       <c r="B204" t="s">
-        <v>768</v>
+        <v>773</v>
       </c>
       <c r="C204" t="s">
         <v>37</v>
@@ -7336,7 +7495,7 @@
     </row>
     <row r="205">
       <c r="B205" t="s">
-        <v>769</v>
+        <v>774</v>
       </c>
       <c r="C205" t="s">
         <v>37</v>
@@ -7353,7 +7512,7 @@
     </row>
     <row r="206">
       <c r="B206" t="s">
-        <v>770</v>
+        <v>775</v>
       </c>
       <c r="C206" t="s">
         <v>37</v>
@@ -7370,7 +7529,7 @@
     </row>
     <row r="207">
       <c r="B207" t="s">
-        <v>771</v>
+        <v>776</v>
       </c>
       <c r="C207" t="s">
         <v>37</v>
@@ -7387,10 +7546,10 @@
     </row>
     <row r="208">
       <c r="B208" t="s">
-        <v>772</v>
+        <v>777</v>
       </c>
       <c r="C208" t="s">
-        <v>37</v>
+        <v>762</v>
       </c>
       <c r="D208" t="s">
         <v>42</v>
@@ -7399,15 +7558,15 @@
         <v>43</v>
       </c>
       <c r="F208" t="s">
-        <v>45</v>
+        <v>596</v>
       </c>
     </row>
     <row r="209">
       <c r="B209" t="s">
-        <v>773</v>
+        <v>778</v>
       </c>
       <c r="C209" t="s">
-        <v>37</v>
+        <v>762</v>
       </c>
       <c r="D209" t="s">
         <v>42</v>
@@ -7416,15 +7575,15 @@
         <v>43</v>
       </c>
       <c r="F209" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
     </row>
     <row r="210">
       <c r="B210" t="s">
-        <v>774</v>
+        <v>779</v>
       </c>
       <c r="C210" t="s">
-        <v>37</v>
+        <v>762</v>
       </c>
       <c r="D210" t="s">
         <v>42</v>
@@ -7433,15 +7592,15 @@
         <v>43</v>
       </c>
       <c r="F210" t="s">
-        <v>45</v>
+        <v>596</v>
       </c>
     </row>
     <row r="211">
       <c r="B211" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
       <c r="C211" t="s">
-        <v>37</v>
+        <v>762</v>
       </c>
       <c r="D211" t="s">
         <v>42</v>
@@ -7450,15 +7609,15 @@
         <v>43</v>
       </c>
       <c r="F211" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
     </row>
     <row r="212">
       <c r="B212" t="s">
-        <v>776</v>
+        <v>781</v>
       </c>
       <c r="C212" t="s">
-        <v>37</v>
+        <v>762</v>
       </c>
       <c r="D212" t="s">
         <v>42</v>
@@ -7467,12 +7626,12 @@
         <v>43</v>
       </c>
       <c r="F212" t="s">
-        <v>45</v>
+        <v>596</v>
       </c>
     </row>
     <row r="213">
       <c r="B213" t="s">
-        <v>777</v>
+        <v>782</v>
       </c>
       <c r="C213" t="s">
         <v>762</v>
@@ -7484,12 +7643,12 @@
         <v>43</v>
       </c>
       <c r="F213" t="s">
-        <v>596</v>
+        <v>109</v>
       </c>
     </row>
     <row r="214">
       <c r="B214" t="s">
-        <v>778</v>
+        <v>783</v>
       </c>
       <c r="C214" t="s">
         <v>762</v>
@@ -7501,12 +7660,12 @@
         <v>43</v>
       </c>
       <c r="F214" t="s">
-        <v>109</v>
+        <v>596</v>
       </c>
     </row>
     <row r="215">
       <c r="B215" t="s">
-        <v>779</v>
+        <v>784</v>
       </c>
       <c r="C215" t="s">
         <v>762</v>
@@ -7518,15 +7677,15 @@
         <v>43</v>
       </c>
       <c r="F215" t="s">
-        <v>596</v>
+        <v>109</v>
       </c>
     </row>
     <row r="216">
       <c r="B216" t="s">
-        <v>780</v>
+        <v>786</v>
       </c>
       <c r="C216" t="s">
-        <v>762</v>
+        <v>39</v>
       </c>
       <c r="D216" t="s">
         <v>42</v>
@@ -7535,15 +7694,15 @@
         <v>43</v>
       </c>
       <c r="F216" t="s">
-        <v>109</v>
+        <v>787</v>
       </c>
     </row>
     <row r="217">
       <c r="B217" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="C217" t="s">
-        <v>762</v>
+        <v>39</v>
       </c>
       <c r="D217" t="s">
         <v>42</v>
@@ -7552,49 +7711,49 @@
         <v>43</v>
       </c>
       <c r="F217" t="s">
-        <v>596</v>
+        <v>170</v>
       </c>
     </row>
     <row r="218">
       <c r="B218" t="s">
-        <v>782</v>
+        <v>791</v>
       </c>
       <c r="C218" t="s">
-        <v>762</v>
+        <v>37</v>
       </c>
       <c r="D218" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E218" t="s">
         <v>43</v>
       </c>
       <c r="F218" t="s">
-        <v>109</v>
+        <v>226</v>
       </c>
     </row>
     <row r="219">
       <c r="B219" t="s">
-        <v>783</v>
+        <v>792</v>
       </c>
       <c r="C219" t="s">
-        <v>762</v>
+        <v>37</v>
       </c>
       <c r="D219" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E219" t="s">
         <v>43</v>
       </c>
       <c r="F219" t="s">
-        <v>596</v>
+        <v>793</v>
       </c>
     </row>
     <row r="220">
       <c r="B220" t="s">
-        <v>784</v>
+        <v>795</v>
       </c>
       <c r="C220" t="s">
-        <v>762</v>
+        <v>794</v>
       </c>
       <c r="D220" t="s">
         <v>42</v>
@@ -7603,15 +7762,15 @@
         <v>43</v>
       </c>
       <c r="F220" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
     </row>
     <row r="221">
       <c r="B221" t="s">
-        <v>786</v>
+        <v>796</v>
       </c>
       <c r="C221" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D221" t="s">
         <v>42</v>
@@ -7620,15 +7779,15 @@
         <v>43</v>
       </c>
       <c r="F221" t="s">
-        <v>787</v>
+        <v>45</v>
       </c>
     </row>
     <row r="222">
       <c r="B222" t="s">
-        <v>789</v>
+        <v>797</v>
       </c>
       <c r="C222" t="s">
-        <v>762</v>
+        <v>794</v>
       </c>
       <c r="D222" t="s">
         <v>42</v>
@@ -7637,15 +7796,15 @@
         <v>43</v>
       </c>
       <c r="F222" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
     </row>
     <row r="223">
       <c r="B223" t="s">
-        <v>790</v>
+        <v>798</v>
       </c>
       <c r="C223" t="s">
-        <v>39</v>
+        <v>794</v>
       </c>
       <c r="D223" t="s">
         <v>42</v>
@@ -7654,43 +7813,707 @@
         <v>43</v>
       </c>
       <c r="F223" t="s">
-        <v>170</v>
+        <v>45</v>
       </c>
     </row>
     <row r="224">
       <c r="B224" t="s">
-        <v>791</v>
+        <v>799</v>
       </c>
       <c r="C224" t="s">
-        <v>37</v>
+        <v>794</v>
       </c>
       <c r="D224" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E224" t="s">
         <v>43</v>
       </c>
       <c r="F224" t="s">
-        <v>226</v>
+        <v>45</v>
       </c>
     </row>
     <row r="225">
       <c r="B225" t="s">
-        <v>792</v>
+        <v>800</v>
       </c>
       <c r="C225" t="s">
+        <v>794</v>
+      </c>
+      <c r="D225" t="s">
+        <v>42</v>
+      </c>
+      <c r="E225" t="s">
+        <v>43</v>
+      </c>
+      <c r="F225" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="B226" t="s">
+        <v>801</v>
+      </c>
+      <c r="C226" t="s">
+        <v>794</v>
+      </c>
+      <c r="D226" t="s">
+        <v>42</v>
+      </c>
+      <c r="E226" t="s">
+        <v>43</v>
+      </c>
+      <c r="F226" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="B227" t="s">
+        <v>802</v>
+      </c>
+      <c r="C227" t="s">
+        <v>794</v>
+      </c>
+      <c r="D227" t="s">
+        <v>42</v>
+      </c>
+      <c r="E227" t="s">
+        <v>43</v>
+      </c>
+      <c r="F227" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="B228" t="s">
+        <v>803</v>
+      </c>
+      <c r="C228" t="s">
+        <v>794</v>
+      </c>
+      <c r="D228" t="s">
+        <v>42</v>
+      </c>
+      <c r="E228" t="s">
+        <v>43</v>
+      </c>
+      <c r="F228" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="B229" t="s">
+        <v>804</v>
+      </c>
+      <c r="C229" t="s">
+        <v>794</v>
+      </c>
+      <c r="D229" t="s">
+        <v>42</v>
+      </c>
+      <c r="E229" t="s">
+        <v>43</v>
+      </c>
+      <c r="F229" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="B230" t="s">
+        <v>805</v>
+      </c>
+      <c r="C230" t="s">
+        <v>794</v>
+      </c>
+      <c r="D230" t="s">
+        <v>42</v>
+      </c>
+      <c r="E230" t="s">
+        <v>43</v>
+      </c>
+      <c r="F230" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="B231" t="s">
+        <v>806</v>
+      </c>
+      <c r="C231" t="s">
+        <v>794</v>
+      </c>
+      <c r="D231" t="s">
+        <v>42</v>
+      </c>
+      <c r="E231" t="s">
+        <v>43</v>
+      </c>
+      <c r="F231" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="B232" t="s">
+        <v>807</v>
+      </c>
+      <c r="C232" t="s">
+        <v>794</v>
+      </c>
+      <c r="D232" t="s">
+        <v>42</v>
+      </c>
+      <c r="E232" t="s">
+        <v>43</v>
+      </c>
+      <c r="F232" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="B233" t="s">
+        <v>808</v>
+      </c>
+      <c r="C233" t="s">
+        <v>794</v>
+      </c>
+      <c r="D233" t="s">
+        <v>42</v>
+      </c>
+      <c r="E233" t="s">
+        <v>43</v>
+      </c>
+      <c r="F233" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="B234" t="s">
+        <v>809</v>
+      </c>
+      <c r="C234" t="s">
+        <v>794</v>
+      </c>
+      <c r="D234" t="s">
+        <v>42</v>
+      </c>
+      <c r="E234" t="s">
+        <v>43</v>
+      </c>
+      <c r="F234" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="B235" t="s">
+        <v>810</v>
+      </c>
+      <c r="C235" t="s">
+        <v>794</v>
+      </c>
+      <c r="D235" t="s">
+        <v>42</v>
+      </c>
+      <c r="E235" t="s">
+        <v>43</v>
+      </c>
+      <c r="F235" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="B236" t="s">
+        <v>811</v>
+      </c>
+      <c r="C236" t="s">
+        <v>794</v>
+      </c>
+      <c r="D236" t="s">
+        <v>42</v>
+      </c>
+      <c r="E236" t="s">
+        <v>43</v>
+      </c>
+      <c r="F236" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="B237" t="s">
+        <v>812</v>
+      </c>
+      <c r="C237" t="s">
+        <v>794</v>
+      </c>
+      <c r="D237" t="s">
+        <v>42</v>
+      </c>
+      <c r="E237" t="s">
+        <v>43</v>
+      </c>
+      <c r="F237" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="B238" t="s">
+        <v>813</v>
+      </c>
+      <c r="C238" t="s">
+        <v>794</v>
+      </c>
+      <c r="D238" t="s">
+        <v>42</v>
+      </c>
+      <c r="E238" t="s">
+        <v>43</v>
+      </c>
+      <c r="F238" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="B239" t="s">
+        <v>814</v>
+      </c>
+      <c r="C239" t="s">
+        <v>794</v>
+      </c>
+      <c r="D239" t="s">
+        <v>42</v>
+      </c>
+      <c r="E239" t="s">
+        <v>43</v>
+      </c>
+      <c r="F239" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="B240" t="s">
+        <v>815</v>
+      </c>
+      <c r="C240" t="s">
+        <v>794</v>
+      </c>
+      <c r="D240" t="s">
+        <v>42</v>
+      </c>
+      <c r="E240" t="s">
+        <v>43</v>
+      </c>
+      <c r="F240" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="B241" t="s">
+        <v>816</v>
+      </c>
+      <c r="C241" t="s">
+        <v>794</v>
+      </c>
+      <c r="D241" t="s">
+        <v>42</v>
+      </c>
+      <c r="E241" t="s">
+        <v>43</v>
+      </c>
+      <c r="F241" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="B242" t="s">
+        <v>817</v>
+      </c>
+      <c r="C242" t="s">
+        <v>794</v>
+      </c>
+      <c r="D242" t="s">
+        <v>42</v>
+      </c>
+      <c r="E242" t="s">
+        <v>43</v>
+      </c>
+      <c r="F242" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="B243" t="s">
+        <v>818</v>
+      </c>
+      <c r="C243" t="s">
+        <v>794</v>
+      </c>
+      <c r="D243" t="s">
+        <v>42</v>
+      </c>
+      <c r="E243" t="s">
+        <v>43</v>
+      </c>
+      <c r="F243" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="B244" t="s">
+        <v>819</v>
+      </c>
+      <c r="C244" t="s">
+        <v>794</v>
+      </c>
+      <c r="D244" t="s">
+        <v>42</v>
+      </c>
+      <c r="E244" t="s">
+        <v>43</v>
+      </c>
+      <c r="F244" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="B245" t="s">
+        <v>820</v>
+      </c>
+      <c r="C245" t="s">
+        <v>794</v>
+      </c>
+      <c r="D245" t="s">
+        <v>42</v>
+      </c>
+      <c r="E245" t="s">
+        <v>43</v>
+      </c>
+      <c r="F245" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="B246" t="s">
+        <v>821</v>
+      </c>
+      <c r="C246" t="s">
+        <v>794</v>
+      </c>
+      <c r="D246" t="s">
+        <v>42</v>
+      </c>
+      <c r="E246" t="s">
+        <v>43</v>
+      </c>
+      <c r="F246" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="B247" t="s">
+        <v>822</v>
+      </c>
+      <c r="C247" t="s">
+        <v>794</v>
+      </c>
+      <c r="D247" t="s">
+        <v>42</v>
+      </c>
+      <c r="E247" t="s">
+        <v>43</v>
+      </c>
+      <c r="F247" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="B248" t="s">
+        <v>823</v>
+      </c>
+      <c r="C248" t="s">
+        <v>794</v>
+      </c>
+      <c r="D248" t="s">
+        <v>42</v>
+      </c>
+      <c r="E248" t="s">
+        <v>43</v>
+      </c>
+      <c r="F248" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="B249" t="s">
+        <v>824</v>
+      </c>
+      <c r="C249" t="s">
+        <v>794</v>
+      </c>
+      <c r="D249" t="s">
+        <v>42</v>
+      </c>
+      <c r="E249" t="s">
+        <v>43</v>
+      </c>
+      <c r="F249" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="B250" t="s">
+        <v>825</v>
+      </c>
+      <c r="C250" t="s">
+        <v>794</v>
+      </c>
+      <c r="D250" t="s">
+        <v>42</v>
+      </c>
+      <c r="E250" t="s">
+        <v>43</v>
+      </c>
+      <c r="F250" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="B251" t="s">
+        <v>826</v>
+      </c>
+      <c r="C251" t="s">
+        <v>794</v>
+      </c>
+      <c r="D251" t="s">
+        <v>42</v>
+      </c>
+      <c r="E251" t="s">
+        <v>43</v>
+      </c>
+      <c r="F251" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="B252" t="s">
+        <v>827</v>
+      </c>
+      <c r="C252" t="s">
+        <v>794</v>
+      </c>
+      <c r="D252" t="s">
+        <v>42</v>
+      </c>
+      <c r="E252" t="s">
+        <v>43</v>
+      </c>
+      <c r="F252" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="B253" t="s">
+        <v>828</v>
+      </c>
+      <c r="C253" t="s">
+        <v>794</v>
+      </c>
+      <c r="D253" t="s">
+        <v>42</v>
+      </c>
+      <c r="E253" t="s">
+        <v>43</v>
+      </c>
+      <c r="F253" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="B254" t="s">
+        <v>829</v>
+      </c>
+      <c r="C254" t="s">
+        <v>794</v>
+      </c>
+      <c r="D254" t="s">
+        <v>42</v>
+      </c>
+      <c r="E254" t="s">
+        <v>43</v>
+      </c>
+      <c r="F254" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="B255" t="s">
+        <v>830</v>
+      </c>
+      <c r="C255" t="s">
+        <v>794</v>
+      </c>
+      <c r="D255" t="s">
+        <v>42</v>
+      </c>
+      <c r="E255" t="s">
+        <v>43</v>
+      </c>
+      <c r="F255" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="B256" t="s">
+        <v>831</v>
+      </c>
+      <c r="C256" t="s">
+        <v>794</v>
+      </c>
+      <c r="D256" t="s">
+        <v>42</v>
+      </c>
+      <c r="E256" t="s">
+        <v>43</v>
+      </c>
+      <c r="F256" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="B257" t="s">
+        <v>832</v>
+      </c>
+      <c r="C257" t="s">
+        <v>794</v>
+      </c>
+      <c r="D257" t="s">
+        <v>42</v>
+      </c>
+      <c r="E257" t="s">
+        <v>43</v>
+      </c>
+      <c r="F257" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="B258" t="s">
+        <v>833</v>
+      </c>
+      <c r="C258" t="s">
+        <v>794</v>
+      </c>
+      <c r="D258" t="s">
+        <v>42</v>
+      </c>
+      <c r="E258" t="s">
+        <v>43</v>
+      </c>
+      <c r="F258" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="B259" t="s">
+        <v>834</v>
+      </c>
+      <c r="C259" t="s">
+        <v>794</v>
+      </c>
+      <c r="D259" t="s">
+        <v>42</v>
+      </c>
+      <c r="E259" t="s">
+        <v>43</v>
+      </c>
+      <c r="F259" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="B260" t="s">
+        <v>631</v>
+      </c>
+      <c r="C260" t="s">
+        <v>794</v>
+      </c>
+      <c r="D260" t="s">
+        <v>42</v>
+      </c>
+      <c r="E260" t="s">
+        <v>43</v>
+      </c>
+      <c r="F260" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="B261" t="s">
+        <v>625</v>
+      </c>
+      <c r="C261" t="s">
+        <v>794</v>
+      </c>
+      <c r="D261" t="s">
+        <v>42</v>
+      </c>
+      <c r="E261" t="s">
+        <v>43</v>
+      </c>
+      <c r="F261" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="B262" t="s">
+        <v>835</v>
+      </c>
+      <c r="C262" t="s">
+        <v>762</v>
+      </c>
+      <c r="D262" t="s">
+        <v>42</v>
+      </c>
+      <c r="E262" t="s">
+        <v>43</v>
+      </c>
+      <c r="F262" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="B263" t="s">
+        <v>837</v>
+      </c>
+      <c r="C263" t="s">
         <v>37</v>
       </c>
-      <c r="D225" t="s">
+      <c r="D263" t="s">
         <v>55</v>
       </c>
-      <c r="E225" t="s">
-        <v>43</v>
-      </c>
-      <c r="F225" t="s">
-        <v>793</v>
-      </c>
-    </row>
+      <c r="E263" t="s">
+        <v>43</v>
+      </c>
+      <c r="F263" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="B264" t="s">
+        <v>839</v>
+      </c>
+      <c r="C264" t="s">
+        <v>794</v>
+      </c>
+      <c r="D264" t="s">
+        <v>42</v>
+      </c>
+      <c r="E264" t="s">
+        <v>43</v>
+      </c>
+      <c r="F264" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="265"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
improved range changing mechanism
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329231" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333968" uniqueCount="844">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2581,6 +2581,18 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId453</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId457</t>
   </si>
 </sst>
 </file>

</xml_diff>